<commit_message>
Adding fixed deposit code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SperidianAutomationProjects\NBFC_CLS\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E517AE-F77F-4402-99C7-3C686E4DF5C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="8" activeTab="10" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -22,10 +21,10 @@
     <sheet name="EWCLeaveRequest" sheetId="7" r:id="rId7"/>
     <sheet name="Customer_CustSearch" sheetId="11" r:id="rId8"/>
     <sheet name="Customer_CustRegister" sheetId="10" r:id="rId9"/>
-    <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId10"/>
-    <sheet name="Customer_NewCustomer" sheetId="13" r:id="rId11"/>
+    <sheet name="AccountOpening_FixedDeposit" sheetId="13" r:id="rId10"/>
+    <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="220">
   <si>
     <t>Run</t>
   </si>
@@ -529,6 +528,18 @@
     <t>aNameAlphabetInput</t>
   </si>
   <si>
+    <t>ZORO</t>
+  </si>
+  <si>
+    <t>LUFFY</t>
+  </si>
+  <si>
+    <t>SANJI</t>
+  </si>
+  <si>
+    <t>ONEPIECE</t>
+  </si>
+  <si>
     <t>occupation</t>
   </si>
   <si>
@@ -574,6 +585,9 @@
     <t>validPANNum</t>
   </si>
   <si>
+    <t>LMHUS2345U</t>
+  </si>
+  <si>
     <t>validTenDigitMobileNum</t>
   </si>
   <si>
@@ -586,6 +600,9 @@
     <t>Alp12</t>
   </si>
   <si>
+    <t>Ocean</t>
+  </si>
+  <si>
     <t>introducerReason</t>
   </si>
   <si>
@@ -634,229 +651,60 @@
     <t>asdf</t>
   </si>
   <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>sanji</t>
-  </si>
-  <si>
-    <t>luffy</t>
-  </si>
-  <si>
-    <t>zoro</t>
-  </si>
-  <si>
-    <t>AMHUS2345B</t>
-  </si>
-  <si>
-    <t>Farm</t>
-  </si>
-  <si>
-    <t>New Customer Module</t>
-  </si>
-  <si>
-    <t>Anu</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>aliasName</t>
-  </si>
-  <si>
-    <t>Singh</t>
-  </si>
-  <si>
-    <t>Rajput</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>Gamer</t>
-  </si>
-  <si>
-    <t>occupOrg</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>guardian</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>Jenny</t>
-  </si>
-  <si>
-    <t>invalidAadhar</t>
-  </si>
-  <si>
-    <t>validPhoneNum</t>
-  </si>
-  <si>
-    <t>invalidPhoneNum</t>
-  </si>
-  <si>
-    <t>weedingDate</t>
-  </si>
-  <si>
-    <t>CKYCId</t>
-  </si>
-  <si>
-    <t>Jony</t>
-  </si>
-  <si>
-    <t>num_Spcl</t>
-  </si>
-  <si>
-    <t>!3#1</t>
-  </si>
-  <si>
-    <t>1234#$%^</t>
-  </si>
-  <si>
-    <t>addressPresentHouse</t>
-  </si>
-  <si>
-    <t>Orkkateeri Veetil12</t>
-  </si>
-  <si>
-    <t>addressPresentHouseNum</t>
-  </si>
-  <si>
-    <t>Buidlingno123%^&amp;</t>
-  </si>
-  <si>
-    <t>addressPresentDoorNum</t>
-  </si>
-  <si>
-    <t>Doorno123%^&amp;</t>
-  </si>
-  <si>
-    <t>addressPresentCity</t>
-  </si>
-  <si>
-    <t>City123%^&amp;</t>
-  </si>
-  <si>
-    <t>Street123%^&amp;</t>
-  </si>
-  <si>
-    <t>addressPresentStreet</t>
-  </si>
-  <si>
-    <t>Malol</t>
-  </si>
-  <si>
-    <t>addressPresentResidence</t>
-  </si>
-  <si>
-    <t>addressPresentElectricPostNum</t>
-  </si>
-  <si>
-    <t>Electric Post No123%^&amp;</t>
-  </si>
-  <si>
-    <t>specialCharInput</t>
-  </si>
-  <si>
-    <t>AlphaNumericInput</t>
-  </si>
-  <si>
-    <t>77A88s99e77u00</t>
-  </si>
-  <si>
-    <t>pin</t>
-  </si>
-  <si>
-    <t>ajith g nair</t>
-  </si>
-  <si>
-    <t>introducerCustName</t>
-  </si>
-  <si>
-    <t>remarks</t>
-  </si>
-  <si>
-    <t>max1</t>
-  </si>
-  <si>
-    <t>alphaNumericInput</t>
-  </si>
-  <si>
-    <t>asd123</t>
-  </si>
-  <si>
-    <t>123aa#$</t>
-  </si>
-  <si>
-    <t>identityNum</t>
-  </si>
-  <si>
-    <t>issuedAuthority</t>
-  </si>
-  <si>
-    <t>456aa#$</t>
-  </si>
-  <si>
-    <t>issueDate</t>
-  </si>
-  <si>
-    <t>27/10/2288</t>
-  </si>
-  <si>
-    <t>validUptoDate</t>
-  </si>
-  <si>
-    <t>duplicateIdentityNum</t>
-  </si>
-  <si>
-    <t>123ab</t>
-  </si>
-  <si>
-    <t>gents</t>
-  </si>
-  <si>
-    <t>27/10/2311</t>
-  </si>
-  <si>
-    <t>ladies</t>
-  </si>
-  <si>
-    <t>unemployed</t>
-  </si>
-  <si>
-    <t>familyName</t>
-  </si>
-  <si>
-    <t>one piece</t>
-  </si>
-  <si>
-    <t>!@#$%!!!</t>
+    <t>pranali</t>
+  </si>
+  <si>
+    <t>san@123</t>
+  </si>
+  <si>
+    <t>AccountOpening_FixedDeposit</t>
+  </si>
+  <si>
+    <t>customerID</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>ReferenceBy</t>
+  </si>
+  <si>
+    <t>NITHIN</t>
+  </si>
+  <si>
+    <t>LedgerNo</t>
+  </si>
+  <si>
+    <t>Foliono</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Lien Amount</t>
+  </si>
+  <si>
+    <t>Lien Remark</t>
+  </si>
+  <si>
+    <t>test01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000000"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="00000000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1071,18 +919,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1397,7 +1239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067DCD9D-336F-4B7B-9363-04AE9D95019D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -1601,11 +1443,128 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F22B618-F971-4F8E-9AEF-0925F5C57140}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="7" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="49">
+        <v>103000012468</v>
+      </c>
+      <c r="H2" s="50">
+        <v>200000</v>
+      </c>
+      <c r="I2" s="51">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>216</v>
+      </c>
+      <c r="N2" s="50">
+        <v>1000</v>
+      </c>
+      <c r="O2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="aka@123"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AE2"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,40 +1643,40 @@
         <v>163</v>
       </c>
       <c r="M1" s="27" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="O1" s="27" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="P1" s="27" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="Q1" s="27" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="R1" s="27" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="S1" s="27" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="T1" s="27" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="U1" s="27" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="V1" s="27" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="W1" s="27" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="X1" s="27" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="Y1" s="27" t="s">
         <v>114</v>
@@ -1729,37 +1688,37 @@
         <v>110</v>
       </c>
       <c r="AB1" s="27" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="AC1" s="27" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="AD1" s="27" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="AE1" s="27" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="AF1" s="27" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="AG1" s="27" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="AH1" s="27" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AI1" s="27" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="AJ1" s="27" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="AK1" s="27" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="AL1" s="27" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:38" s="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1782,82 +1741,82 @@
         <v>92</v>
       </c>
       <c r="G2" s="41">
-        <v>1234</v>
+        <v>1234567</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="I2" s="42">
         <v>34982</v>
       </c>
       <c r="J2" s="41" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="L2" s="41" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="M2" s="41" t="s">
         <v>56</v>
       </c>
       <c r="N2" s="41" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O2" s="41">
         <v>10000</v>
       </c>
       <c r="P2" s="41" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="Q2" s="41" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="R2" s="41" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="S2" s="41" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="T2" s="41">
         <v>87654321</v>
       </c>
       <c r="U2" s="43">
-        <v>987633334521</v>
+        <v>987633334567</v>
       </c>
       <c r="V2" s="41" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="W2" s="41">
-        <v>8989989806</v>
+        <v>8989989800</v>
       </c>
       <c r="X2" s="44" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="Y2" s="41" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="Z2" s="41">
-        <v>1234</v>
+        <v>12345</v>
       </c>
       <c r="AA2" s="41" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="AB2" s="41" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="AC2" s="43">
         <v>103000015690</v>
       </c>
       <c r="AD2" s="41" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="AE2" s="41">
         <v>1234</v>
       </c>
       <c r="AF2" s="41" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="AG2" s="46">
         <v>45590</v>
@@ -1869,397 +1828,28 @@
         <v>146746</v>
       </c>
       <c r="AJ2" s="41" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="AK2" s="43">
         <v>103123415690</v>
       </c>
       <c r="AL2" s="47" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{55C4D6F8-9280-4B03-BD98-C3080CAA1DD3}"/>
-    <hyperlink ref="X2" r:id="rId2" xr:uid="{1DD5089E-1EF7-49AA-857E-1B02F3FC65E4}"/>
-    <hyperlink ref="AL2" r:id="rId3" xr:uid="{17B2A2D8-C298-49F7-9960-213ED4801EB5}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="X2" r:id="rId2"/>
+    <hyperlink ref="AL2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE550206-D522-4FBB-803C-85C7F494A602}">
-  <dimension ref="A1:AW2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AL14" sqref="AL14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" style="48" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25" style="48" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="24.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16" style="48" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.140625" style="48"/>
-    <col min="36" max="36" width="19.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14" style="48" customWidth="1"/>
-    <col min="39" max="39" width="13.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="20.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14" style="48" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="9.140625" style="48"/>
-    <col min="48" max="48" width="12.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="50" max="16384" width="9.140625" style="48"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:49" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="T1" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="U1" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="X1" s="27" t="s">
-        <v>225</v>
-      </c>
-      <c r="Y1" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="Z1" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="AA1" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="AB1" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="AC1" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="AD1" s="27" t="s">
-        <v>239</v>
-      </c>
-      <c r="AE1" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="AF1" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="AG1" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="AH1" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="AI1" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="AJ1" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="AK1" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="AL1" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="AM1" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN1" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="AO1" s="27" t="s">
-        <v>255</v>
-      </c>
-      <c r="AP1" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="AQ1" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="AR1" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="AS1" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="AT1" s="48" t="s">
-        <v>263</v>
-      </c>
-      <c r="AU1" s="48" t="s">
-        <v>265</v>
-      </c>
-      <c r="AV1" s="48" t="s">
-        <v>266</v>
-      </c>
-      <c r="AW1" s="48" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:49" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="K2" s="45">
-        <v>129215</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="N2" s="48">
-        <v>25000</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q2" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="S2" s="48" t="s">
-        <v>229</v>
-      </c>
-      <c r="T2" s="48">
-        <v>9990003330</v>
-      </c>
-      <c r="U2" s="48">
-        <v>123</v>
-      </c>
-      <c r="V2" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="W2" s="45">
-        <v>89769</v>
-      </c>
-      <c r="X2" s="49">
-        <v>87901234567801</v>
-      </c>
-      <c r="Y2" s="48" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z2" s="48" t="s">
-        <v>231</v>
-      </c>
-      <c r="AA2" s="48" t="s">
-        <v>233</v>
-      </c>
-      <c r="AB2" s="48" t="s">
-        <v>235</v>
-      </c>
-      <c r="AC2" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="AD2" s="48" t="s">
-        <v>238</v>
-      </c>
-      <c r="AE2" s="48" t="s">
-        <v>240</v>
-      </c>
-      <c r="AF2" s="48" t="s">
-        <v>243</v>
-      </c>
-      <c r="AG2" s="50" t="s">
-        <v>269</v>
-      </c>
-      <c r="AH2" s="48" t="s">
-        <v>246</v>
-      </c>
-      <c r="AI2" s="48">
-        <v>679302</v>
-      </c>
-      <c r="AJ2" s="48" t="s">
-        <v>248</v>
-      </c>
-      <c r="AK2" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="AL2" s="51">
-        <v>1234567891234</v>
-      </c>
-      <c r="AM2" s="43">
-        <v>103000015690</v>
-      </c>
-      <c r="AN2" s="48" t="s">
-        <v>253</v>
-      </c>
-      <c r="AO2" s="41" t="s">
-        <v>262</v>
-      </c>
-      <c r="AP2" s="48" t="s">
-        <v>257</v>
-      </c>
-      <c r="AQ2" s="48" t="s">
-        <v>259</v>
-      </c>
-      <c r="AR2" s="48" t="s">
-        <v>264</v>
-      </c>
-      <c r="AS2" s="48" t="s">
-        <v>254</v>
-      </c>
-      <c r="AT2" s="48">
-        <v>2</v>
-      </c>
-      <c r="AU2" s="48">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="48">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="48" t="s">
-        <v>268</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{1DFAF61B-C0A4-4574-A5E1-3720F6DD9C3A}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{2125EA55-B892-4DDB-A7AA-2E0D03A8671C}"/>
-    <hyperlink ref="AG2" r:id="rId3" xr:uid="{3F83D89A-3E6D-4AC5-899F-43FEC206A402}"/>
-    <hyperlink ref="AK2" r:id="rId4" xr:uid="{F3A94B01-297D-4A99-BC5C-861BA20D088B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F5BEBC-63DB-4F03-9AF6-8CE69341974D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2341,7 +1931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52F80EF-30F9-4CBE-97A9-F5DB22DCED8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2415,7 +2005,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A4DB3F-2AA2-4FA2-81DE-DE19EC1C5288}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2554,7 +2144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDD8DAA-E0A8-4A27-994A-B8C1DDBA60FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2616,7 +2206,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A776D0A-C93D-4530-8ACF-529782C02B1B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2786,7 +2376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6371D0A3-708E-4B63-973F-AE2BCF9E4611}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2969,7 +2559,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43876BD-E772-4993-8A82-594262F04F89}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3303,10 +2893,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{D0E94D23-5A52-4AEE-B35B-D5A75550EC1B}"/>
-    <hyperlink ref="Y2" r:id="rId2" display="!@#$%^" xr:uid="{76E94768-A019-42D0-9CF6-3514C1339D1A}"/>
-    <hyperlink ref="AA2" r:id="rId3" xr:uid="{94D4DA94-2909-4E83-AD4C-269FA28AA3FB}"/>
-    <hyperlink ref="Q2" r:id="rId4" xr:uid="{A8FB5BF9-CE00-4C79-A53B-08C97A572F60}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="Y2" r:id="rId2" display="!@#$%^"/>
+    <hyperlink ref="AA2" r:id="rId3"/>
+    <hyperlink ref="Q2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -3314,11 +2904,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0E4354-FC05-4BBC-B6A0-D3AD380E4808}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3379,10 +2969,10 @@
         <v>87</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>205</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>92</v>
+        <v>206</v>
       </c>
       <c r="G2" s="3">
         <v>10300001480</v>
@@ -3402,7 +2992,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{AE9DDA39-D293-45BF-A68F-AC222C390A8B}"/>
+    <hyperlink ref="F2" r:id="rId1" display="aka@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Fixeddeposit-Completed till testcase 26
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="232">
   <si>
     <t>Run</t>
   </si>
@@ -697,6 +697,39 @@
   </si>
   <si>
     <t>NomineeCustomerID</t>
+  </si>
+  <si>
+    <t>OperatorCustomerID</t>
+  </si>
+  <si>
+    <t>Adding new operator</t>
+  </si>
+  <si>
+    <t>AccountNo</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>InterestTransferAmount</t>
+  </si>
+  <si>
+    <t>OperatorRemark</t>
+  </si>
+  <si>
+    <t>Relation/Desig.</t>
+  </si>
+  <si>
+    <t>Newuserid</t>
+  </si>
+  <si>
+    <t>Newpassword</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>Mhatre</t>
   </si>
 </sst>
 </file>
@@ -799,7 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -928,6 +961,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1447,20 +1486,24 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1509,8 +1552,32 @@
       <c r="P1" s="48" t="s">
         <v>220</v>
       </c>
+      <c r="Q1" s="52" t="s">
+        <v>221</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>227</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="T1" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="U1" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="V1" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="W1" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>207</v>
       </c>
@@ -1530,7 +1597,7 @@
         <v>206</v>
       </c>
       <c r="G2" s="49">
-        <v>103000012468</v>
+        <v>102000015729</v>
       </c>
       <c r="H2" s="50">
         <v>200000</v>
@@ -1558,14 +1625,39 @@
       </c>
       <c r="P2" s="49">
         <v>103000012745</v>
+      </c>
+      <c r="Q2" s="53">
+        <v>103000012519</v>
+      </c>
+      <c r="R2" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" t="s">
+        <v>222</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2" s="54">
+        <v>1000</v>
+      </c>
+      <c r="W2" t="s">
+        <v>231</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="aka@123"/>
+    <hyperlink ref="X2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2918,7 +3010,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit changes on user creation module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="438">
   <si>
     <t>Run</t>
   </si>
@@ -1349,6 +1349,9 @@
   </si>
   <si>
     <t>adi@123</t>
+  </si>
+  <si>
+    <t>Role</t>
   </si>
 </sst>
 </file>
@@ -2880,7 +2883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -3560,8 +3563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3642,7 +3645,7 @@
         <v>416</v>
       </c>
       <c r="G2" s="80" t="s">
-        <v>360</v>
+        <v>437</v>
       </c>
       <c r="H2" s="75" t="s">
         <v>361</v>
@@ -3691,11 +3694,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="83" t="s">

</xml_diff>

<commit_message>
Commit added authorization in institutional customer module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -24,9 +24,10 @@
     <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId10"/>
     <sheet name="Customer_NewCustomer" sheetId="13" r:id="rId11"/>
     <sheet name="LoanOpening" sheetId="14" r:id="rId12"/>
-    <sheet name="InstitutionalCustomer" sheetId="15" r:id="rId13"/>
-    <sheet name="User_creation" sheetId="16" r:id="rId14"/>
-    <sheet name="Customer_CustRating" sheetId="17" r:id="rId15"/>
+    <sheet name="Otherloanoping_documentsecurity" sheetId="18" r:id="rId13"/>
+    <sheet name="InstitutionalCustomer" sheetId="15" r:id="rId14"/>
+    <sheet name="User_creation" sheetId="16" r:id="rId15"/>
+    <sheet name="Customer_CustRating" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="456">
   <si>
     <t>Run</t>
   </si>
@@ -1352,6 +1353,60 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>regYear</t>
+  </si>
+  <si>
+    <t>docNo</t>
+  </si>
+  <si>
+    <t>regDate</t>
+  </si>
+  <si>
+    <t>worth</t>
+  </si>
+  <si>
+    <t>marketGahanVal</t>
+  </si>
+  <si>
+    <t>nameInNominee</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>TC_Otherloanoping_documentsecurityModule</t>
+  </si>
+  <si>
+    <t>ggw366</t>
+  </si>
+  <si>
+    <t>hent</t>
+  </si>
+  <si>
+    <t>glACCCode</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>intName</t>
+  </si>
+  <si>
+    <t>intAddress</t>
+  </si>
+  <si>
+    <t>dhei</t>
+  </si>
+  <si>
+    <t>dheiei</t>
+  </si>
+  <si>
+    <t>glName</t>
+  </si>
+  <si>
+    <t>as09</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1422,7 @@
     <numFmt numFmtId="169" formatCode="000000000000000"/>
     <numFmt numFmtId="170" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1412,12 +1467,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000C0"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6A3E3E"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -1481,7 +1530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1658,9 +1707,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2884,7 +2930,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2987,10 +3033,10 @@
       <c r="G2" s="55">
         <v>123456789012</v>
       </c>
-      <c r="H2" s="88">
+      <c r="H2" s="87">
         <v>103000066507</v>
       </c>
-      <c r="I2" s="88">
+      <c r="I2" s="87">
         <v>103000013095</v>
       </c>
       <c r="J2" s="52">
@@ -3047,15 +3093,252 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CD2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:CD2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="7" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="H1" s="78" t="s">
+        <v>271</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="J1" s="78" t="s">
+        <v>273</v>
+      </c>
+      <c r="K1" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="L1" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="M1" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="N1" s="78" t="s">
+        <v>277</v>
+      </c>
+      <c r="O1" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="P1" s="78" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q1" s="78" t="s">
+        <v>196</v>
+      </c>
+      <c r="R1" s="78" t="s">
+        <v>280</v>
+      </c>
+      <c r="S1" s="78" t="s">
+        <v>281</v>
+      </c>
+      <c r="T1" s="78" t="s">
+        <v>282</v>
+      </c>
+      <c r="U1" s="78" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="78" t="s">
+        <v>284</v>
+      </c>
+      <c r="W1" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="X1" s="78" t="s">
+        <v>438</v>
+      </c>
+      <c r="Y1" s="78" t="s">
+        <v>439</v>
+      </c>
+      <c r="Z1" s="78" t="s">
+        <v>342</v>
+      </c>
+      <c r="AA1" s="78" t="s">
+        <v>440</v>
+      </c>
+      <c r="AB1" s="78" t="s">
+        <v>441</v>
+      </c>
+      <c r="AC1" s="78" t="s">
+        <v>442</v>
+      </c>
+      <c r="AD1" s="78" t="s">
+        <v>443</v>
+      </c>
+      <c r="AE1" s="78" t="s">
+        <v>444</v>
+      </c>
+      <c r="AF1" s="78" t="s">
+        <v>448</v>
+      </c>
+      <c r="AG1" s="78" t="s">
+        <v>449</v>
+      </c>
+      <c r="AH1" s="78" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
+        <v>445</v>
+      </c>
+      <c r="B2" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>287</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>288</v>
+      </c>
+      <c r="G2" s="87">
+        <v>123456789012</v>
+      </c>
+      <c r="H2" s="87">
+        <v>102000000084</v>
+      </c>
+      <c r="I2" s="87">
+        <v>103000012486</v>
+      </c>
+      <c r="J2" s="58">
+        <v>12</v>
+      </c>
+      <c r="K2" s="72">
+        <v>45575</v>
+      </c>
+      <c r="L2" s="58">
+        <v>12</v>
+      </c>
+      <c r="M2" s="72">
+        <v>45575</v>
+      </c>
+      <c r="N2" s="58">
+        <v>1</v>
+      </c>
+      <c r="O2" s="58">
+        <v>1</v>
+      </c>
+      <c r="P2" s="58" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q2" s="58" t="s">
+        <v>290</v>
+      </c>
+      <c r="R2" s="58">
+        <v>3</v>
+      </c>
+      <c r="S2" s="58">
+        <v>12</v>
+      </c>
+      <c r="T2" s="58">
+        <v>22</v>
+      </c>
+      <c r="U2" s="58">
+        <v>12000</v>
+      </c>
+      <c r="V2" s="58" t="s">
+        <v>435</v>
+      </c>
+      <c r="W2" s="58" t="s">
+        <v>436</v>
+      </c>
+      <c r="X2" s="58">
+        <v>2024</v>
+      </c>
+      <c r="Y2" s="58" t="s">
+        <v>455</v>
+      </c>
+      <c r="Z2" s="58" t="s">
+        <v>446</v>
+      </c>
+      <c r="AA2" s="72">
+        <v>45575</v>
+      </c>
+      <c r="AB2" s="58">
+        <v>1900000</v>
+      </c>
+      <c r="AC2" s="58">
+        <v>2300000</v>
+      </c>
+      <c r="AD2" s="58" t="s">
+        <v>447</v>
+      </c>
+      <c r="AE2" s="72">
+        <v>35713</v>
+      </c>
+      <c r="AF2" s="58">
+        <v>690</v>
+      </c>
+      <c r="AG2" s="58">
+        <v>11046</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:86" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>1</v>
       </c>
@@ -3239,10 +3522,10 @@
       <c r="BI1" s="65" t="s">
         <v>339</v>
       </c>
-      <c r="BJ1" s="68" t="s">
+      <c r="BJ1" s="78" t="s">
         <v>340</v>
       </c>
-      <c r="BK1" s="68" t="s">
+      <c r="BK1" s="78" t="s">
         <v>341</v>
       </c>
       <c r="BL1" s="65" t="s">
@@ -3287,23 +3570,35 @@
       <c r="BY1" s="65" t="s">
         <v>353</v>
       </c>
-      <c r="BZ1" s="72" t="s">
+      <c r="BZ1" s="78" t="s">
         <v>354</v>
       </c>
-      <c r="CA1" s="72" t="s">
+      <c r="CA1" s="78" t="s">
         <v>355</v>
       </c>
-      <c r="CB1" s="72" t="s">
+      <c r="CB1" s="78" t="s">
         <v>356</v>
       </c>
-      <c r="CC1" s="72" t="s">
+      <c r="CC1" s="78" t="s">
         <v>357</v>
       </c>
       <c r="CD1" s="65" t="s">
         <v>358</v>
       </c>
+      <c r="CE1" s="78" t="s">
+        <v>284</v>
+      </c>
+      <c r="CF1" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="CG1" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="CH1" s="27" t="s">
+        <v>451</v>
+      </c>
     </row>
-    <row r="2" spans="1:82" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:86" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>359</v>
       </c>
@@ -3475,10 +3770,10 @@
       <c r="BE2" s="58" t="s">
         <v>397</v>
       </c>
-      <c r="BF2" s="73">
+      <c r="BF2" s="72">
         <v>146016</v>
       </c>
-      <c r="BG2" s="73" t="s">
+      <c r="BG2" s="72" t="s">
         <v>398</v>
       </c>
       <c r="BH2" s="58" t="s">
@@ -3517,10 +3812,10 @@
       <c r="BS2" s="71">
         <v>123456789123456</v>
       </c>
-      <c r="BT2" s="73">
+      <c r="BT2" s="72">
         <v>45658</v>
       </c>
-      <c r="BU2" s="73">
+      <c r="BU2" s="72">
         <v>45658</v>
       </c>
       <c r="BV2" s="58"/>
@@ -3542,11 +3837,23 @@
       <c r="CB2" s="58" t="s">
         <v>405</v>
       </c>
-      <c r="CC2" s="73" t="s">
+      <c r="CC2" s="72" t="s">
         <v>406</v>
       </c>
       <c r="CD2" s="63">
         <v>103000012745</v>
+      </c>
+      <c r="CE2" s="58" t="s">
+        <v>435</v>
+      </c>
+      <c r="CF2" s="58" t="s">
+        <v>436</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>452</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -3559,125 +3866,125 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="76" t="s">
         <v>407</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="76" t="s">
         <v>292</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="76" t="s">
         <v>293</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="76" t="s">
         <v>408</v>
       </c>
-      <c r="L1" s="77" t="s">
+      <c r="L1" s="76" t="s">
         <v>409</v>
       </c>
-      <c r="M1" s="77" t="s">
+      <c r="M1" s="76" t="s">
         <v>410</v>
       </c>
-      <c r="N1" s="77" t="s">
+      <c r="N1" s="76" t="s">
         <v>411</v>
       </c>
-      <c r="O1" s="77" t="s">
+      <c r="O1" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="77" t="s">
+      <c r="P1" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="79" t="s">
+      <c r="Q1" s="78" t="s">
         <v>412</v>
       </c>
-      <c r="R1" s="79" t="s">
+      <c r="R1" s="78" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="73" t="s">
         <v>414</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="73" t="s">
         <v>415</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="77" t="s">
         <v>416</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="79" t="s">
         <v>437</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="74" t="s">
         <v>361</v>
       </c>
-      <c r="I2" s="78" t="s">
+      <c r="I2" s="77" t="s">
         <v>362</v>
       </c>
-      <c r="J2" s="76">
+      <c r="J2" s="75">
         <v>7899996542</v>
       </c>
-      <c r="K2" s="76">
+      <c r="K2" s="75">
         <v>102</v>
       </c>
-      <c r="L2" s="76">
+      <c r="L2" s="75">
         <v>3</v>
       </c>
-      <c r="M2" s="76">
+      <c r="M2" s="75">
         <v>5</v>
       </c>
-      <c r="N2" s="76" t="s">
+      <c r="N2" s="75" t="s">
         <v>417</v>
       </c>
-      <c r="O2" s="76" t="s">
+      <c r="O2" s="75" t="s">
         <v>418</v>
       </c>
-      <c r="P2" s="76" t="s">
+      <c r="P2" s="75" t="s">
         <v>419</v>
       </c>
-      <c r="Q2" s="81" t="s">
+      <c r="Q2" s="80" t="s">
         <v>420</v>
       </c>
-      <c r="R2" s="81" t="s">
+      <c r="R2" s="80" t="s">
         <v>421</v>
       </c>
     </row>
@@ -3690,7 +3997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -3704,126 +4011,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="83" t="s">
+      <c r="G1" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="83" t="s">
+      <c r="H1" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="I1" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="83" t="s">
+      <c r="J1" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="83" t="s">
+      <c r="L1" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="83" t="s">
+      <c r="M1" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="N1" s="83" t="s">
+      <c r="N1" s="82" t="s">
         <v>422</v>
       </c>
-      <c r="O1" s="85" t="s">
+      <c r="O1" s="84" t="s">
         <v>271</v>
       </c>
-      <c r="P1" s="85" t="s">
+      <c r="P1" s="84" t="s">
         <v>423</v>
       </c>
-      <c r="Q1" s="85" t="s">
+      <c r="Q1" s="84" t="s">
         <v>424</v>
       </c>
-      <c r="R1" s="85" t="s">
+      <c r="R1" s="84" t="s">
         <v>425</v>
       </c>
-      <c r="S1" s="85" t="s">
+      <c r="S1" s="84" t="s">
         <v>426</v>
       </c>
-      <c r="T1" s="85" t="s">
+      <c r="T1" s="84" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="81" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>287</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="83" t="s">
         <v>288</v>
       </c>
-      <c r="G2" s="82">
+      <c r="G2" s="81">
         <v>10300001480</v>
       </c>
-      <c r="H2" s="87">
+      <c r="H2" s="86">
         <v>1030000148060</v>
       </c>
-      <c r="I2" s="86">
+      <c r="I2" s="85">
         <v>102000015729</v>
       </c>
-      <c r="J2" s="82" t="s">
+      <c r="J2" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="K2" s="82" t="s">
+      <c r="K2" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="L2" s="81" t="s">
         <v>429</v>
       </c>
-      <c r="M2" s="82">
+      <c r="M2" s="81">
         <v>123456</v>
       </c>
-      <c r="N2" s="82" t="s">
+      <c r="N2" s="81" t="s">
         <v>430</v>
       </c>
-      <c r="O2" s="88">
+      <c r="O2" s="87">
         <v>103000014806</v>
       </c>
-      <c r="P2" s="89" t="s">
+      <c r="P2" s="88" t="s">
         <v>431</v>
       </c>
-      <c r="Q2" s="85" t="s">
+      <c r="Q2" s="84" t="s">
         <v>432</v>
       </c>
-      <c r="R2" s="85">
+      <c r="R2" s="84">
         <v>4</v>
       </c>
-      <c r="S2" s="85" t="s">
+      <c r="S2" s="84" t="s">
         <v>433</v>
       </c>
-      <c r="T2" s="85" t="s">
+      <c r="T2" s="84" t="s">
         <v>434</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit done changes in institutional customer module with properties file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3095,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3280,7 +3280,7 @@
       <c r="V2" s="58" t="s">
         <v>435</v>
       </c>
-      <c r="W2" s="58" t="s">
+      <c r="W2" s="67" t="s">
         <v>436</v>
       </c>
       <c r="X2" s="58">
@@ -3317,6 +3317,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="W2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Authorize added for Quick & New Customer Module. Completed Gold Loan module.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E2E5E6-379A-4EAC-8DA7-67D3E84E9742}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4D8461-FE86-4410-BC25-6B082F4FA3B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="9" activeTab="9" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="9" activeTab="10" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="291">
   <si>
     <t>Run</t>
   </si>
@@ -779,9 +779,6 @@
     <t>pin</t>
   </si>
   <si>
-    <t>ajith g nair</t>
-  </si>
-  <si>
     <t>introducerCustName</t>
   </si>
   <si>
@@ -902,7 +899,16 @@
     <t>purity</t>
   </si>
   <si>
-    <t>sanctioned</t>
+    <t>nomineeName</t>
+  </si>
+  <si>
+    <t>QUICK DHAMU</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>ajitha k t</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1140,6 +1146,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1662,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F22B618-F971-4F8E-9AEF-0925F5C57140}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,7 +1845,7 @@
       <c r="E2" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="52" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="41">
@@ -1951,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE550206-D522-4FBB-803C-85C7F494A602}">
   <dimension ref="A1:BF2"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,46 +2131,46 @@
         <v>246</v>
       </c>
       <c r="AJ1" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="AK1" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="AK1" s="27" t="s">
+      <c r="AL1" s="27" t="s">
         <v>249</v>
-      </c>
-      <c r="AL1" s="27" t="s">
-        <v>250</v>
       </c>
       <c r="AM1" s="27" t="s">
         <v>103</v>
       </c>
       <c r="AN1" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AO1" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="AP1" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="AP1" s="27" t="s">
-        <v>255</v>
-      </c>
       <c r="AQ1" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AR1" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="AS1" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="AS1" s="27" t="s">
-        <v>260</v>
-      </c>
       <c r="AT1" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AU1" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="AV1" s="27" t="s">
         <v>264</v>
       </c>
-      <c r="AV1" s="27" t="s">
+      <c r="AW1" s="27" t="s">
         <v>265</v>
-      </c>
-      <c r="AW1" s="27" t="s">
-        <v>266</v>
       </c>
       <c r="AX1" s="27" t="s">
         <v>194</v>
@@ -2170,25 +2179,25 @@
         <v>195</v>
       </c>
       <c r="AZ1" s="27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="BA1" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="BB1" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="BB1" s="27" t="s">
+      <c r="BC1" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="BC1" s="27" t="s">
+      <c r="BD1" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="BE1" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="BD1" s="27" t="s">
-        <v>277</v>
-      </c>
-      <c r="BE1" s="27" t="s">
+      <c r="BF1" s="27" t="s">
         <v>275</v>
-      </c>
-      <c r="BF1" s="27" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:58" ht="30" x14ac:dyDescent="0.25">
@@ -2289,7 +2298,7 @@
         <v>242</v>
       </c>
       <c r="AG2" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AH2" s="48" t="s">
         <v>245</v>
@@ -2298,7 +2307,7 @@
         <v>679302</v>
       </c>
       <c r="AJ2" s="48" t="s">
-        <v>247</v>
+        <v>290</v>
       </c>
       <c r="AK2" s="44" t="s">
         <v>196</v>
@@ -2310,22 +2319,22 @@
         <v>103000015690</v>
       </c>
       <c r="AN2" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="AO2" s="41" t="s">
+        <v>260</v>
+      </c>
+      <c r="AP2" s="48" t="s">
+        <v>255</v>
+      </c>
+      <c r="AQ2" s="48" t="s">
+        <v>257</v>
+      </c>
+      <c r="AR2" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="AS2" s="48" t="s">
         <v>252</v>
-      </c>
-      <c r="AO2" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="AP2" s="48" t="s">
-        <v>256</v>
-      </c>
-      <c r="AQ2" s="48" t="s">
-        <v>258</v>
-      </c>
-      <c r="AR2" s="48" t="s">
-        <v>263</v>
-      </c>
-      <c r="AS2" s="48" t="s">
-        <v>253</v>
       </c>
       <c r="AT2" s="48">
         <v>2</v>
@@ -2337,16 +2346,16 @@
         <v>1</v>
       </c>
       <c r="AW2" s="48" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AX2" s="43">
         <v>103123415690</v>
       </c>
       <c r="AY2" s="47" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AZ2" s="48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="BA2" s="48">
         <v>678</v>
@@ -2382,9 +2391,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4656AD2A-6EE7-455B-AE6F-DC0029899BED}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -2402,9 +2411,10 @@
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
@@ -2427,31 +2437,34 @@
         <v>106</v>
       </c>
       <c r="H1" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>281</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="27" t="s">
-        <v>283</v>
-      </c>
       <c r="K1" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L1" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="M1" s="27" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="P1" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="27" t="s">
-        <v>288</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>204</v>
       </c>
@@ -2471,7 +2484,7 @@
         <v>92</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H2">
         <v>12345</v>
@@ -2483,7 +2496,7 @@
         <v>1234</v>
       </c>
       <c r="K2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -2495,7 +2508,10 @@
         <v>22</v>
       </c>
       <c r="O2">
-        <v>5000</v>
+        <v>10000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -3410,7 +3426,7 @@
         <v>153</v>
       </c>
       <c r="AT1" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:46" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -3526,7 +3542,7 @@
         <v>142</v>
       </c>
       <c r="AL2" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AM2" s="22" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
Commit document security module- Cash and Transfer Mode
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="458">
   <si>
     <t>Run</t>
   </si>
@@ -1379,9 +1379,6 @@
     <t>TC_Otherloanoping_documentsecurityModule</t>
   </si>
   <si>
-    <t>ggw366</t>
-  </si>
-  <si>
     <t>hent</t>
   </si>
   <si>
@@ -1406,7 +1403,16 @@
     <t>glName</t>
   </si>
   <si>
-    <t>as09</t>
+    <t>makerId</t>
+  </si>
+  <si>
+    <t>ty88</t>
+  </si>
+  <si>
+    <t>hj77</t>
+  </si>
+  <si>
+    <t>amountInCashMode</t>
   </si>
 </sst>
 </file>
@@ -3093,9 +3099,9 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
       <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
@@ -3109,7 +3115,7 @@
     <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>1</v>
       </c>
@@ -3204,16 +3210,22 @@
         <v>444</v>
       </c>
       <c r="AF1" s="78" t="s">
+        <v>447</v>
+      </c>
+      <c r="AG1" s="78" t="s">
         <v>448</v>
       </c>
-      <c r="AG1" s="78" t="s">
-        <v>449</v>
-      </c>
       <c r="AH1" s="78" t="s">
+        <v>453</v>
+      </c>
+      <c r="AI1" s="78" t="s">
         <v>454</v>
       </c>
+      <c r="AJ1" s="78" t="s">
+        <v>457</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
         <v>445</v>
       </c>
@@ -3290,19 +3302,19 @@
         <v>455</v>
       </c>
       <c r="Z2" s="58" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="AA2" s="72">
         <v>45575</v>
       </c>
       <c r="AB2" s="58">
-        <v>1900000</v>
+        <v>2200000</v>
       </c>
       <c r="AC2" s="58">
         <v>2300000</v>
       </c>
       <c r="AD2" s="58" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AE2" s="72">
         <v>35713</v>
@@ -3311,6 +3323,12 @@
         <v>690</v>
       </c>
       <c r="AG2" s="58">
+        <v>11100</v>
+      </c>
+      <c r="AI2" s="58" t="s">
+        <v>287</v>
+      </c>
+      <c r="AJ2" s="58">
         <v>11046</v>
       </c>
     </row>
@@ -3593,10 +3611,10 @@
         <v>285</v>
       </c>
       <c r="CG1" s="27" t="s">
+        <v>449</v>
+      </c>
+      <c r="CH1" s="27" t="s">
         <v>450</v>
-      </c>
-      <c r="CH1" s="27" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:86" ht="60" x14ac:dyDescent="0.25">
@@ -3851,10 +3869,10 @@
         <v>436</v>
       </c>
       <c r="CG2" t="s">
+        <v>451</v>
+      </c>
+      <c r="CH2" t="s">
         <v>452</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit changes done in institutional module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Customer_CustRegister" sheetId="10" r:id="rId9"/>
     <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId10"/>
     <sheet name="Customer_NewCustomer" sheetId="13" r:id="rId11"/>
-    <sheet name="LoanOpening" sheetId="14" r:id="rId12"/>
+    <sheet name="Otherloanopening_jewelsecurity" sheetId="14" r:id="rId12"/>
     <sheet name="Otherloanoping_documentsecurity" sheetId="18" r:id="rId13"/>
     <sheet name="InstitutionalCustomer" sheetId="15" r:id="rId14"/>
     <sheet name="User_creation" sheetId="16" r:id="rId15"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="459">
   <si>
     <t>Run</t>
   </si>
@@ -1413,6 +1413,9 @@
   </si>
   <si>
     <t>amountInCashMode</t>
+  </si>
+  <si>
+    <t>gsjsik</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1531,12 +1534,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1755,6 +1767,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2933,10 +2948,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2944,9 +2959,10 @@
     <col min="7" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>1</v>
       </c>
@@ -3016,8 +3032,26 @@
       <c r="W1" s="56" t="s">
         <v>285</v>
       </c>
+      <c r="X1" s="78" t="s">
+        <v>454</v>
+      </c>
+      <c r="Y1" s="78" t="s">
+        <v>443</v>
+      </c>
+      <c r="Z1" s="89" t="s">
+        <v>444</v>
+      </c>
+      <c r="AA1" s="78" t="s">
+        <v>447</v>
+      </c>
+      <c r="AB1" s="78" t="s">
+        <v>448</v>
+      </c>
+      <c r="AC1" s="78" t="s">
+        <v>457</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>286</v>
       </c>
@@ -3040,7 +3074,7 @@
         <v>123456789012</v>
       </c>
       <c r="H2" s="87">
-        <v>103000066507</v>
+        <v>102000056456</v>
       </c>
       <c r="I2" s="87">
         <v>103000013095</v>
@@ -3086,6 +3120,24 @@
       </c>
       <c r="W2" s="58" t="s">
         <v>436</v>
+      </c>
+      <c r="X2" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z2" s="72">
+        <v>34617</v>
+      </c>
+      <c r="AA2" s="58">
+        <v>690</v>
+      </c>
+      <c r="AB2" s="58">
+        <v>11100</v>
+      </c>
+      <c r="AC2" s="58">
+        <v>11046</v>
       </c>
     </row>
   </sheetData>
@@ -3101,8 +3153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AJ1" sqref="AJ1:AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3345,8 +3397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Authorization updated as required using TransId.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4D8461-FE86-4410-BC25-6B082F4FA3B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2296353-3FFC-4029-9C41-71013DE0E3E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="9" activeTab="10" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="10" activeTab="12" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId10"/>
     <sheet name="Customer_NewCustomer" sheetId="13" r:id="rId11"/>
     <sheet name="AccOpn_JewelLoan_GoldLoan" sheetId="15" r:id="rId12"/>
+    <sheet name="AccOpn_LoanAdva_PersnlLoanWeek" sheetId="16" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="297">
   <si>
     <t>Run</t>
   </si>
@@ -302,21 +303,9 @@
     <t>zxcvb</t>
   </si>
   <si>
-    <t>loginUserName</t>
-  </si>
-  <si>
-    <t>loginValidPassword</t>
-  </si>
-  <si>
     <t>loginInValidPassword</t>
   </si>
   <si>
-    <t>akash</t>
-  </si>
-  <si>
-    <t>aka@123</t>
-  </si>
-  <si>
     <t>invalidMobileNum2</t>
   </si>
   <si>
@@ -909,6 +898,36 @@
   </si>
   <si>
     <t>ajitha k t</t>
+  </si>
+  <si>
+    <t>CHANDRAMATHI P K</t>
+  </si>
+  <si>
+    <t>ab12</t>
+  </si>
+  <si>
+    <t>NITHIN</t>
+  </si>
+  <si>
+    <t>referedByOption</t>
+  </si>
+  <si>
+    <t>MortgagerRegNo</t>
+  </si>
+  <si>
+    <t>validCode</t>
+  </si>
+  <si>
+    <t>securitiesCustName</t>
+  </si>
+  <si>
+    <t>basicPay</t>
+  </si>
+  <si>
+    <t>retdDate</t>
+  </si>
+  <si>
+    <t>sanctionedAmt</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1031,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1056,9 +1075,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1146,9 +1162,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1669,857 +1682,928 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F22B618-F971-4F8E-9AEF-0925F5C57140}">
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" style="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21" style="40" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="21.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16" style="40" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="20.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16" style="40" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="20.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="15.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17" style="40" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="40"/>
+    <col min="1" max="1" width="15.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" style="39" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="21.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16" style="39" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="20.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16" style="39" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="20.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17" style="39" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="27" t="s">
+      <c r="E1" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="K1" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="L1" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="M1" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC1" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD1" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF1" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="AG1" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="AH1" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI1" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="AJ1" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" s="40" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="40">
+        <v>1234</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2" s="41">
+        <v>34982</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="L1" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="O1" s="27" t="s">
+      <c r="M2" s="40">
+        <v>10000</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="O2" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="P1" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q1" s="27" t="s">
+      <c r="P2" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="R1" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="T1" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="U1" s="27" t="s">
+      <c r="R2" s="40">
+        <v>87654321</v>
+      </c>
+      <c r="S2" s="42">
+        <v>987633334521</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="U2" s="40">
+        <v>8989989806</v>
+      </c>
+      <c r="V2" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W2" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="X2" s="40">
+        <v>1234</v>
+      </c>
+      <c r="Y2" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="W1" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="X1" s="27" t="s">
+      <c r="Z2" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="Y1" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z1" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA1" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB1" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="AC1" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="AD1" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="AE1" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="AF1" s="27" t="s">
+      <c r="AA2" s="42">
+        <v>102000010761</v>
+      </c>
+      <c r="AB2" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC2" s="40">
+        <v>1234</v>
+      </c>
+      <c r="AD2" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="AG1" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="AH1" s="27" t="s">
+      <c r="AE2" s="45">
+        <v>45590</v>
+      </c>
+      <c r="AF2" s="44">
+        <v>45575</v>
+      </c>
+      <c r="AG2" s="44">
+        <v>146746</v>
+      </c>
+      <c r="AH2" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="AI1" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="AJ1" s="27" t="s">
+      <c r="AI2" s="42">
+        <v>103123415690</v>
+      </c>
+      <c r="AJ2" s="46" t="s">
         <v>192</v>
-      </c>
-      <c r="AK1" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL1" s="27" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" s="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="41">
-        <v>1234</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>201</v>
-      </c>
-      <c r="I2" s="42">
-        <v>34982</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="L2" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="M2" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="41" t="s">
-        <v>164</v>
-      </c>
-      <c r="O2" s="41">
-        <v>10000</v>
-      </c>
-      <c r="P2" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q2" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="R2" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="S2" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="T2" s="41">
-        <v>87654321</v>
-      </c>
-      <c r="U2" s="43">
-        <v>987633334521</v>
-      </c>
-      <c r="V2" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="W2" s="41">
-        <v>8989989806</v>
-      </c>
-      <c r="X2" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y2" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="Z2" s="41">
-        <v>1234</v>
-      </c>
-      <c r="AA2" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="AB2" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="AC2" s="43">
-        <v>102000010761</v>
-      </c>
-      <c r="AD2" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="AE2" s="41">
-        <v>1234</v>
-      </c>
-      <c r="AF2" s="41" t="s">
-        <v>191</v>
-      </c>
-      <c r="AG2" s="46">
-        <v>45590</v>
-      </c>
-      <c r="AH2" s="45">
-        <v>45575</v>
-      </c>
-      <c r="AI2" s="45">
-        <v>146746</v>
-      </c>
-      <c r="AJ2" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="AK2" s="43">
-        <v>103123415690</v>
-      </c>
-      <c r="AL2" s="47" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{55C4D6F8-9280-4B03-BD98-C3080CAA1DD3}"/>
-    <hyperlink ref="X2" r:id="rId2" xr:uid="{1DD5089E-1EF7-49AA-857E-1B02F3FC65E4}"/>
-    <hyperlink ref="AL2" r:id="rId3" xr:uid="{17B2A2D8-C298-49F7-9960-213ED4801EB5}"/>
+    <hyperlink ref="V2" r:id="rId1" xr:uid="{1DD5089E-1EF7-49AA-857E-1B02F3FC65E4}"/>
+    <hyperlink ref="AJ2" r:id="rId2" xr:uid="{17B2A2D8-C298-49F7-9960-213ED4801EB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE550206-D522-4FBB-803C-85C7F494A602}">
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" style="48" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25" style="48" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="24.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16" style="48" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.140625" style="48"/>
-    <col min="36" max="36" width="19.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14" style="48" customWidth="1"/>
-    <col min="39" max="39" width="13.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="20.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14" style="48" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="9.140625" style="48"/>
-    <col min="48" max="48" width="12.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17" style="48" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="26" style="48" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.140625" style="48"/>
-    <col min="56" max="56" width="13.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19.140625" style="48" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.7109375" style="48" bestFit="1" customWidth="1"/>
-    <col min="59" max="16384" width="9.140625" style="48"/>
+    <col min="1" max="1" width="14.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" style="47" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25" style="47" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="24.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" style="47" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.140625" style="47"/>
+    <col min="34" max="34" width="19.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14" style="47" customWidth="1"/>
+    <col min="37" max="37" width="13.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" style="47" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="9.140625" style="47"/>
+    <col min="46" max="46" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17" style="47" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="26" style="47" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.140625" style="47"/>
+    <col min="54" max="54" width="13.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="19.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="57" max="16384" width="9.140625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="27" t="s">
+      <c r="E1" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="AC1" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD1" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="AF1" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG1" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH1" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI1" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ1" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="AK1" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="AL1" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="AM1" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN1" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="AO1" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="AP1" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="AQ1" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR1" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="AS1" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="AT1" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="AU1" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="AV1" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW1" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="AX1" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="AY1" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="AZ1" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="BA1" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB1" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC1" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="BD1" s="26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="I1" s="27" t="s">
+      <c r="H2" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="I2" s="44">
+        <v>129215</v>
+      </c>
+      <c r="J2" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="K1" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="M1" s="27" t="s">
+      <c r="K2" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="47">
+        <v>25000</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="O2" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="N1" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="T1" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="U1" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="W1" s="27" t="s">
+      <c r="P2" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q2" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="R2" s="47">
+        <v>9990003330</v>
+      </c>
+      <c r="S2" s="47">
+        <v>123</v>
+      </c>
+      <c r="T2" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="U2" s="44">
+        <v>89769</v>
+      </c>
+      <c r="V2" s="48">
+        <v>87901234567801</v>
+      </c>
+      <c r="W2" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="X1" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y1" s="27" t="s">
+      <c r="X2" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="Z1" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="AA1" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="AB1" s="27" t="s">
+      <c r="Y2" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA2" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB2" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="AC1" s="27" t="s">
+      <c r="AC2" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AD2" s="47" t="s">
         <v>238</v>
       </c>
-      <c r="AE1" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="AF1" s="27" t="s">
+      <c r="AE2" s="49" t="s">
+        <v>263</v>
+      </c>
+      <c r="AF2" s="47" t="s">
         <v>241</v>
       </c>
-      <c r="AG1" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="AH1" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="AI1" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="AJ1" s="27" t="s">
+      <c r="AG2" s="47">
+        <v>679302</v>
+      </c>
+      <c r="AH2" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="AI2" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="AJ2" s="50">
+        <v>1234567891234</v>
+      </c>
+      <c r="AK2" s="42">
+        <v>103000015690</v>
+      </c>
+      <c r="AL2" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="AK1" s="27" t="s">
+      <c r="AM2" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="AN2" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="AO2" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="AP2" s="47" t="s">
+        <v>258</v>
+      </c>
+      <c r="AQ2" s="47" t="s">
         <v>248</v>
       </c>
-      <c r="AL1" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="AM1" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN1" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="AO1" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="AP1" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="AQ1" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="AR1" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="AS1" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="AT1" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="AU1" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="AV1" s="27" t="s">
+      <c r="AR2" s="47">
+        <v>2</v>
+      </c>
+      <c r="AS2" s="47">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="47">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="47" t="s">
+        <v>262</v>
+      </c>
+      <c r="AV2" s="42">
+        <v>103123415690</v>
+      </c>
+      <c r="AW2" s="46" t="s">
         <v>264</v>
       </c>
-      <c r="AW1" s="27" t="s">
-        <v>265</v>
-      </c>
-      <c r="AX1" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="AY1" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="AZ1" s="27" t="s">
-        <v>269</v>
-      </c>
-      <c r="BA1" s="27" t="s">
-        <v>271</v>
-      </c>
-      <c r="BB1" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="BC1" s="27" t="s">
-        <v>273</v>
-      </c>
-      <c r="BD1" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="BE1" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="BF1" s="27" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="2" spans="1:58" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="K2" s="45">
-        <v>129215</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="N2" s="48">
-        <v>25000</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q2" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="S2" s="48" t="s">
-        <v>228</v>
-      </c>
-      <c r="T2" s="48">
-        <v>9990003330</v>
-      </c>
-      <c r="U2" s="48">
-        <v>123</v>
-      </c>
-      <c r="V2" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="W2" s="45">
-        <v>89769</v>
-      </c>
-      <c r="X2" s="49">
-        <v>87901234567801</v>
-      </c>
-      <c r="Y2" s="48" t="s">
-        <v>227</v>
-      </c>
-      <c r="Z2" s="48" t="s">
-        <v>230</v>
-      </c>
-      <c r="AA2" s="48" t="s">
-        <v>232</v>
-      </c>
-      <c r="AB2" s="48" t="s">
-        <v>234</v>
-      </c>
-      <c r="AC2" s="48" t="s">
-        <v>236</v>
-      </c>
-      <c r="AD2" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="AE2" s="48" t="s">
-        <v>239</v>
-      </c>
-      <c r="AF2" s="48" t="s">
-        <v>242</v>
-      </c>
-      <c r="AG2" s="50" t="s">
-        <v>267</v>
-      </c>
-      <c r="AH2" s="48" t="s">
-        <v>245</v>
-      </c>
-      <c r="AI2" s="48">
-        <v>679302</v>
-      </c>
-      <c r="AJ2" s="48" t="s">
-        <v>290</v>
-      </c>
-      <c r="AK2" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="AL2" s="51">
-        <v>1234567891234</v>
-      </c>
-      <c r="AM2" s="43">
-        <v>103000015690</v>
-      </c>
-      <c r="AN2" s="48" t="s">
-        <v>251</v>
-      </c>
-      <c r="AO2" s="41" t="s">
-        <v>260</v>
-      </c>
-      <c r="AP2" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="AQ2" s="48" t="s">
-        <v>257</v>
-      </c>
-      <c r="AR2" s="48" t="s">
-        <v>262</v>
-      </c>
-      <c r="AS2" s="48" t="s">
-        <v>252</v>
-      </c>
-      <c r="AT2" s="48">
-        <v>2</v>
-      </c>
-      <c r="AU2" s="48">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="48">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="48" t="s">
+      <c r="AX2" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="AX2" s="43">
-        <v>103123415690</v>
-      </c>
-      <c r="AY2" s="47" t="s">
-        <v>268</v>
-      </c>
-      <c r="AZ2" s="48" t="s">
-        <v>270</v>
-      </c>
-      <c r="BA2" s="48">
+      <c r="AY2" s="47">
         <v>678</v>
       </c>
-      <c r="BB2" s="48">
+      <c r="AZ2" s="47">
         <v>67654</v>
       </c>
-      <c r="BC2" s="48">
+      <c r="BA2" s="47">
         <v>2010</v>
       </c>
-      <c r="BD2" s="48">
+      <c r="BB2" s="47">
         <v>100</v>
       </c>
-      <c r="BE2" s="48">
+      <c r="BC2" s="47">
         <v>1001</v>
       </c>
-      <c r="BF2" s="48">
+      <c r="BD2" s="47">
         <v>2020</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{1DFAF61B-C0A4-4574-A5E1-3720F6DD9C3A}"/>
-    <hyperlink ref="V2" r:id="rId2" xr:uid="{2125EA55-B892-4DDB-A7AA-2E0D03A8671C}"/>
-    <hyperlink ref="AG2" r:id="rId3" xr:uid="{3F83D89A-3E6D-4AC5-899F-43FEC206A402}"/>
-    <hyperlink ref="AK2" r:id="rId4" xr:uid="{F3A94B01-297D-4A99-BC5C-861BA20D088B}"/>
-    <hyperlink ref="AY2" r:id="rId5" display="ASD123!@#" xr:uid="{2E63344B-267B-4F51-9556-1454CDBC54A4}"/>
+    <hyperlink ref="T2" r:id="rId1" xr:uid="{2125EA55-B892-4DDB-A7AA-2E0D03A8671C}"/>
+    <hyperlink ref="AE2" r:id="rId2" xr:uid="{3F83D89A-3E6D-4AC5-899F-43FEC206A402}"/>
+    <hyperlink ref="AI2" r:id="rId3" xr:uid="{F3A94B01-297D-4A99-BC5C-861BA20D088B}"/>
+    <hyperlink ref="AW2" r:id="rId4" display="ASD123!@#" xr:uid="{2E63344B-267B-4F51-9556-1454CDBC54A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4656AD2A-6EE7-455B-AE6F-DC0029899BED}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="47" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="47" customWidth="1"/>
+    <col min="3" max="3" width="17" style="47" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="47" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="47"/>
+    <col min="11" max="11" width="11.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="47"/>
+    <col min="13" max="13" width="10.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="27" t="s">
+      <c r="E1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>280</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="K1" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="L1" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="K1" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" s="47">
+        <v>12345</v>
+      </c>
+      <c r="G2" s="44">
+        <v>129215</v>
+      </c>
+      <c r="H2" s="47">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="J2" s="47">
+        <v>2</v>
+      </c>
+      <c r="K2" s="47">
+        <v>10</v>
+      </c>
+      <c r="L2" s="47">
+        <v>22</v>
+      </c>
+      <c r="M2" s="47">
+        <v>10000</v>
+      </c>
+      <c r="N2" s="47" t="s">
         <v>284</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>286</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="H2">
-        <v>12345</v>
-      </c>
-      <c r="I2" s="45">
-        <v>129215</v>
-      </c>
-      <c r="J2">
-        <v>1234</v>
-      </c>
-      <c r="K2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <v>22</v>
-      </c>
-      <c r="O2">
-        <v>10000</v>
-      </c>
-      <c r="P2" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{C5EBD320-9366-4725-9064-32D2CA5CA710}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18961F5D-5559-4B15-A632-EA58C15475AE}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" style="47"/>
+    <col min="2" max="2" width="6.140625" style="47" customWidth="1"/>
+    <col min="3" max="16384" width="18.85546875" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>288</v>
+      </c>
+      <c r="G2" s="45">
+        <v>129581</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>289</v>
+      </c>
+      <c r="I2" s="47">
+        <v>1234</v>
+      </c>
+      <c r="J2" s="45">
+        <v>45590</v>
+      </c>
+      <c r="K2" s="47">
+        <v>1</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="M2" s="47">
+        <v>10000</v>
+      </c>
+      <c r="N2" s="45">
+        <v>150461</v>
+      </c>
+      <c r="O2" s="47">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3235,373 +3319,358 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43876BD-E772-4993-8A82-594262F04F89}">
-  <dimension ref="A1:AT3"/>
+  <dimension ref="A1:AR3"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AT6" sqref="AT6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="15" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="19" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="13.140625" style="30" customWidth="1"/>
-    <col min="24" max="24" width="14.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" style="30"/>
-    <col min="26" max="26" width="22.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21" style="30" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24" style="30" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19" style="30" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20" style="30" bestFit="1" customWidth="1"/>
-    <col min="46" max="16384" width="17.28515625" style="30"/>
+    <col min="1" max="1" width="23.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="13.140625" style="29" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" style="29"/>
+    <col min="24" max="24" width="22.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21" style="29" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24" style="29" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18" style="29" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19" style="29" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="25.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="22.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20" style="29" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="17.28515625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:44" s="26" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
       <c r="E1" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" s="29" t="s">
+      <c r="N1" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z1" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC1" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD1" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF1" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG1" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI1" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ1" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="AK1" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL1" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="AM1" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN1" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="AO1" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="AP1" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ1" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="AR1" s="26" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="29">
+        <v>98765432</v>
+      </c>
+      <c r="H2" s="29">
+        <v>888999000</v>
+      </c>
+      <c r="I2" s="29">
+        <v>99900088801</v>
+      </c>
+      <c r="J2" s="21">
+        <v>9846968244</v>
+      </c>
+      <c r="K2" s="31">
+        <v>1234567890</v>
+      </c>
+      <c r="L2" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="P1" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="S1" s="27" t="s">
+      <c r="N2" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="O2" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q2" s="29">
+        <v>252522</v>
+      </c>
+      <c r="R2" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="S2" s="33">
+        <v>102000015879</v>
+      </c>
+      <c r="T2" s="33">
+        <v>102000000350</v>
+      </c>
+      <c r="U2" s="33">
+        <v>102000000600</v>
+      </c>
+      <c r="V2" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="W2" s="34">
+        <v>12345</v>
+      </c>
+      <c r="X2" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="U1" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="X1" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y1" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z1" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA1" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB1" s="29" t="s">
+      <c r="Y2" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA2" s="21">
+        <v>12222</v>
+      </c>
+      <c r="AB2" s="36">
+        <v>142447</v>
+      </c>
+      <c r="AC2" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="AC1" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD1" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="AE1" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF1" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="AG1" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="AH1" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="AI1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="AJ1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="AK1" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="AL1" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="AM1" s="27" t="s">
+      <c r="AD2" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE2" s="21">
+        <v>12345</v>
+      </c>
+      <c r="AF2" s="25">
+        <v>102000007421</v>
+      </c>
+      <c r="AG2" s="25">
+        <v>102000016378</v>
+      </c>
+      <c r="AH2" s="25">
+        <v>103000016369</v>
+      </c>
+      <c r="AI2" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="AJ2" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="AK2" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="AN1" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="AO1" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="AP1" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="AQ1" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="AR1" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="AS1" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="AT1" s="27" t="s">
-        <v>278</v>
+      <c r="AL2" s="37">
+        <v>1000020509812</v>
+      </c>
+      <c r="AM2" s="37">
+        <v>1000020512345</v>
+      </c>
+      <c r="AN2" s="25">
+        <v>102000000302</v>
+      </c>
+      <c r="AO2" s="36">
+        <v>146464</v>
+      </c>
+      <c r="AP2" s="36">
+        <v>147111</v>
+      </c>
+      <c r="AQ2" s="36">
+        <v>126293</v>
+      </c>
+      <c r="AR2" s="36">
+        <v>146016</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="I2" s="30">
-        <v>98765432</v>
-      </c>
-      <c r="J2" s="30">
-        <v>888999000</v>
-      </c>
-      <c r="K2" s="30">
-        <v>99900088801</v>
-      </c>
-      <c r="L2" s="22">
-        <v>9846968244</v>
-      </c>
-      <c r="M2" s="32">
-        <v>1234567890</v>
-      </c>
-      <c r="N2" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="O2" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="P2" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="R2" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="S2" s="30">
-        <v>252522</v>
-      </c>
-      <c r="T2" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="U2" s="34">
-        <v>102000015879</v>
-      </c>
-      <c r="V2" s="34">
-        <v>102000000350</v>
-      </c>
-      <c r="W2" s="34">
-        <v>102000000600</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="Y2" s="35">
-        <v>12345</v>
-      </c>
-      <c r="Z2" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="AA2" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB2" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC2" s="22">
-        <v>12222</v>
-      </c>
-      <c r="AD2" s="37">
-        <v>142447</v>
-      </c>
-      <c r="AE2" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG2" s="22">
-        <v>12345</v>
-      </c>
-      <c r="AH2" s="26">
-        <v>102000007421</v>
-      </c>
-      <c r="AI2" s="26">
-        <v>102000016378</v>
-      </c>
-      <c r="AJ2" s="26">
-        <v>103000016369</v>
-      </c>
-      <c r="AK2" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="AL2" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="AM2" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="AN2" s="38">
-        <v>1000020509812</v>
-      </c>
-      <c r="AO2" s="38">
-        <v>1000020512345</v>
-      </c>
-      <c r="AP2" s="26">
-        <v>102000000302</v>
-      </c>
-      <c r="AQ2" s="37">
-        <v>146464</v>
-      </c>
-      <c r="AR2" s="37">
-        <v>147111</v>
-      </c>
-      <c r="AS2" s="37">
-        <v>126293</v>
-      </c>
-      <c r="AT2" s="37">
-        <v>146016</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="22"/>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AH3" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{D0E94D23-5A52-4AEE-B35B-D5A75550EC1B}"/>
-    <hyperlink ref="Y2" r:id="rId2" display="!@#$%^" xr:uid="{76E94768-A019-42D0-9CF6-3514C1339D1A}"/>
-    <hyperlink ref="AA2" r:id="rId3" xr:uid="{94D4DA94-2909-4E83-AD4C-269FA28AA3FB}"/>
-    <hyperlink ref="Q2" r:id="rId4" xr:uid="{A8FB5BF9-CE00-4C79-A53B-08C97A572F60}"/>
+    <hyperlink ref="W2" r:id="rId1" display="!@#$%^" xr:uid="{76E94768-A019-42D0-9CF6-3514C1339D1A}"/>
+    <hyperlink ref="Y2" r:id="rId2" xr:uid="{94D4DA94-2909-4E83-AD4C-269FA28AA3FB}"/>
+    <hyperlink ref="O2" r:id="rId3" xr:uid="{A8FB5BF9-CE00-4C79-A53B-08C97A572F60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0E4354-FC05-4BBC-B6A0-D3AD380E4808}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="20.85546875" style="23"/>
-    <col min="10" max="10" width="13.28515625" style="23" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" style="23"/>
-    <col min="12" max="12" width="26.140625" style="23" customWidth="1"/>
-    <col min="13" max="16384" width="20.85546875" style="23"/>
+    <col min="1" max="7" width="20.85546875" style="22"/>
+    <col min="8" max="8" width="13.28515625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" style="22"/>
+    <col min="10" max="10" width="26.140625" style="22" customWidth="1"/>
+    <col min="11" max="16384" width="20.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -3615,30 +3684,24 @@
         <v>86</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H1" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -3649,33 +3712,24 @@
       <c r="D2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="E2" s="3">
         <v>10300001480</v>
       </c>
-      <c r="H2" s="25">
+      <c r="F2" s="24">
         <v>1030000148060</v>
       </c>
-      <c r="I2" s="24">
+      <c r="G2" s="23">
         <v>102000015729</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>108</v>
+      <c r="H2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{AE9DDA39-D293-45BF-A68F-AC222C390A8B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit with addition of searching customer with transaction id while authorizing
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -2950,8 +2950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AF10" sqref="AF10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit with module name update and testcase count for other loan opening
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -23,11 +23,13 @@
     <sheet name="Customer_CustRegister" sheetId="10" r:id="rId9"/>
     <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId10"/>
     <sheet name="Customer_NewCustomer" sheetId="13" r:id="rId11"/>
-    <sheet name="Otherloanopening_jewelsecurity" sheetId="14" r:id="rId12"/>
-    <sheet name="Otherloanoping_documentsecurity" sheetId="18" r:id="rId13"/>
-    <sheet name="InstitutionalCustomer" sheetId="15" r:id="rId14"/>
-    <sheet name="User_creation" sheetId="16" r:id="rId15"/>
-    <sheet name="Customer_CustRating" sheetId="17" r:id="rId16"/>
+    <sheet name="Otherloanopeningjewelsecurity-C" sheetId="14" r:id="rId12"/>
+    <sheet name="Otherloanopeningjewelsecurity-T" sheetId="19" r:id="rId13"/>
+    <sheet name="documensecurity-Cash" sheetId="18" r:id="rId14"/>
+    <sheet name="documensecurity-Transfer" sheetId="20" r:id="rId15"/>
+    <sheet name="InstitutionalCustomer" sheetId="15" r:id="rId16"/>
+    <sheet name="User_creation" sheetId="16" r:id="rId17"/>
+    <sheet name="Customer_CustRating" sheetId="17" r:id="rId18"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="461">
   <si>
     <t>Run</t>
   </si>
@@ -899,9 +901,6 @@
     <t>loginValidPassword1</t>
   </si>
   <si>
-    <t>TC_LoanOpeningModule</t>
-  </si>
-  <si>
     <t>gopinath</t>
   </si>
   <si>
@@ -1376,9 +1375,6 @@
     <t>dob</t>
   </si>
   <si>
-    <t>TC_Otherloanoping_documentsecurityModule</t>
-  </si>
-  <si>
     <t>hent</t>
   </si>
   <si>
@@ -1416,6 +1412,18 @@
   </si>
   <si>
     <t>gsjsik</t>
+  </si>
+  <si>
+    <t>TC_Otherloan_jewelsecurityModule-Transfer</t>
+  </si>
+  <si>
+    <t>TC_Otherloan_jewelsecurityModule-Cash</t>
+  </si>
+  <si>
+    <t>TC_Otherloanopening_documentsecurityModule-Cash</t>
+  </si>
+  <si>
+    <t>TC_Otherloanopening_documentsecurityModule-Transfer</t>
   </si>
 </sst>
 </file>
@@ -2950,12 +2958,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="7" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -3033,30 +3042,30 @@
         <v>285</v>
       </c>
       <c r="X1" s="78" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="Y1" s="78" t="s">
+        <v>442</v>
+      </c>
+      <c r="Z1" s="89" t="s">
         <v>443</v>
       </c>
-      <c r="Z1" s="89" t="s">
-        <v>444</v>
-      </c>
       <c r="AA1" s="78" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AB1" s="78" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="AC1" s="78" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="AD1" s="78" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>286</v>
+    <row r="2" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
+        <v>458</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>2</v>
@@ -3068,10 +3077,10 @@
         <v>87</v>
       </c>
       <c r="E2" s="53" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2" s="54" t="s">
         <v>287</v>
-      </c>
-      <c r="F2" s="54" t="s">
-        <v>288</v>
       </c>
       <c r="G2" s="55">
         <v>123456789012</v>
@@ -3101,10 +3110,10 @@
         <v>1</v>
       </c>
       <c r="P2" s="52" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q2" s="52" t="s">
         <v>289</v>
-      </c>
-      <c r="Q2" s="52" t="s">
-        <v>290</v>
       </c>
       <c r="R2" s="52">
         <v>3</v>
@@ -3119,16 +3128,16 @@
         <v>12000</v>
       </c>
       <c r="V2" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="W2" s="58" t="s">
         <v>435</v>
       </c>
-      <c r="W2" s="58" t="s">
-        <v>436</v>
-      </c>
       <c r="X2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Y2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="Z2" s="72">
         <v>34617</v>
@@ -3157,10 +3166,215 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="H1" s="78" t="s">
+        <v>271</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="J1" s="78" t="s">
+        <v>273</v>
+      </c>
+      <c r="K1" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="L1" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="M1" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="N1" s="78" t="s">
+        <v>277</v>
+      </c>
+      <c r="O1" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="P1" s="78" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q1" s="78" t="s">
+        <v>196</v>
+      </c>
+      <c r="R1" s="78" t="s">
+        <v>280</v>
+      </c>
+      <c r="S1" s="78" t="s">
+        <v>281</v>
+      </c>
+      <c r="T1" s="78" t="s">
+        <v>282</v>
+      </c>
+      <c r="U1" s="78" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="78" t="s">
+        <v>284</v>
+      </c>
+      <c r="W1" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="X1" s="78" t="s">
+        <v>452</v>
+      </c>
+      <c r="Y1" s="78" t="s">
+        <v>442</v>
+      </c>
+      <c r="Z1" s="89" t="s">
+        <v>443</v>
+      </c>
+      <c r="AA1" s="78" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB1" s="78" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC1" s="78" t="s">
+        <v>455</v>
+      </c>
+      <c r="AD1" s="78" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" s="58" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="87">
+        <v>123456789012</v>
+      </c>
+      <c r="H2" s="87">
+        <v>102000056456</v>
+      </c>
+      <c r="I2" s="87">
+        <v>103000013095</v>
+      </c>
+      <c r="J2" s="58">
+        <v>12</v>
+      </c>
+      <c r="K2" s="72">
+        <v>45575</v>
+      </c>
+      <c r="L2" s="58">
+        <v>12</v>
+      </c>
+      <c r="M2" s="72">
+        <v>45575</v>
+      </c>
+      <c r="N2" s="58">
+        <v>1</v>
+      </c>
+      <c r="O2" s="58">
+        <v>1</v>
+      </c>
+      <c r="P2" s="58" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q2" s="58" t="s">
+        <v>289</v>
+      </c>
+      <c r="R2" s="58">
+        <v>3</v>
+      </c>
+      <c r="S2" s="58">
+        <v>12</v>
+      </c>
+      <c r="T2" s="58">
+        <v>22</v>
+      </c>
+      <c r="U2" s="58">
+        <v>12000</v>
+      </c>
+      <c r="V2" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="W2" s="58" t="s">
+        <v>435</v>
+      </c>
+      <c r="X2" s="58" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y2" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="Z2" s="72">
+        <v>34617</v>
+      </c>
+      <c r="AA2" s="58">
+        <v>690</v>
+      </c>
+      <c r="AB2" s="58">
+        <v>11046</v>
+      </c>
+      <c r="AC2" s="58">
+        <v>11046</v>
+      </c>
+      <c r="AD2" s="58">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AH11" sqref="AH11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,48 +3458,48 @@
         <v>285</v>
       </c>
       <c r="X1" s="78" t="s">
+        <v>437</v>
+      </c>
+      <c r="Y1" s="78" t="s">
         <v>438</v>
       </c>
-      <c r="Y1" s="78" t="s">
+      <c r="Z1" s="78" t="s">
+        <v>341</v>
+      </c>
+      <c r="AA1" s="78" t="s">
         <v>439</v>
       </c>
-      <c r="Z1" s="78" t="s">
-        <v>342</v>
-      </c>
-      <c r="AA1" s="78" t="s">
+      <c r="AB1" s="78" t="s">
         <v>440</v>
       </c>
-      <c r="AB1" s="78" t="s">
+      <c r="AC1" s="78" t="s">
         <v>441</v>
       </c>
-      <c r="AC1" s="78" t="s">
+      <c r="AD1" s="78" t="s">
         <v>442</v>
       </c>
-      <c r="AD1" s="78" t="s">
+      <c r="AE1" s="78" t="s">
         <v>443</v>
       </c>
-      <c r="AE1" s="78" t="s">
-        <v>444</v>
-      </c>
       <c r="AF1" s="78" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AG1" s="78" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="AH1" s="78" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AI1" s="78" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="AJ1" s="78" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>445</v>
+        <v>459</v>
       </c>
       <c r="B2" s="81" t="s">
         <v>2</v>
@@ -3297,10 +3511,10 @@
         <v>87</v>
       </c>
       <c r="E2" s="81" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2" s="83" t="s">
         <v>287</v>
-      </c>
-      <c r="F2" s="83" t="s">
-        <v>288</v>
       </c>
       <c r="G2" s="87">
         <v>123456789012</v>
@@ -3330,10 +3544,10 @@
         <v>1</v>
       </c>
       <c r="P2" s="58" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q2" s="58" t="s">
         <v>289</v>
-      </c>
-      <c r="Q2" s="58" t="s">
-        <v>290</v>
       </c>
       <c r="R2" s="58">
         <v>3</v>
@@ -3348,19 +3562,19 @@
         <v>12000</v>
       </c>
       <c r="V2" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="W2" s="67" t="s">
         <v>435</v>
-      </c>
-      <c r="W2" s="67" t="s">
-        <v>436</v>
       </c>
       <c r="X2" s="58">
         <v>2024</v>
       </c>
       <c r="Y2" s="58" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Z2" s="58" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AA2" s="72">
         <v>45575</v>
@@ -3372,7 +3586,7 @@
         <v>2300000</v>
       </c>
       <c r="AD2" s="58" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AE2" s="72">
         <v>35713</v>
@@ -3387,7 +3601,7 @@
         <v>50</v>
       </c>
       <c r="AI2" s="58" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AJ2" s="58">
         <v>11046</v>
@@ -3402,7 +3616,249 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="H1" s="78" t="s">
+        <v>271</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="J1" s="78" t="s">
+        <v>273</v>
+      </c>
+      <c r="K1" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="L1" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="M1" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="N1" s="78" t="s">
+        <v>277</v>
+      </c>
+      <c r="O1" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="P1" s="78" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q1" s="78" t="s">
+        <v>196</v>
+      </c>
+      <c r="R1" s="78" t="s">
+        <v>280</v>
+      </c>
+      <c r="S1" s="78" t="s">
+        <v>281</v>
+      </c>
+      <c r="T1" s="78" t="s">
+        <v>282</v>
+      </c>
+      <c r="U1" s="78" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="78" t="s">
+        <v>284</v>
+      </c>
+      <c r="W1" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="X1" s="78" t="s">
+        <v>437</v>
+      </c>
+      <c r="Y1" s="78" t="s">
+        <v>438</v>
+      </c>
+      <c r="Z1" s="78" t="s">
+        <v>341</v>
+      </c>
+      <c r="AA1" s="78" t="s">
+        <v>439</v>
+      </c>
+      <c r="AB1" s="78" t="s">
+        <v>440</v>
+      </c>
+      <c r="AC1" s="78" t="s">
+        <v>441</v>
+      </c>
+      <c r="AD1" s="78" t="s">
+        <v>442</v>
+      </c>
+      <c r="AE1" s="78" t="s">
+        <v>443</v>
+      </c>
+      <c r="AF1" s="78" t="s">
+        <v>445</v>
+      </c>
+      <c r="AG1" s="78" t="s">
+        <v>446</v>
+      </c>
+      <c r="AH1" s="78" t="s">
+        <v>451</v>
+      </c>
+      <c r="AI1" s="78" t="s">
+        <v>452</v>
+      </c>
+      <c r="AJ1" s="78" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" s="58" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
+        <v>460</v>
+      </c>
+      <c r="B2" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="87">
+        <v>123456789012</v>
+      </c>
+      <c r="H2" s="87">
+        <v>102000000084</v>
+      </c>
+      <c r="I2" s="87">
+        <v>103000012486</v>
+      </c>
+      <c r="J2" s="58">
+        <v>12</v>
+      </c>
+      <c r="K2" s="72">
+        <v>45575</v>
+      </c>
+      <c r="L2" s="58">
+        <v>12</v>
+      </c>
+      <c r="M2" s="72">
+        <v>45575</v>
+      </c>
+      <c r="N2" s="58">
+        <v>1</v>
+      </c>
+      <c r="O2" s="58">
+        <v>1</v>
+      </c>
+      <c r="P2" s="58" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q2" s="58" t="s">
+        <v>289</v>
+      </c>
+      <c r="R2" s="58">
+        <v>3</v>
+      </c>
+      <c r="S2" s="58">
+        <v>12</v>
+      </c>
+      <c r="T2" s="58">
+        <v>22</v>
+      </c>
+      <c r="U2" s="58">
+        <v>12000</v>
+      </c>
+      <c r="V2" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="W2" s="67" t="s">
+        <v>435</v>
+      </c>
+      <c r="X2" s="58">
+        <v>2024</v>
+      </c>
+      <c r="Y2" s="58" t="s">
+        <v>453</v>
+      </c>
+      <c r="Z2" s="58" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA2" s="72">
+        <v>45575</v>
+      </c>
+      <c r="AB2" s="58">
+        <v>2200000</v>
+      </c>
+      <c r="AC2" s="58">
+        <v>2300000</v>
+      </c>
+      <c r="AD2" s="58" t="s">
+        <v>444</v>
+      </c>
+      <c r="AE2" s="72">
+        <v>35713</v>
+      </c>
+      <c r="AF2" s="58">
+        <v>690</v>
+      </c>
+      <c r="AG2" s="58">
+        <v>11100</v>
+      </c>
+      <c r="AH2" s="58">
+        <v>50</v>
+      </c>
+      <c r="AI2" s="58" t="s">
+        <v>286</v>
+      </c>
+      <c r="AJ2" s="58">
+        <v>11046</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="W2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH2"/>
   <sheetViews>
@@ -3441,139 +3897,139 @@
         <v>208</v>
       </c>
       <c r="H1" s="65" t="s">
+        <v>290</v>
+      </c>
+      <c r="I1" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="J1" s="65" t="s">
         <v>292</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="K1" s="65" t="s">
         <v>293</v>
       </c>
-      <c r="K1" s="65" t="s">
+      <c r="L1" s="65" t="s">
         <v>294</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="M1" s="65" t="s">
         <v>295</v>
       </c>
-      <c r="M1" s="65" t="s">
+      <c r="N1" s="65" t="s">
         <v>296</v>
       </c>
-      <c r="N1" s="65" t="s">
+      <c r="O1" s="65" t="s">
         <v>297</v>
       </c>
-      <c r="O1" s="65" t="s">
+      <c r="P1" s="65" t="s">
         <v>298</v>
-      </c>
-      <c r="P1" s="65" t="s">
-        <v>299</v>
       </c>
       <c r="Q1" s="65" t="s">
         <v>247</v>
       </c>
       <c r="R1" s="65" t="s">
+        <v>299</v>
+      </c>
+      <c r="S1" s="65" t="s">
         <v>300</v>
       </c>
-      <c r="S1" s="65" t="s">
+      <c r="T1" s="65" t="s">
         <v>301</v>
       </c>
-      <c r="T1" s="65" t="s">
+      <c r="U1" s="65" t="s">
         <v>302</v>
       </c>
-      <c r="U1" s="65" t="s">
+      <c r="V1" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="V1" s="65" t="s">
+      <c r="W1" s="65" t="s">
         <v>304</v>
       </c>
-      <c r="W1" s="65" t="s">
+      <c r="X1" s="65" t="s">
         <v>305</v>
       </c>
-      <c r="X1" s="65" t="s">
+      <c r="Y1" s="65" t="s">
         <v>306</v>
       </c>
-      <c r="Y1" s="65" t="s">
+      <c r="Z1" s="65" t="s">
         <v>307</v>
       </c>
-      <c r="Z1" s="65" t="s">
+      <c r="AA1" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="AA1" s="65" t="s">
+      <c r="AB1" s="65" t="s">
         <v>309</v>
       </c>
-      <c r="AB1" s="65" t="s">
+      <c r="AC1" s="65" t="s">
         <v>310</v>
       </c>
-      <c r="AC1" s="65" t="s">
+      <c r="AD1" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="AD1" s="65" t="s">
+      <c r="AE1" s="65" t="s">
         <v>312</v>
       </c>
-      <c r="AE1" s="65" t="s">
+      <c r="AF1" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="AF1" s="65" t="s">
+      <c r="AG1" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="AG1" s="65" t="s">
+      <c r="AH1" s="65" t="s">
         <v>315</v>
       </c>
-      <c r="AH1" s="65" t="s">
+      <c r="AI1" s="65" t="s">
         <v>316</v>
       </c>
-      <c r="AI1" s="65" t="s">
+      <c r="AJ1" s="65" t="s">
         <v>317</v>
       </c>
-      <c r="AJ1" s="65" t="s">
+      <c r="AK1" s="65" t="s">
         <v>318</v>
       </c>
-      <c r="AK1" s="65" t="s">
+      <c r="AL1" s="65" t="s">
         <v>319</v>
       </c>
-      <c r="AL1" s="65" t="s">
+      <c r="AM1" s="65" t="s">
         <v>320</v>
       </c>
-      <c r="AM1" s="65" t="s">
+      <c r="AN1" s="65" t="s">
         <v>321</v>
       </c>
-      <c r="AN1" s="65" t="s">
+      <c r="AO1" s="65" t="s">
         <v>322</v>
       </c>
-      <c r="AO1" s="65" t="s">
+      <c r="AP1" s="65" t="s">
         <v>323</v>
       </c>
-      <c r="AP1" s="65" t="s">
+      <c r="AQ1" s="65" t="s">
         <v>324</v>
       </c>
-      <c r="AQ1" s="65" t="s">
+      <c r="AR1" s="65" t="s">
         <v>325</v>
       </c>
-      <c r="AR1" s="65" t="s">
+      <c r="AS1" s="65" t="s">
         <v>326</v>
       </c>
-      <c r="AS1" s="65" t="s">
+      <c r="AT1" s="65" t="s">
         <v>327</v>
       </c>
-      <c r="AT1" s="65" t="s">
+      <c r="AU1" s="65" t="s">
         <v>328</v>
       </c>
-      <c r="AU1" s="65" t="s">
+      <c r="AV1" s="65" t="s">
         <v>329</v>
       </c>
-      <c r="AV1" s="65" t="s">
+      <c r="AW1" s="65" t="s">
         <v>330</v>
       </c>
-      <c r="AW1" s="65" t="s">
+      <c r="AX1" s="65" t="s">
         <v>331</v>
       </c>
-      <c r="AX1" s="65" t="s">
+      <c r="AY1" s="65" t="s">
         <v>332</v>
       </c>
-      <c r="AY1" s="65" t="s">
+      <c r="AZ1" s="65" t="s">
         <v>333</v>
-      </c>
-      <c r="AZ1" s="65" t="s">
-        <v>334</v>
       </c>
       <c r="BA1" s="65" t="s">
         <v>55</v>
@@ -3582,10 +4038,10 @@
         <v>250</v>
       </c>
       <c r="BC1" s="65" t="s">
+        <v>334</v>
+      </c>
+      <c r="BD1" s="65" t="s">
         <v>335</v>
-      </c>
-      <c r="BD1" s="65" t="s">
-        <v>336</v>
       </c>
       <c r="BE1" s="65" t="s">
         <v>256</v>
@@ -3594,31 +4050,31 @@
         <v>258</v>
       </c>
       <c r="BG1" s="65" t="s">
+        <v>336</v>
+      </c>
+      <c r="BH1" s="65" t="s">
         <v>337</v>
       </c>
-      <c r="BH1" s="65" t="s">
+      <c r="BI1" s="65" t="s">
         <v>338</v>
       </c>
-      <c r="BI1" s="65" t="s">
+      <c r="BJ1" s="78" t="s">
         <v>339</v>
       </c>
-      <c r="BJ1" s="78" t="s">
+      <c r="BK1" s="78" t="s">
         <v>340</v>
       </c>
-      <c r="BK1" s="78" t="s">
+      <c r="BL1" s="65" t="s">
         <v>341</v>
       </c>
-      <c r="BL1" s="65" t="s">
+      <c r="BM1" s="65" t="s">
         <v>342</v>
       </c>
-      <c r="BM1" s="65" t="s">
+      <c r="BN1" s="65" t="s">
         <v>343</v>
       </c>
-      <c r="BN1" s="65" t="s">
+      <c r="BO1" s="65" t="s">
         <v>344</v>
-      </c>
-      <c r="BO1" s="65" t="s">
-        <v>345</v>
       </c>
       <c r="BP1" s="65" t="s">
         <v>106</v>
@@ -3627,43 +4083,43 @@
         <v>149</v>
       </c>
       <c r="BR1" s="65" t="s">
+        <v>345</v>
+      </c>
+      <c r="BS1" s="65" t="s">
         <v>346</v>
       </c>
-      <c r="BS1" s="65" t="s">
+      <c r="BT1" s="65" t="s">
         <v>347</v>
       </c>
-      <c r="BT1" s="65" t="s">
+      <c r="BU1" s="65" t="s">
         <v>348</v>
       </c>
-      <c r="BU1" s="65" t="s">
+      <c r="BV1" s="65" t="s">
         <v>349</v>
       </c>
-      <c r="BV1" s="65" t="s">
+      <c r="BW1" s="65" t="s">
         <v>350</v>
       </c>
-      <c r="BW1" s="65" t="s">
+      <c r="BX1" s="65" t="s">
         <v>351</v>
       </c>
-      <c r="BX1" s="65" t="s">
+      <c r="BY1" s="65" t="s">
         <v>352</v>
       </c>
-      <c r="BY1" s="65" t="s">
+      <c r="BZ1" s="78" t="s">
         <v>353</v>
       </c>
-      <c r="BZ1" s="78" t="s">
+      <c r="CA1" s="78" t="s">
         <v>354</v>
       </c>
-      <c r="CA1" s="78" t="s">
+      <c r="CB1" s="78" t="s">
         <v>355</v>
       </c>
-      <c r="CB1" s="78" t="s">
+      <c r="CC1" s="78" t="s">
         <v>356</v>
       </c>
-      <c r="CC1" s="78" t="s">
+      <c r="CD1" s="65" t="s">
         <v>357</v>
-      </c>
-      <c r="CD1" s="65" t="s">
-        <v>358</v>
       </c>
       <c r="CE1" s="78" t="s">
         <v>284</v>
@@ -3672,15 +4128,15 @@
         <v>285</v>
       </c>
       <c r="CG1" s="27" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="CH1" s="27" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="2" spans="1:86" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B2" s="59" t="s">
         <v>2</v>
@@ -3692,19 +4148,19 @@
         <v>87</v>
       </c>
       <c r="E2" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2" s="62" t="s">
         <v>287</v>
       </c>
-      <c r="F2" s="62" t="s">
-        <v>288</v>
-      </c>
       <c r="G2" s="66" t="s">
+        <v>359</v>
+      </c>
+      <c r="H2" s="60" t="s">
         <v>360</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="I2" s="62" t="s">
         <v>361</v>
-      </c>
-      <c r="I2" s="62" t="s">
-        <v>362</v>
       </c>
       <c r="J2" s="61">
         <v>7899996542</v>
@@ -3713,34 +4169,34 @@
         <v>45940</v>
       </c>
       <c r="L2" s="64" t="s">
+        <v>362</v>
+      </c>
+      <c r="M2" s="58" t="s">
         <v>363</v>
       </c>
-      <c r="M2" s="58" t="s">
+      <c r="N2" s="58" t="s">
         <v>364</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="O2" s="70" t="s">
         <v>365</v>
       </c>
-      <c r="O2" s="70" t="s">
+      <c r="P2" s="58" t="s">
         <v>366</v>
-      </c>
-      <c r="P2" s="58" t="s">
-        <v>367</v>
       </c>
       <c r="Q2" s="58">
         <v>678655</v>
       </c>
       <c r="R2" s="58" t="s">
+        <v>367</v>
+      </c>
+      <c r="S2" s="58" t="s">
         <v>368</v>
       </c>
-      <c r="S2" s="58" t="s">
+      <c r="T2" s="58" t="s">
         <v>369</v>
       </c>
-      <c r="T2" s="58" t="s">
+      <c r="U2" s="68" t="s">
         <v>370</v>
-      </c>
-      <c r="U2" s="68" t="s">
-        <v>371</v>
       </c>
       <c r="V2" s="58">
         <v>19075551234</v>
@@ -3749,13 +4205,13 @@
         <v>7899996742</v>
       </c>
       <c r="X2" s="67" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Y2" s="58" t="s">
+        <v>371</v>
+      </c>
+      <c r="Z2" s="58" t="s">
         <v>372</v>
-      </c>
-      <c r="Z2" s="58" t="s">
-        <v>373</v>
       </c>
       <c r="AA2" s="58">
         <v>6378</v>
@@ -3764,40 +4220,40 @@
         <v>1567</v>
       </c>
       <c r="AC2" s="58" t="s">
+        <v>373</v>
+      </c>
+      <c r="AD2" s="58" t="s">
         <v>374</v>
       </c>
-      <c r="AD2" s="58" t="s">
+      <c r="AE2" s="58" t="s">
         <v>375</v>
       </c>
-      <c r="AE2" s="58" t="s">
+      <c r="AF2" s="58" t="s">
         <v>376</v>
       </c>
-      <c r="AF2" s="58" t="s">
+      <c r="AG2" s="58" t="s">
         <v>377</v>
       </c>
-      <c r="AG2" s="58" t="s">
+      <c r="AH2" s="58" t="s">
         <v>378</v>
       </c>
-      <c r="AH2" s="58" t="s">
+      <c r="AI2" s="58" t="s">
         <v>379</v>
       </c>
-      <c r="AI2" s="58" t="s">
+      <c r="AJ2" s="58" t="s">
         <v>380</v>
       </c>
-      <c r="AJ2" s="58" t="s">
+      <c r="AK2" s="58" t="s">
         <v>381</v>
       </c>
-      <c r="AK2" s="58" t="s">
+      <c r="AL2" s="58" t="s">
         <v>382</v>
       </c>
-      <c r="AL2" s="58" t="s">
+      <c r="AM2" s="58" t="s">
         <v>383</v>
       </c>
-      <c r="AM2" s="58" t="s">
+      <c r="AN2" s="58" t="s">
         <v>384</v>
-      </c>
-      <c r="AN2" s="58" t="s">
-        <v>385</v>
       </c>
       <c r="AO2" s="58">
         <v>357892</v>
@@ -3806,28 +4262,28 @@
         <v>7899996527</v>
       </c>
       <c r="AQ2" s="58" t="s">
+        <v>385</v>
+      </c>
+      <c r="AR2" s="58" t="s">
         <v>386</v>
       </c>
-      <c r="AR2" s="58" t="s">
+      <c r="AS2" s="58" t="s">
         <v>387</v>
       </c>
-      <c r="AS2" s="58" t="s">
+      <c r="AT2" s="58" t="s">
         <v>388</v>
       </c>
-      <c r="AT2" s="58" t="s">
+      <c r="AU2" s="58" t="s">
         <v>389</v>
       </c>
-      <c r="AU2" s="58" t="s">
+      <c r="AV2" s="58" t="s">
         <v>390</v>
       </c>
-      <c r="AV2" s="58" t="s">
+      <c r="AW2" s="58" t="s">
         <v>391</v>
       </c>
-      <c r="AW2" s="58" t="s">
+      <c r="AX2" s="58" t="s">
         <v>392</v>
-      </c>
-      <c r="AX2" s="58" t="s">
-        <v>393</v>
       </c>
       <c r="AY2" s="58">
         <v>766577</v>
@@ -3836,28 +4292,28 @@
         <v>8977667786</v>
       </c>
       <c r="BA2" s="58" t="s">
+        <v>393</v>
+      </c>
+      <c r="BB2" s="58" t="s">
         <v>394</v>
-      </c>
-      <c r="BB2" s="58" t="s">
-        <v>395</v>
       </c>
       <c r="BC2" s="63">
         <v>103000012468</v>
       </c>
       <c r="BD2" s="58" t="s">
+        <v>395</v>
+      </c>
+      <c r="BE2" s="58" t="s">
         <v>396</v>
-      </c>
-      <c r="BE2" s="58" t="s">
-        <v>397</v>
       </c>
       <c r="BF2" s="72">
         <v>146016</v>
       </c>
       <c r="BG2" s="72" t="s">
+        <v>397</v>
+      </c>
+      <c r="BH2" s="58" t="s">
         <v>398</v>
-      </c>
-      <c r="BH2" s="58" t="s">
-        <v>399</v>
       </c>
       <c r="BI2" s="58">
         <v>3636</v>
@@ -3881,10 +4337,10 @@
         <v>13</v>
       </c>
       <c r="BP2" s="58" t="s">
+        <v>399</v>
+      </c>
+      <c r="BQ2" s="58" t="s">
         <v>400</v>
-      </c>
-      <c r="BQ2" s="58" t="s">
-        <v>401</v>
       </c>
       <c r="BR2" s="71">
         <v>123456789123456</v>
@@ -3906,34 +4362,34 @@
         <v>3637</v>
       </c>
       <c r="BY2" s="58" t="s">
+        <v>401</v>
+      </c>
+      <c r="BZ2" s="58" t="s">
         <v>402</v>
       </c>
-      <c r="BZ2" s="58" t="s">
+      <c r="CA2" s="58" t="s">
         <v>403</v>
       </c>
-      <c r="CA2" s="58" t="s">
+      <c r="CB2" s="58" t="s">
         <v>404</v>
       </c>
-      <c r="CB2" s="58" t="s">
+      <c r="CC2" s="72" t="s">
         <v>405</v>
-      </c>
-      <c r="CC2" s="72" t="s">
-        <v>406</v>
       </c>
       <c r="CD2" s="63">
         <v>103000012745</v>
       </c>
       <c r="CE2" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="CF2" s="58" t="s">
         <v>435</v>
       </c>
-      <c r="CF2" s="58" t="s">
-        <v>436</v>
-      </c>
       <c r="CG2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="CH2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3946,7 +4402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -3976,28 +4432,28 @@
         <v>89</v>
       </c>
       <c r="G1" s="76" t="s">
+        <v>406</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>290</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>291</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>292</v>
+      </c>
+      <c r="K1" s="76" t="s">
         <v>407</v>
       </c>
-      <c r="H1" s="76" t="s">
-        <v>291</v>
-      </c>
-      <c r="I1" s="76" t="s">
-        <v>292</v>
-      </c>
-      <c r="J1" s="76" t="s">
-        <v>293</v>
-      </c>
-      <c r="K1" s="76" t="s">
+      <c r="L1" s="76" t="s">
         <v>408</v>
       </c>
-      <c r="L1" s="76" t="s">
+      <c r="M1" s="76" t="s">
         <v>409</v>
       </c>
-      <c r="M1" s="76" t="s">
+      <c r="N1" s="76" t="s">
         <v>410</v>
-      </c>
-      <c r="N1" s="76" t="s">
-        <v>411</v>
       </c>
       <c r="O1" s="76" t="s">
         <v>99</v>
@@ -4006,15 +4462,15 @@
         <v>116</v>
       </c>
       <c r="Q1" s="78" t="s">
+        <v>411</v>
+      </c>
+      <c r="R1" s="78" t="s">
         <v>412</v>
-      </c>
-      <c r="R1" s="78" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B2" s="73" t="s">
         <v>2</v>
@@ -4026,19 +4482,19 @@
         <v>87</v>
       </c>
       <c r="E2" s="73" t="s">
+        <v>414</v>
+      </c>
+      <c r="F2" s="77" t="s">
         <v>415</v>
       </c>
-      <c r="F2" s="77" t="s">
-        <v>416</v>
-      </c>
       <c r="G2" s="79" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H2" s="74" t="s">
+        <v>360</v>
+      </c>
+      <c r="I2" s="77" t="s">
         <v>361</v>
-      </c>
-      <c r="I2" s="77" t="s">
-        <v>362</v>
       </c>
       <c r="J2" s="75">
         <v>7899996542</v>
@@ -4053,19 +4509,19 @@
         <v>5</v>
       </c>
       <c r="N2" s="75" t="s">
+        <v>416</v>
+      </c>
+      <c r="O2" s="75" t="s">
         <v>417</v>
       </c>
-      <c r="O2" s="75" t="s">
+      <c r="P2" s="75" t="s">
         <v>418</v>
       </c>
-      <c r="P2" s="75" t="s">
+      <c r="Q2" s="80" t="s">
         <v>419</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="R2" s="80" t="s">
         <v>420</v>
-      </c>
-      <c r="R2" s="80" t="s">
-        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -4077,7 +4533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -4131,30 +4587,30 @@
         <v>111</v>
       </c>
       <c r="N1" s="82" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="O1" s="84" t="s">
         <v>271</v>
       </c>
       <c r="P1" s="84" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q1" s="84" t="s">
         <v>423</v>
       </c>
-      <c r="Q1" s="84" t="s">
+      <c r="R1" s="84" t="s">
         <v>424</v>
       </c>
-      <c r="R1" s="84" t="s">
+      <c r="S1" s="84" t="s">
         <v>425</v>
       </c>
-      <c r="S1" s="84" t="s">
+      <c r="T1" s="84" t="s">
         <v>426</v>
-      </c>
-      <c r="T1" s="84" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B2" s="81" t="s">
         <v>2</v>
@@ -4166,10 +4622,10 @@
         <v>87</v>
       </c>
       <c r="E2" s="81" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2" s="83" t="s">
         <v>287</v>
-      </c>
-      <c r="F2" s="83" t="s">
-        <v>288</v>
       </c>
       <c r="G2" s="81">
         <v>10300001480</v>
@@ -4187,31 +4643,31 @@
         <v>108</v>
       </c>
       <c r="L2" s="81" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M2" s="81">
         <v>123456</v>
       </c>
       <c r="N2" s="81" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O2" s="87">
         <v>103000014806</v>
       </c>
       <c r="P2" s="88" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q2" s="84" t="s">
         <v>431</v>
-      </c>
-      <c r="Q2" s="84" t="s">
-        <v>432</v>
       </c>
       <c r="R2" s="84">
         <v>4</v>
       </c>
       <c r="S2" s="84" t="s">
+        <v>432</v>
+      </c>
+      <c r="T2" s="84" t="s">
         <v>433</v>
-      </c>
-      <c r="T2" s="84" t="s">
-        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Commit - Fixed Deposit opening - Transfer
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation-Beacon\NBFC_CLS_2.0\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7840C8-CD6D-46C5-9551-4BD32B90BB96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <sheet name="AccountOpening_FixedDeposit" sheetId="13" r:id="rId10"/>
     <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="234">
   <si>
     <t>Run</t>
   </si>
@@ -726,16 +727,22 @@
     <t>Newpassword</t>
   </si>
   <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>Mhatre</t>
+    <t>vijayalakshmi</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>vijayauthorize</t>
+  </si>
+  <si>
+    <t>Pass@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000000"/>
@@ -1281,39 +1288,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection sqref="A1:U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" customWidth="1"/>
+    <col min="3" max="3" width="40.7265625" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="22.54296875" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="20.7265625" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
-    <col min="17" max="17" width="27.42578125" customWidth="1"/>
-    <col min="18" max="18" width="27.85546875" customWidth="1"/>
-    <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.7109375" customWidth="1"/>
-    <col min="25" max="25" width="13.5703125" customWidth="1"/>
+    <col min="17" max="17" width="27.453125" customWidth="1"/>
+    <col min="18" max="18" width="27.81640625" customWidth="1"/>
+    <col min="19" max="19" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.7265625" customWidth="1"/>
+    <col min="25" max="25" width="13.54296875" customWidth="1"/>
     <col min="26" max="26" width="14" customWidth="1"/>
-    <col min="39" max="39" width="21.7109375" customWidth="1"/>
+    <col min="39" max="39" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1397,7 +1404,7 @@
       <c r="AM1" s="9"/>
       <c r="AN1" s="9"/>
     </row>
-    <row r="2" spans="1:40" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1485,25 +1492,26 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.26953125" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" customWidth="1"/>
+    <col min="22" max="22" width="13.26953125" customWidth="1"/>
+    <col min="25" max="25" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1585,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>207</v>
       </c>
@@ -1591,10 +1599,10 @@
         <v>87</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="G2" s="49">
         <v>102000015729</v>
@@ -1645,16 +1653,16 @@
         <v>1000</v>
       </c>
       <c r="W2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="X2" s="55" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="aka@123"/>
-    <hyperlink ref="X2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="X2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1662,52 +1670,52 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView topLeftCell="AB1" workbookViewId="0">
       <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.453125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.1796875" style="40" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.453125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7265625" style="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7265625" style="40" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.1796875" style="40" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="40" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="21.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7265625" style="40" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="21.7265625" style="40" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" style="40" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="40" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16" style="40" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="20.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="20.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.81640625" style="40" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16" style="40" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="20.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="15.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="20.7265625" style="40" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="15.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.26953125" style="40" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.1796875" style="40" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="17" style="40" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="40"/>
+    <col min="38" max="38" width="11.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.1796875" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
@@ -1823,7 +1831,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:38" s="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" s="41" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>157</v>
       </c>
@@ -1941,9 +1949,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="X2" r:id="rId2"/>
-    <hyperlink ref="AL2" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="X2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="AL2" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1951,27 +1959,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="23.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -2000,7 +2008,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>77</v>
       </c>
@@ -2033,19 +2041,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -2074,7 +2082,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>81</v>
       </c>
@@ -2107,16 +2115,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2179,7 +2187,7 @@
       <c r="AN1" s="9"/>
       <c r="AO1" s="9"/>
     </row>
-    <row r="2" spans="1:41" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -2246,23 +2254,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2282,7 +2290,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -2308,16 +2316,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2387,7 +2395,7 @@
       <c r="AQ1" s="9"/>
       <c r="AR1" s="9"/>
     </row>
-    <row r="2" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -2455,7 +2463,7 @@
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>52</v>
       </c>
@@ -2463,7 +2471,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>53</v>
       </c>
@@ -2478,29 +2486,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AR3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1796875" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.1796875" customWidth="1"/>
+    <col min="15" max="15" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2576,7 +2584,7 @@
       <c r="AQ1" s="9"/>
       <c r="AR1" s="9"/>
     </row>
-    <row r="2" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -2650,7 +2658,7 @@
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
         <v>62</v>
       </c>
@@ -2661,62 +2669,62 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="30" customWidth="1"/>
     <col min="5" max="5" width="15" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="30" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="19" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="13.140625" style="30" customWidth="1"/>
-    <col min="24" max="24" width="14.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" style="30"/>
-    <col min="26" max="26" width="22.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.1796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.54296875" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26953125" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.54296875" style="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.54296875" style="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.1796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.1796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13.1796875" style="30" customWidth="1"/>
+    <col min="24" max="24" width="14.1796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.26953125" style="30"/>
+    <col min="26" max="26" width="22.26953125" style="30" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.7265625" style="30" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21" style="30" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.81640625" style="30" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="24" style="30" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.453125" style="30" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="18" style="30" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.1796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.1796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.81640625" style="30" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="19" style="30" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.1796875" style="30" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.81640625" style="30" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="20" style="30" bestFit="1" customWidth="1"/>
-    <col min="46" max="16384" width="17.28515625" style="30"/>
+    <col min="46" max="16384" width="17.26953125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
@@ -2853,7 +2861,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>112</v>
       </c>
@@ -2990,15 +2998,15 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="AJ3" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="Y2" r:id="rId2" display="!@#$%^"/>
-    <hyperlink ref="AA2" r:id="rId3"/>
-    <hyperlink ref="Q2" r:id="rId4"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="Y2" r:id="rId2" display="!@#$%^" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="AA2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="Q2" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -3006,23 +3014,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.81640625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="9" width="20.85546875" style="23"/>
-    <col min="10" max="10" width="13.28515625" style="23" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" style="23"/>
-    <col min="12" max="12" width="26.140625" style="23" customWidth="1"/>
-    <col min="13" max="16384" width="20.85546875" style="23"/>
+    <col min="1" max="9" width="20.81640625" style="23"/>
+    <col min="10" max="10" width="13.26953125" style="23" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" style="23"/>
+    <col min="12" max="12" width="26.1796875" style="23" customWidth="1"/>
+    <col min="13" max="16384" width="20.81640625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -3057,7 +3065,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>113</v>
       </c>
@@ -3094,7 +3102,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="aka@123"/>
+    <hyperlink ref="F2" r:id="rId1" display="aka@123" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated both Gold Loan & Personal Loan Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2296353-3FFC-4029-9C41-71013DE0E3E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC7D4BA-471D-4C8B-BFB8-749B20C6F1D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="10" activeTab="12" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="300">
   <si>
     <t>Run</t>
   </si>
@@ -928,6 +928,15 @@
   </si>
   <si>
     <t>sanctionedAmt</t>
+  </si>
+  <si>
+    <t>WEWE</t>
+  </si>
+  <si>
+    <t>Personal Loan Weekly</t>
+  </si>
+  <si>
+    <t>Gold Loan</t>
   </si>
 </sst>
 </file>
@@ -2377,7 +2386,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,7 +2453,7 @@
     </row>
     <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>200</v>
+        <v>299</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -2496,13 +2505,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18961F5D-5559-4B15-A632-EA58C15475AE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="47"/>
+    <col min="1" max="1" width="20.42578125" style="47" customWidth="1"/>
     <col min="2" max="2" width="6.140625" style="47" customWidth="1"/>
     <col min="3" max="16384" width="18.85546875" style="47"/>
   </cols>
@@ -2556,7 +2565,7 @@
     </row>
     <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>200</v>
+        <v>298</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -2588,8 +2597,8 @@
       <c r="K2" s="47">
         <v>1</v>
       </c>
-      <c r="L2" s="21" t="s">
-        <v>284</v>
+      <c r="L2" t="s">
+        <v>297</v>
       </c>
       <c r="M2" s="47">
         <v>10000</v>

</xml_diff>

<commit_message>
Jewel Gold Loan Renewal Module 1st Commit
Jewel Gold Loan Renewal Module 1st Commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DE1357-14F2-471F-A559-01E381FDC2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92EFFC5-6145-48AF-B24B-02E0F8F8CA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="11" activeTab="11" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="11" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="309">
   <si>
     <t>Run</t>
   </si>
@@ -880,9 +880,6 @@
     <t>AgeAsOn</t>
   </si>
   <si>
-    <t>Multiple FD Opening</t>
-  </si>
-  <si>
     <t>CustomerName</t>
   </si>
   <si>
@@ -937,18 +934,6 @@
     <t>IsMultipleAccountText</t>
   </si>
   <si>
-    <t>LoginNewUserName</t>
-  </si>
-  <si>
-    <t>LoginNewPassword</t>
-  </si>
-  <si>
-    <t>kajol</t>
-  </si>
-  <si>
-    <t>test@123</t>
-  </si>
-  <si>
     <t>GL_Amount</t>
   </si>
   <si>
@@ -956,6 +941,30 @@
   </si>
   <si>
     <t>Multiple FD Opening_Transfer</t>
+  </si>
+  <si>
+    <t>Loan_Closure_Cash</t>
+  </si>
+  <si>
+    <t>Item_Description</t>
+  </si>
+  <si>
+    <t>Item_Quantity</t>
+  </si>
+  <si>
+    <t>necklace</t>
+  </si>
+  <si>
+    <t>Stone_Weight</t>
+  </si>
+  <si>
+    <t>Item_Weight</t>
+  </si>
+  <si>
+    <t>Dirt_Weight</t>
+  </si>
+  <si>
+    <t>Enter_Purity</t>
   </si>
 </sst>
 </file>
@@ -2415,7 +2424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BDDCE6-BD63-42C9-AF7A-6F36E86885A8}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2438,51 +2447,51 @@
         <v>86</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F1" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="20" t="s">
-        <v>287</v>
-      </c>
       <c r="K1" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="L1" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="L1" s="20" t="s">
-        <v>290</v>
-      </c>
       <c r="M1" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O1" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="P1" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="Q1" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="R1" s="40" t="s">
         <v>298</v>
-      </c>
-      <c r="R1" s="40" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -2494,7 +2503,7 @@
         <v>87</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F2">
         <v>500000</v>
@@ -2509,19 +2518,19 @@
         <v>630</v>
       </c>
       <c r="J2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K2">
         <v>4000</v>
       </c>
       <c r="L2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -2543,15 +2552,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114A26A3-26D4-4B0C-9E41-5E33C05312DF}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -2565,54 +2574,48 @@
         <v>86</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F1" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="20" t="s">
-        <v>287</v>
-      </c>
       <c r="K1" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="L1" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="L1" s="20" t="s">
-        <v>290</v>
-      </c>
       <c r="M1" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O1" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="P1" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="Q1" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="Q1" s="40" t="s">
-        <v>298</v>
-      </c>
-      <c r="R1" s="40" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>299</v>
-      </c>
-      <c r="S1" s="40" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>304</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -2624,7 +2627,7 @@
         <v>87</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F2">
         <v>500000</v>
@@ -2639,19 +2642,19 @@
         <v>630</v>
       </c>
       <c r="J2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K2">
         <v>4000</v>
       </c>
       <c r="L2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -2662,17 +2665,8 @@
       <c r="Q2">
         <v>5</v>
       </c>
-      <c r="R2" t="s">
-        <v>301</v>
-      </c>
-      <c r="S2" s="41" t="s">
-        <v>302</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{C7A33926-3606-4272-86C8-62BDACB03FA9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2681,13 +2675,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D198CE-51CE-4243-8BC2-307B322856E1}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2704,54 +2706,36 @@
         <v>86</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>285</v>
+        <v>306</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="P1" s="40" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q1" s="40" t="s">
-        <v>298</v>
-      </c>
-      <c r="R1" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="S1" s="40" t="s">
-        <v>300</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -2763,55 +2747,26 @@
         <v>87</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>282</v>
+        <v>304</v>
       </c>
       <c r="F2">
-        <v>500000</v>
+        <v>25</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="I2">
-        <v>630</v>
-      </c>
-      <c r="J2" t="s">
-        <v>288</v>
-      </c>
-      <c r="K2">
-        <v>4000</v>
-      </c>
-      <c r="L2" t="s">
-        <v>291</v>
-      </c>
-      <c r="M2" t="s">
-        <v>295</v>
-      </c>
-      <c r="N2" t="s">
-        <v>293</v>
-      </c>
-      <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>5</v>
-      </c>
-      <c r="R2" t="s">
-        <v>301</v>
-      </c>
-      <c r="S2" s="41" t="s">
-        <v>302</v>
-      </c>
+      <c r="J2">
+        <v>22</v>
+      </c>
+      <c r="S2" s="41"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{1FF19BBF-A627-4A1B-822F-7F51DBF067A4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated the script as required - Fixed Deposit (Client registration and Authorization part modified)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7840C8-CD6D-46C5-9551-4BD32B90BB96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0AF5C3-C218-4A7C-A6B1-391182C43C15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="235">
   <si>
     <t>Run</t>
   </si>
@@ -737,6 +737,9 @@
   </si>
   <si>
     <t>Pass@123</t>
+  </si>
+  <si>
+    <t>Transactionid</t>
   </si>
 </sst>
 </file>
@@ -1493,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1511,7 +1514,7 @@
     <col min="25" max="25" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1584,8 +1587,11 @@
       <c r="X1" s="52" t="s">
         <v>229</v>
       </c>
+      <c r="Y1" s="52" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>207</v>
       </c>
@@ -1657,6 +1663,9 @@
       </c>
       <c r="X2" s="55" t="s">
         <v>233</v>
+      </c>
+      <c r="Y2">
+        <v>617339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Commit-General opening Cash
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinusha.shetty\Documents\GitHub\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC7D4BA-471D-4C8B-BFB8-749B20C6F1D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03576EEF-078D-4502-A118-BFCB8C32ACA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="10" activeTab="12" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Customer_NewCustomer" sheetId="13" r:id="rId11"/>
     <sheet name="AccOpn_JewelLoan_GoldLoan" sheetId="15" r:id="rId12"/>
     <sheet name="AccOpn_LoanAdva_PersnlLoanWeek" sheetId="16" r:id="rId13"/>
+    <sheet name="GeneralOpening" sheetId="17" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="306">
   <si>
     <t>Run</t>
   </si>
@@ -937,6 +938,24 @@
   </si>
   <si>
     <t>Gold Loan</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>Openaccount</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -2505,8 +2524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18961F5D-5559-4B15-A632-EA58C15475AE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2608,6 +2627,74 @@
       </c>
       <c r="O2" s="47">
         <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADC2D69-8F2A-4C4D-B091-B72256E6B3B3}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2">
+        <v>500000</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="H2">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gold Loan Renewal Cash
Gold Loan Renewal Cash
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92EFFC5-6145-48AF-B24B-02E0F8F8CA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9C61F9-6CD5-4FDD-9BFE-9B37750C081D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="11" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="12" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,8 @@
     <sheet name="Customer_NewCustomer" sheetId="13" r:id="rId11"/>
     <sheet name="Multiple_FD_Transfer" sheetId="15" r:id="rId12"/>
     <sheet name="Multiple_FD_Cash" sheetId="14" r:id="rId13"/>
-    <sheet name="Closure_and_Renewals_Cash" sheetId="16" r:id="rId14"/>
+    <sheet name="Closure_and_Renewals_Transfer" sheetId="17" r:id="rId14"/>
+    <sheet name="Closure_and_Renewals_Cash" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="311">
   <si>
     <t>Run</t>
   </si>
@@ -965,6 +966,12 @@
   </si>
   <si>
     <t>Enter_Purity</t>
+  </si>
+  <si>
+    <t>Sanctioned_Amount</t>
+  </si>
+  <si>
+    <t>Loan_Closure_Transfer</t>
   </si>
 </sst>
 </file>
@@ -2672,11 +2679,122 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B90D486-903F-4F95-9CDA-9638AB00129B}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+    </row>
+    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>22</v>
+      </c>
+      <c r="K2">
+        <v>323975</v>
+      </c>
+      <c r="L2" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D198CE-51CE-4243-8BC2-307B322856E1}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,6 +2808,7 @@
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2723,8 +2842,12 @@
       <c r="J1" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
+      <c r="K1" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>286</v>
+      </c>
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
@@ -2763,6 +2886,12 @@
       </c>
       <c r="J2">
         <v>22</v>
+      </c>
+      <c r="K2">
+        <v>323975</v>
+      </c>
+      <c r="L2" t="s">
+        <v>287</v>
       </c>
       <c r="S2" s="41"/>
     </row>

</xml_diff>

<commit_message>
Completed both Suspense_Asset & Deposit_Loan Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC7D4BA-471D-4C8B-BFB8-749B20C6F1D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCE55C5-AA50-4327-A27C-B223268FD693}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="10" activeTab="12" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="13" activeTab="14" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="Customer_NewCustomer" sheetId="13" r:id="rId11"/>
     <sheet name="AccOpn_JewelLoan_GoldLoan" sheetId="15" r:id="rId12"/>
     <sheet name="AccOpn_LoanAdva_PersnlLoanWeek" sheetId="16" r:id="rId13"/>
+    <sheet name="DepoOpn_FxdDepo_BondCumulative" sheetId="17" r:id="rId14"/>
+    <sheet name="GeneralOpening_SuspenseAsset" sheetId="18" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="310">
   <si>
     <t>Run</t>
   </si>
@@ -937,6 +939,36 @@
   </si>
   <si>
     <t>Gold Loan</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Deposit Loan</t>
+  </si>
+  <si>
+    <t>accNum</t>
+  </si>
+  <si>
+    <t>nomineeAadhaar</t>
+  </si>
+  <si>
+    <t>nomineeCustId</t>
+  </si>
+  <si>
+    <t>quick vasu</t>
+  </si>
+  <si>
+    <t>nomineeDOB</t>
+  </si>
+  <si>
+    <t>Suspense Asset</t>
+  </si>
+  <si>
+    <t>openingAmt</t>
   </si>
 </sst>
 </file>
@@ -2505,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18961F5D-5559-4B15-A632-EA58C15475AE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2613,6 +2645,174 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A293D14-2B59-43EF-9E33-943EC1F10100}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2">
+        <v>327</v>
+      </c>
+      <c r="H2" s="25">
+        <v>151525256636</v>
+      </c>
+      <c r="I2" s="25">
+        <v>102000015929</v>
+      </c>
+      <c r="J2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K2" s="45">
+        <v>135142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA0B315-22E7-482C-AEAA-F94A2BA4AD7B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Authorize credentials is updated in Config properties. Suggestions are working fine
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0AF5C3-C218-4A7C-A6B1-391182C43C15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4132E8FA-2C8E-4C58-805C-BBD242FAB008}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Customer_CustRegister" sheetId="10" r:id="rId9"/>
     <sheet name="AccountOpening_FixedDeposit" sheetId="13" r:id="rId10"/>
     <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId11"/>
+    <sheet name="AccountOpening_Loan_ACOPL_TwoWh" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="230">
   <si>
     <t>Run</t>
   </si>
@@ -721,25 +722,10 @@
     <t>Relation/Desig.</t>
   </si>
   <si>
-    <t>Newuserid</t>
-  </si>
-  <si>
-    <t>Newpassword</t>
-  </si>
-  <si>
-    <t>vijayalakshmi</t>
-  </si>
-  <si>
-    <t>test@123</t>
-  </si>
-  <si>
-    <t>vijayauthorize</t>
-  </si>
-  <si>
-    <t>Pass@123</t>
-  </si>
-  <si>
     <t>Transactionid</t>
+  </si>
+  <si>
+    <t>AccountOpening_loanOpening_ACOPL_TwoWheeler</t>
   </si>
 </sst>
 </file>
@@ -842,7 +828,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -976,7 +962,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1496,25 +1481,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.26953125" customWidth="1"/>
-    <col min="25" max="25" width="11.6328125" customWidth="1"/>
+    <col min="5" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.26953125" customWidth="1"/>
+    <col min="21" max="21" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1527,71 +1510,59 @@
       <c r="D1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>89</v>
+      <c r="E1" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>209</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="I1" s="48" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="J1" s="48" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="K1" s="48" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="L1" s="48" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M1" s="48" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="N1" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="O1" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="P1" s="48" t="s">
         <v>220</v>
       </c>
+      <c r="O1" s="52" t="s">
+        <v>221</v>
+      </c>
+      <c r="P1" s="52" t="s">
+        <v>227</v>
+      </c>
       <c r="Q1" s="52" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="R1" s="52" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="S1" s="52" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="T1" s="52" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="U1" s="52" t="s">
-        <v>224</v>
-      </c>
-      <c r="V1" s="52" t="s">
-        <v>225</v>
-      </c>
-      <c r="W1" s="52" t="s">
         <v>228</v>
       </c>
-      <c r="X1" s="52" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y1" s="52" t="s">
-        <v>234</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>207</v>
       </c>
@@ -1604,77 +1575,61 @@
       <c r="D2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="G2" s="49">
+      <c r="E2" s="49">
         <v>102000015729</v>
       </c>
-      <c r="H2" s="50">
+      <c r="F2" s="50">
         <v>200000</v>
       </c>
-      <c r="I2" s="51">
+      <c r="G2" s="51">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H2" t="s">
         <v>212</v>
       </c>
-      <c r="K2">
+      <c r="I2">
         <v>11</v>
       </c>
-      <c r="L2">
+      <c r="J2">
         <v>5</v>
       </c>
+      <c r="K2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" s="50">
+        <v>1000</v>
+      </c>
       <c r="M2" t="s">
-        <v>216</v>
-      </c>
-      <c r="N2" s="50">
+        <v>219</v>
+      </c>
+      <c r="N2" s="49">
+        <v>103000012745</v>
+      </c>
+      <c r="O2" s="53">
+        <v>103000012519</v>
+      </c>
+      <c r="P2" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>222</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>2</v>
+      </c>
+      <c r="T2" s="54">
         <v>1000</v>
       </c>
-      <c r="O2" t="s">
-        <v>219</v>
-      </c>
-      <c r="P2" s="49">
-        <v>103000012745</v>
-      </c>
-      <c r="Q2" s="53">
-        <v>103000012519</v>
-      </c>
-      <c r="R2" t="s">
-        <v>177</v>
-      </c>
-      <c r="S2" t="s">
-        <v>222</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
       <c r="U2">
-        <v>2</v>
-      </c>
-      <c r="V2" s="54">
-        <v>1000</v>
-      </c>
-      <c r="W2" t="s">
-        <v>232</v>
-      </c>
-      <c r="X2" s="55" t="s">
-        <v>233</v>
-      </c>
-      <c r="Y2">
         <v>617339</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="X2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1964,6 +1919,52 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Third Commit- general opening
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinusha.shetty\Documents\GitHub\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583A68D9-5200-4B51-A315-E5966B8769BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B4A5AB-52DF-4CBD-ABA1-369163F77D2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="11" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="12" activeTab="14" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="AccOpn_JewelLoan_GoldLoan" sheetId="15" r:id="rId12"/>
     <sheet name="AccOpn_LoanAdva_PersnlLoanWeek" sheetId="16" r:id="rId13"/>
     <sheet name="GeneralOpening" sheetId="17" r:id="rId14"/>
+    <sheet name="JewelClosure" sheetId="18" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="306">
   <si>
     <t>Run</t>
   </si>
@@ -2218,7 +2219,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>200</v>
       </c>
@@ -2639,8 +2640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADC2D69-8F2A-4C4D-B091-B72256E6B3B3}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,6 +2701,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EA83C6-9643-4AD8-92C4-848D1A561ED9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Otherloan-Vehiclesecurity-cash flow(TwoWheelerLoan 23027)  first push
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4132E8FA-2C8E-4C58-805C-BBD242FAB008}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E30300D-E124-4AEC-BE55-CB9D407894B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="233">
   <si>
     <t>Run</t>
   </si>
@@ -726,6 +726,15 @@
   </si>
   <si>
     <t>AccountOpening_loanOpening_ACOPL_TwoWheeler</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>ADI</t>
+  </si>
+  <si>
+    <t>ResolutionNo</t>
   </si>
 </sst>
 </file>
@@ -1483,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V1" activeCellId="1" sqref="N1:N2 V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1638,7 +1647,7 @@
   <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+      <selection activeCell="AE1" sqref="AE1:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1924,18 +1933,21 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1948,8 +1960,17 @@
       <c r="D1" s="20" t="s">
         <v>86</v>
       </c>
+      <c r="E1" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>229</v>
       </c>
@@ -1961,6 +1982,15 @@
       </c>
       <c r="D2" s="3" t="s">
         <v>87</v>
+      </c>
+      <c r="E2" s="53">
+        <v>102000015729</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>231</v>
+      </c>
+      <c r="G2" s="41">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fourth commit Jewel Loan Closure Cash and transfer
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinusha.shetty\Documents\GitHub\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B4A5AB-52DF-4CBD-ABA1-369163F77D2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B3FDB8-B730-4B6C-B5DF-1A35F5A086F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="12" activeTab="14" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="12" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="309">
   <si>
     <t>Run</t>
   </si>
@@ -957,6 +957,15 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>JewlClosure</t>
+  </si>
+  <si>
+    <t>GeneralOpening</t>
   </si>
 </sst>
 </file>
@@ -2219,7 +2228,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>200</v>
       </c>
@@ -2640,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADC2D69-8F2A-4C4D-B091-B72256E6B3B3}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2672,9 +2681,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -2706,15 +2715,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EA83C6-9643-4AD8-92C4-848D1A561ED9}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -2727,10 +2736,19 @@
       <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
+      <c r="E1" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>305</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -2740,6 +2758,15 @@
       </c>
       <c r="D2" s="29" t="s">
         <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>5568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module - Transactions_Jewel (Cash & Transfer) - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCE55C5-AA50-4327-A27C-B223268FD693}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED73108F-8335-4A64-84C9-DB9DA2C1B057}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="13" activeTab="14" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="13" activeTab="15" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="AccOpn_LoanAdva_PersnlLoanWeek" sheetId="16" r:id="rId13"/>
     <sheet name="DepoOpn_FxdDepo_BondCumulative" sheetId="17" r:id="rId14"/>
     <sheet name="GeneralOpening_SuspenseAsset" sheetId="18" r:id="rId15"/>
+    <sheet name="Transactions_Jewel" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="311">
   <si>
     <t>Run</t>
   </si>
@@ -969,6 +970,9 @@
   </si>
   <si>
     <t>openingAmt</t>
+  </si>
+  <si>
+    <t>Transactions_Jewel</t>
   </si>
 </sst>
 </file>
@@ -2750,8 +2754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA0B315-22E7-482C-AEAA-F94A2BA4AD7B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2809,6 +2813,67 @@
       </c>
       <c r="G2">
         <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E9BB6C-5F71-4838-A95A-B4D261F9C9B2}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I have corrected the errors (failures code updated and xpath issue resolved)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E30300D-E124-4AEC-BE55-CB9D407894B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF6CF3-E560-49D2-9318-73CE2D7311F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="238">
   <si>
     <t>Run</t>
   </si>
@@ -731,10 +731,25 @@
     <t>customerName</t>
   </si>
   <si>
-    <t>ADI</t>
-  </si>
-  <si>
     <t>ResolutionNo</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>ResoultionDate</t>
+  </si>
+  <si>
+    <t>30/05/2025</t>
+  </si>
+  <si>
+    <t>PRADEEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canvassername </t>
+  </si>
+  <si>
+    <t>ASMA</t>
   </si>
 </sst>
 </file>
@@ -1492,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V1" activeCellId="1" sqref="N1:N2 V1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AE2"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1:AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1933,10 +1948,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1945,9 +1960,11 @@
     <col min="5" max="5" width="13.1796875" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" customWidth="1"/>
     <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1967,10 +1984,19 @@
         <v>230</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>229</v>
       </c>
@@ -1984,17 +2010,27 @@
         <v>87</v>
       </c>
       <c r="E2" s="53">
-        <v>102000015729</v>
+        <v>103000012417</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G2" s="41">
         <v>1234</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="I2" t="s">
+        <v>235</v>
+      </c>
+      <c r="J2" s="53" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Module - ShareOpening_AClassShare (Cash & Transfer) Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED73108F-8335-4A64-84C9-DB9DA2C1B057}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F529C2-E898-4139-9408-ADD35E64AE04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="13" activeTab="15" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="14" activeTab="16" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="DepoOpn_FxdDepo_BondCumulative" sheetId="17" r:id="rId14"/>
     <sheet name="GeneralOpening_SuspenseAsset" sheetId="18" r:id="rId15"/>
     <sheet name="Transactions_Jewel" sheetId="19" r:id="rId16"/>
+    <sheet name="ShareOpn_AClassShare" sheetId="20" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="314">
   <si>
     <t>Run</t>
   </si>
@@ -973,6 +974,15 @@
   </si>
   <si>
     <t>Transactions_Jewel</t>
+  </si>
+  <si>
+    <t>Share Opening_A class Share</t>
+  </si>
+  <si>
+    <t>ab3110cd</t>
+  </si>
+  <si>
+    <t>shares</t>
   </si>
 </sst>
 </file>
@@ -2657,7 +2667,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2755,7 +2765,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2824,8 +2834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E9BB6C-5F71-4838-A95A-B4D261F9C9B2}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2874,6 +2884,78 @@
       </c>
       <c r="G2">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C893DE7D-9C23-4ECD-A939-5604C80AB096}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="45">
+        <v>138794</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="H2" s="47">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Error fixed in FD opening
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF6CF3-E560-49D2-9318-73CE2D7311F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53F66A-D0A8-4875-8338-2884231487E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="244">
   <si>
     <t>Run</t>
   </si>
@@ -743,13 +743,31 @@
     <t>30/05/2025</t>
   </si>
   <si>
-    <t>PRADEEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canvassername </t>
-  </si>
-  <si>
-    <t>ASMA</t>
+    <t>EquitableMortRegNo</t>
+  </si>
+  <si>
+    <t>Ad353</t>
+  </si>
+  <si>
+    <t>EMRDate</t>
+  </si>
+  <si>
+    <t>15/04/2025</t>
+  </si>
+  <si>
+    <t>Agentcode</t>
+  </si>
+  <si>
+    <t>DSACode</t>
+  </si>
+  <si>
+    <t>VehicleNo</t>
+  </si>
+  <si>
+    <t>TN 01 AB 1234</t>
+  </si>
+  <si>
+    <t>RC.No</t>
   </si>
 </sst>
 </file>
@@ -1948,10 +1966,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1961,10 +1979,14 @@
     <col min="6" max="6" width="14.08984375" customWidth="1"/>
     <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.81640625" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1989,14 +2011,26 @@
       <c r="H1" s="27" t="s">
         <v>233</v>
       </c>
-      <c r="I1" s="52" t="s">
-        <v>211</v>
-      </c>
-      <c r="J1" s="52" t="s">
-        <v>236</v>
+      <c r="I1" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>229</v>
       </c>
@@ -2021,11 +2055,23 @@
       <c r="H2" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="I2" t="s">
-        <v>235</v>
-      </c>
-      <c r="J2" s="53" t="s">
-        <v>237</v>
+      <c r="I2" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="K2" s="41">
+        <v>7</v>
+      </c>
+      <c r="L2" s="41">
+        <v>1</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="N2" s="41">
+        <v>1234567890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6th commit JewelLoan closure
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinusha.shetty\Documents\GitHub\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B3FDB8-B730-4B6C-B5DF-1A35F5A086F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D65A65D-1F8E-4234-9376-526592347505}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="12" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="310">
   <si>
     <t>Run</t>
   </si>
@@ -966,6 +966,9 @@
   </si>
   <si>
     <t>GeneralOpening</t>
+  </si>
+  <si>
+    <t>TransAmount</t>
   </si>
 </sst>
 </file>
@@ -2647,15 +2650,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADC2D69-8F2A-4C4D-B091-B72256E6B3B3}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -2680,8 +2683,11 @@
       <c r="H1" s="26" t="s">
         <v>305</v>
       </c>
+      <c r="I1" s="26" t="s">
+        <v>309</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>308</v>
       </c>
@@ -2705,6 +2711,9 @@
       </c>
       <c r="H2">
         <v>500000</v>
+      </c>
+      <c r="I2">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jewel gold loan renewel issue resolved
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DDE81C-CC3F-4FC9-8C37-933814B5793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E5D0AF-13D3-4163-8DEA-2D15988D0F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="12" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="12" activeTab="14" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -28,6 +28,8 @@
     <sheet name="Multiple_FD_Cash" sheetId="14" r:id="rId13"/>
     <sheet name="Jewel_GoldLoan_Renewal_Transfer" sheetId="17" r:id="rId14"/>
     <sheet name="Jewel_Gold_Loan_Renewal_Cash" sheetId="16" r:id="rId15"/>
+    <sheet name="Jewel_Loan_Transcharge_Transfer" sheetId="20" r:id="rId16"/>
+    <sheet name="Jewel_Loan_Transcharge_Cash" sheetId="19" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="315">
   <si>
     <t>Run</t>
   </si>
@@ -978,18 +980,25 @@
   </si>
   <si>
     <t>Jewel_Gold_Loan_Renewal_Cash</t>
+  </si>
+  <si>
+    <t>Jewel_Loan_Transcharge_Cash</t>
+  </si>
+  <si>
+    <t>Trans_Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000000"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="00000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1081,7 +1090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1195,6 +1204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2688,8 +2698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B90D486-903F-4F95-9CDA-9638AB00129B}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2811,8 +2821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D198CE-51CE-4243-8BC2-307B322856E1}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,9 +2916,191 @@
         <v>22</v>
       </c>
       <c r="K2">
-        <v>77648</v>
+        <v>115132</v>
       </c>
       <c r="L2" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A2D4F4-53C4-4CDF-AD04-714D1833AF0B}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+    </row>
+    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="16">
+        <v>100</v>
+      </c>
+      <c r="F2" s="43">
+        <v>500</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="H2" s="42">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>500</v>
+      </c>
+      <c r="S2" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECA92A6-11EC-4522-BB26-96E840668B4C}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+    </row>
+    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="16">
+        <v>100</v>
+      </c>
+      <c r="F2" s="43">
+        <v>500</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>287</v>
       </c>
       <c r="S2" s="41"/>

</xml_diff>

<commit_message>
Jewel Gold loan Renewal Transfer module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E5D0AF-13D3-4163-8DEA-2D15988D0F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56706A9A-9D2B-444E-9B29-A44EF592BFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="12" activeTab="14" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="13" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -2698,8 +2698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B90D486-903F-4F95-9CDA-9638AB00129B}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,7 +2799,7 @@
         <v>22</v>
       </c>
       <c r="K2">
-        <v>77648</v>
+        <v>182069</v>
       </c>
       <c r="L2" t="s">
         <v>287</v>
@@ -2808,7 +2808,7 @@
         <v>3</v>
       </c>
       <c r="N2">
-        <v>61583</v>
+        <v>66937</v>
       </c>
       <c r="S2" s="41"/>
     </row>
@@ -2821,7 +2821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D198CE-51CE-4243-8BC2-307B322856E1}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Transaction_Transactions_Jewel (Cash & Transfer), Error fixed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F529C2-E898-4139-9408-ADD35E64AE04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103E904F-794C-4B9F-8EC7-55296FA2899C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="14" activeTab="16" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="17" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="GeneralOpening_SuspenseAsset" sheetId="18" r:id="rId15"/>
     <sheet name="Transactions_Jewel" sheetId="19" r:id="rId16"/>
     <sheet name="ShareOpn_AClassShare" sheetId="20" r:id="rId17"/>
+    <sheet name="LoanChargePosting" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="315">
   <si>
     <t>Run</t>
   </si>
@@ -983,6 +984,9 @@
   </si>
   <si>
     <t>shares</t>
+  </si>
+  <si>
+    <t>ChargePosting_LoanChargePosting</t>
   </si>
 </sst>
 </file>
@@ -2835,7 +2839,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,7 +2881,7 @@
         <v>87</v>
       </c>
       <c r="E2">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>301</v>
@@ -2895,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C893DE7D-9C23-4ECD-A939-5604C80AB096}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,6 +2960,55 @@
       </c>
       <c r="H2" s="47">
         <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C227A2-6798-4C87-8584-0248AD2A50A5}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module - Processing&Posting_ChargePosting_LoanChargePosting (Cash & Transfer) Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103E904F-794C-4B9F-8EC7-55296FA2899C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1575F3-F290-473B-9160-E2377059DF3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="17" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="315">
   <si>
     <t>Run</t>
   </si>
@@ -993,12 +993,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000000"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="00000000000000"/>
+    <numFmt numFmtId="169" formatCode="0000.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1090,7 +1091,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1222,6 +1223,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2839,7 +2841,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,15 +2971,15 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C227A2-6798-4C87-8584-0248AD2A50A5}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -2993,8 +2995,14 @@
       <c r="E1" s="26" t="s">
         <v>285</v>
       </c>
+      <c r="F1" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>303</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>314</v>
       </c>
@@ -3007,12 +3015,19 @@
       <c r="D2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="E2">
-        <v>2000</v>
+      <c r="E2" s="51">
+        <v>5000</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Jewel Loan transaction transfer module
Jewel Loan transaction transfer module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56706A9A-9D2B-444E-9B29-A44EF592BFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524B3734-0164-407A-A244-DD5320D7A9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="13" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="14" activeTab="15" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="316">
   <si>
     <t>Run</t>
   </si>
@@ -986,6 +986,9 @@
   </si>
   <si>
     <t>Trans_Amount</t>
+  </si>
+  <si>
+    <t>Jewel_Loan_Transcharge_Transfer</t>
   </si>
 </sst>
 </file>
@@ -2698,7 +2701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B90D486-903F-4F95-9CDA-9638AB00129B}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -2932,13 +2935,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A2D4F4-53C4-4CDF-AD04-714D1833AF0B}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
@@ -2991,7 +2994,7 @@
     </row>
     <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Rework Jewel Loan Renewal Transfer
Rework Jewel Loan Renewal Transfer
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524B3734-0164-407A-A244-DD5320D7A9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BFA613-85AF-47E9-9117-7A915E7FA886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="14" activeTab="15" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="13" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Jewel_Gold_Loan_Renewal_Cash" sheetId="16" r:id="rId15"/>
     <sheet name="Jewel_Loan_Transcharge_Transfer" sheetId="20" r:id="rId16"/>
     <sheet name="Jewel_Loan_Transcharge_Cash" sheetId="19" r:id="rId17"/>
+    <sheet name="GL_Acc_Trans_Cash" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="317">
   <si>
     <t>Run</t>
   </si>
@@ -989,6 +990,9 @@
   </si>
   <si>
     <t>Jewel_Loan_Transcharge_Transfer</t>
+  </si>
+  <si>
+    <t>GL_Acc_Transaction_Cash</t>
   </si>
 </sst>
 </file>
@@ -2701,8 +2705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B90D486-903F-4F95-9CDA-9638AB00129B}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2802,7 +2806,7 @@
         <v>22</v>
       </c>
       <c r="K2">
-        <v>182069</v>
+        <v>195458</v>
       </c>
       <c r="L2" t="s">
         <v>287</v>
@@ -2811,7 +2815,7 @@
         <v>3</v>
       </c>
       <c r="N2">
-        <v>66937</v>
+        <v>329375</v>
       </c>
       <c r="S2" s="41"/>
     </row>
@@ -2935,7 +2939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A2D4F4-53C4-4CDF-AD04-714D1833AF0B}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -3087,6 +3091,92 @@
     <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>313</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="16">
+        <v>100</v>
+      </c>
+      <c r="F2" s="43">
+        <v>500</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AECF4C-F4E6-4F57-8D51-CCB135FF85E6}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>316</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
OL Transaction and OL closure
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinusha.shetty\Documents\GitHub\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B130D91C-B781-4083-9176-172CA91325AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE74D0E6-A1DC-4BBA-B4A5-D0A3756C15B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="12" activeTab="15" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="13" activeTab="17" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -29,6 +29,8 @@
     <sheet name="GeneralOpening" sheetId="17" r:id="rId14"/>
     <sheet name="JewelClosure" sheetId="18" r:id="rId15"/>
     <sheet name="Transaction" sheetId="19" r:id="rId16"/>
+    <sheet name="TransactionClosure" sheetId="20" r:id="rId17"/>
+    <sheet name="SuspenseAsset" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="312">
   <si>
     <t>Run</t>
   </si>
@@ -966,10 +968,16 @@
     <t>AccountNumber</t>
   </si>
   <si>
-    <t>Transactiother_Loan_Cash_Transfer</t>
-  </si>
-  <si>
     <t>Transferamount</t>
+  </si>
+  <si>
+    <t>Other_Loan_Transaction_Cash_and_Transfer</t>
+  </si>
+  <si>
+    <t>Other_Loan_Closure_Cash_and_Transfer</t>
+  </si>
+  <si>
+    <t>SusAssetTransaction-Cash_Transfer</t>
   </si>
 </sst>
 </file>
@@ -2800,8 +2808,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413AA4D7-50EF-4C1B-85A7-D00937A17C5D}">
   <dimension ref="A1:K2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2">
+        <v>500000</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="H2">
+        <v>500000</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" s="21">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6FDE26-2090-4565-A99C-803235B88492}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2">
+        <v>500000</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="H2">
+        <v>500000</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" s="21">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A06A448-AC82-4C19-B1FF-9C1FCCE07522}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,12 +3022,12 @@
         <v>307</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Updated class names as required and placed under Transaction package.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1575F3-F290-473B-9160-E2377059DF3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA0E1D-D3B7-4353-969B-CB7E29D58E09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="17" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="16" activeTab="19" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -31,6 +31,8 @@
     <sheet name="Transactions_Jewel" sheetId="19" r:id="rId16"/>
     <sheet name="ShareOpn_AClassShare" sheetId="20" r:id="rId17"/>
     <sheet name="LoanChargePosting" sheetId="21" r:id="rId18"/>
+    <sheet name="MembMang_Loan" sheetId="22" r:id="rId19"/>
+    <sheet name="MembMang_Deposit" sheetId="23" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="320">
   <si>
     <t>Run</t>
   </si>
@@ -987,6 +989,21 @@
   </si>
   <si>
     <t>ChargePosting_LoanChargePosting</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>MemberManagement_Deposit</t>
+  </si>
+  <si>
+    <t>MemberManagement_Loan</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -2973,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C227A2-6798-4C87-8584-0248AD2A50A5}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,6 +3045,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1995239C-1EAA-4833-968E-62F8E1515AF6}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3106,6 +3178,61 @@
       <c r="H2" s="18"/>
       <c r="I2" s="19" t="s">
         <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A867EB9B-F04E-43CD-8EA1-F0F23332E62D}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renewal transfer module updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DACD92-F304-4BD9-83B8-EB718F7AEA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D11018-EA59-43AB-BA97-BB5A0DA69DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="15" activeTab="17" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="13" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,8 @@
     <sheet name="Jewel_Gold_Loan_Renewal_Cash" sheetId="16" r:id="rId15"/>
     <sheet name="Jewel_Loan_Transcharge_Transfer" sheetId="20" r:id="rId16"/>
     <sheet name="Jewel_Loan_Transcharge_Cash" sheetId="19" r:id="rId17"/>
-    <sheet name="GL_Acc_Trans_Cash" sheetId="21" r:id="rId18"/>
+    <sheet name="GL_Acc_Trans_Transfer" sheetId="22" r:id="rId18"/>
+    <sheet name="GL_Acc_Trans_Cash" sheetId="21" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="319">
   <si>
     <t>Run</t>
   </si>
@@ -974,9 +975,6 @@
     <t>Account_Number</t>
   </si>
   <si>
-    <t>Enter_Amount</t>
-  </si>
-  <si>
     <t>Jewel_Gold_Loan_Renewal_Transfer</t>
   </si>
   <si>
@@ -999,6 +997,9 @@
   </si>
   <si>
     <t>Particulars</t>
+  </si>
+  <si>
+    <t>GL_Acc_Transaction_Transfer</t>
   </si>
 </sst>
 </file>
@@ -2712,10 +2713,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B90D486-903F-4F95-9CDA-9638AB00129B}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2729,12 +2730,10 @@
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -2766,26 +2765,20 @@
         <v>307</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>308</v>
-      </c>
-      <c r="L1" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="L1" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="N1" s="20" t="s">
-        <v>310</v>
-      </c>
-      <c r="O1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
       <c r="P1" s="40"/>
       <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
     </row>
-    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -2814,19 +2807,13 @@
       <c r="J2">
         <v>22</v>
       </c>
-      <c r="K2">
-        <v>195458</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2" t="s">
         <v>287</v>
       </c>
-      <c r="M2" s="42">
+      <c r="L2" s="42">
         <v>3</v>
       </c>
-      <c r="N2">
-        <v>329375</v>
-      </c>
-      <c r="S2" s="41"/>
+      <c r="Q2" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2902,7 +2889,7 @@
     </row>
     <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -2946,10 +2933,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A2D4F4-53C4-4CDF-AD04-714D1833AF0B}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2961,12 +2948,11 @@
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -2983,7 +2969,7 @@
         <v>283</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>286</v>
@@ -2991,23 +2977,20 @@
       <c r="H1" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="I1" s="20" t="s">
-        <v>310</v>
-      </c>
+      <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
       <c r="L1" s="20"/>
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="O1" s="40"/>
       <c r="P1" s="40"/>
       <c r="Q1" s="40"/>
       <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
     </row>
-    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -3030,10 +3013,7 @@
       <c r="H2" s="42">
         <v>3</v>
       </c>
-      <c r="I2">
-        <v>500</v>
-      </c>
-      <c r="S2" s="41"/>
+      <c r="R2" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3079,7 +3059,7 @@
         <v>283</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>286</v>
@@ -3099,7 +3079,7 @@
     </row>
     <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -3127,10 +3107,94 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C47C40-1604-468B-979E-291CAC04260A}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="44">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="R2" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AECF4C-F4E6-4F57-8D51-CCB135FF85E6}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -3161,13 +3225,13 @@
         <v>86</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F1" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>317</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>318</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
@@ -3183,7 +3247,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
First commit on Vehicle security loan cash flow - Two wheeler loan (23037).
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53F66A-D0A8-4875-8338-2884231487E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4996A5-1C5B-4FF8-8F51-8ADD89F8D169}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="273">
   <si>
     <t>Run</t>
   </si>
@@ -746,9 +746,6 @@
     <t>EquitableMortRegNo</t>
   </si>
   <si>
-    <t>Ad353</t>
-  </si>
-  <si>
     <t>EMRDate</t>
   </si>
   <si>
@@ -761,13 +758,103 @@
     <t>DSACode</t>
   </si>
   <si>
-    <t>VehicleNo</t>
-  </si>
-  <si>
-    <t>TN 01 AB 1234</t>
-  </si>
-  <si>
-    <t>RC.No</t>
+    <t>VehicleDetails</t>
+  </si>
+  <si>
+    <t>BMW Z models</t>
+  </si>
+  <si>
+    <t>EXshowroomprice</t>
+  </si>
+  <si>
+    <t>RoadTax</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Regotherchargers</t>
+  </si>
+  <si>
+    <t>DealerDiscount</t>
+  </si>
+  <si>
+    <t>DownPayment</t>
+  </si>
+  <si>
+    <t>InsuranceDocNo</t>
+  </si>
+  <si>
+    <t>Yearofmanufacture</t>
+  </si>
+  <si>
+    <t>IDV</t>
+  </si>
+  <si>
+    <t>VehicleColor</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>RegDate</t>
+  </si>
+  <si>
+    <t>PermitNo</t>
+  </si>
+  <si>
+    <t>EngineNo</t>
+  </si>
+  <si>
+    <t>ChassisNo</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>ZXI</t>
+  </si>
+  <si>
+    <t>RTODetails</t>
+  </si>
+  <si>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>25/10/2300</t>
+  </si>
+  <si>
+    <t>InsuredFutureDate</t>
+  </si>
+  <si>
+    <t>InsuredPastDate</t>
+  </si>
+  <si>
+    <t>customerName1</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>SanctionedAmount</t>
+  </si>
+  <si>
+    <t>NoOfInstallement</t>
+  </si>
+  <si>
+    <t>Ad343</t>
+  </si>
+  <si>
+    <t>PAS789456321</t>
+  </si>
+  <si>
+    <t>KA0H378910039</t>
+  </si>
+  <si>
+    <t>J3V1063002345</t>
+  </si>
+  <si>
+    <t>AWZUXX8P7EA123456</t>
   </si>
 </sst>
 </file>
@@ -870,7 +957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1004,6 +1091,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1525,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H2"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1966,10 +2056,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1982,11 +2072,31 @@
     <col min="9" max="9" width="19.26953125" customWidth="1"/>
     <col min="10" max="10" width="14.453125" customWidth="1"/>
     <col min="11" max="11" width="12.453125" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" customWidth="1"/>
+    <col min="14" max="14" width="18.08984375" customWidth="1"/>
+    <col min="15" max="15" width="13.36328125" customWidth="1"/>
+    <col min="16" max="16" width="10.08984375" customWidth="1"/>
+    <col min="17" max="17" width="17.1796875" customWidth="1"/>
+    <col min="18" max="18" width="14.90625" customWidth="1"/>
+    <col min="19" max="19" width="13.1796875" customWidth="1"/>
+    <col min="20" max="20" width="15.6328125" customWidth="1"/>
+    <col min="21" max="21" width="17.1796875" customWidth="1"/>
+    <col min="23" max="23" width="16.54296875" customWidth="1"/>
+    <col min="24" max="24" width="14.81640625" customWidth="1"/>
+    <col min="25" max="25" width="11.453125" customWidth="1"/>
+    <col min="26" max="26" width="18.1796875" customWidth="1"/>
+    <col min="27" max="27" width="16" customWidth="1"/>
+    <col min="28" max="28" width="19.6328125" customWidth="1"/>
+    <col min="29" max="29" width="14" customWidth="1"/>
+    <col min="30" max="30" width="11.7265625" customWidth="1"/>
+    <col min="31" max="31" width="18.7265625" customWidth="1"/>
+    <col min="32" max="32" width="17.453125" customWidth="1"/>
+    <col min="33" max="33" width="19.7265625" customWidth="1"/>
+    <col min="34" max="34" width="17.36328125" customWidth="1"/>
+    <col min="35" max="35" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -2015,22 +2125,85 @@
         <v>235</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K1" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="L1" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="M1" s="27" t="s">
-        <v>241</v>
-      </c>
       <c r="N1" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="O1" s="27" t="s">
         <v>243</v>
       </c>
+      <c r="P1" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="S1" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="T1" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="W1" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="X1" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y1" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z1" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="AA1" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB1" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="AC1" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="AD1" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="AE1" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="AF1" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="AG1" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="AH1" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="AI1" s="52" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>229</v>
       </c>
@@ -2050,16 +2223,16 @@
         <v>232</v>
       </c>
       <c r="G2" s="41">
-        <v>1234</v>
+        <v>1342</v>
       </c>
       <c r="H2" s="45" t="s">
         <v>234</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="J2" s="45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K2" s="41">
         <v>7</v>
@@ -2068,10 +2241,73 @@
         <v>1</v>
       </c>
       <c r="M2" s="41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N2" s="41">
-        <v>1234567890</v>
+        <v>9500</v>
+      </c>
+      <c r="O2" s="41">
+        <v>700</v>
+      </c>
+      <c r="P2" s="41">
+        <v>600</v>
+      </c>
+      <c r="Q2" s="41">
+        <v>100</v>
+      </c>
+      <c r="R2" s="41">
+        <v>1200</v>
+      </c>
+      <c r="S2" s="55">
+        <v>500</v>
+      </c>
+      <c r="T2" s="55" t="s">
+        <v>269</v>
+      </c>
+      <c r="U2" s="55">
+        <v>2025</v>
+      </c>
+      <c r="V2" s="55">
+        <v>1800</v>
+      </c>
+      <c r="W2" s="45">
+        <v>47556</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y2" s="45">
+        <v>45740</v>
+      </c>
+      <c r="Z2" s="55" t="s">
+        <v>270</v>
+      </c>
+      <c r="AA2" s="55" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB2" s="55" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC2" s="55" t="s">
+        <v>258</v>
+      </c>
+      <c r="AD2" s="55" t="s">
+        <v>260</v>
+      </c>
+      <c r="AE2" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="AF2" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="AG2">
+        <v>8519</v>
+      </c>
+      <c r="AH2">
+        <v>36</v>
+      </c>
+      <c r="AI2">
+        <v>677536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module - MemberManagement Loan/Deposit Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA0E1D-D3B7-4353-969B-CB7E29D58E09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E911973-C4C9-4A9E-8B31-E18A4B2C1F33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="16" activeTab="19" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="319">
   <si>
     <t>Run</t>
   </si>
@@ -994,16 +994,13 @@
     <t>name</t>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>MemberManagement_Deposit</t>
   </si>
   <si>
     <t>MemberManagement_Loan</t>
   </si>
   <si>
-    <t>n</t>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -3053,7 +3050,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3080,7 +3077,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -3092,7 +3089,7 @@
         <v>87</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>301</v>
@@ -3190,7 +3187,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,7 +3214,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -3229,7 +3226,7 @@
         <v>87</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>301</v>

</xml_diff>

<commit_message>
Vehicle security loan - Two Wheeler loan (23027) cash flow completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4996A5-1C5B-4FF8-8F51-8ADD89F8D169}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FF130C-5C97-4B30-9684-72A384ABF7BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="273">
   <si>
     <t>Run</t>
   </si>
@@ -833,9 +833,6 @@
     <t>customerName1</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>SanctionedAmount</t>
   </si>
   <si>
@@ -855,6 +852,9 @@
   </si>
   <si>
     <t>AWZUXX8P7EA123456</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
@@ -2056,10 +2056,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2093,10 +2093,9 @@
     <col min="32" max="32" width="17.453125" customWidth="1"/>
     <col min="33" max="33" width="19.7265625" customWidth="1"/>
     <col min="34" max="34" width="17.36328125" customWidth="1"/>
-    <col min="35" max="35" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -2194,16 +2193,13 @@
         <v>264</v>
       </c>
       <c r="AG1" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="AH1" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="AH1" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="AI1" s="52" t="s">
-        <v>228</v>
-      </c>
     </row>
-    <row r="2" spans="1:35" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>229</v>
       </c>
@@ -2229,7 +2225,7 @@
         <v>234</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J2" s="45" t="s">
         <v>237</v>
@@ -2262,7 +2258,7 @@
         <v>500</v>
       </c>
       <c r="T2" s="55" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U2" s="55">
         <v>2025</v>
@@ -2280,13 +2276,13 @@
         <v>45740</v>
       </c>
       <c r="Z2" s="55" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA2" s="55" t="s">
         <v>270</v>
       </c>
-      <c r="AA2" s="55" t="s">
+      <c r="AB2" s="55" t="s">
         <v>271</v>
-      </c>
-      <c r="AB2" s="55" t="s">
-        <v>272</v>
       </c>
       <c r="AC2" s="55" t="s">
         <v>258</v>
@@ -2298,16 +2294,13 @@
         <v>261</v>
       </c>
       <c r="AF2" s="53" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="AG2">
         <v>8519</v>
       </c>
       <c r="AH2">
         <v>36</v>
-      </c>
-      <c r="AI2">
-        <v>677536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module - Nominee Management Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E911973-C4C9-4A9E-8B31-E18A4B2C1F33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DA8D45-ACBB-4B2D-BD2E-C960F8750331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="16" activeTab="19" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="17" activeTab="20" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="LoanChargePosting" sheetId="21" r:id="rId18"/>
     <sheet name="MembMang_Loan" sheetId="22" r:id="rId19"/>
     <sheet name="MembMang_Deposit" sheetId="23" r:id="rId20"/>
+    <sheet name="NomineeMang" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="321">
   <si>
     <t>Run</t>
   </si>
@@ -1001,6 +1002,12 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Nominee Management</t>
+  </si>
+  <si>
+    <t>q</t>
   </si>
 </sst>
 </file>
@@ -3050,7 +3057,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3186,8 +3193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A867EB9B-F04E-43CD-8EA1-F0F23332E62D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3230,6 +3237,55 @@
       </c>
       <c r="F2" s="21" t="s">
         <v>301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC09DCA-5CB4-4866-8FBA-9095C34DB2E7}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module - Collection Importing Cash & Transfer. Status - Completed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DA8D45-ACBB-4B2D-BD2E-C960F8750331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C06C18-2609-4402-A524-F680A6082E94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="17" activeTab="20" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="18" activeTab="21" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="MembMang_Loan" sheetId="22" r:id="rId19"/>
     <sheet name="MembMang_Deposit" sheetId="23" r:id="rId20"/>
     <sheet name="NomineeMang" sheetId="24" r:id="rId21"/>
+    <sheet name="CollectionImporting" sheetId="25" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="322">
   <si>
     <t>Run</t>
   </si>
@@ -1008,6 +1009,9 @@
   </si>
   <si>
     <t>q</t>
+  </si>
+  <si>
+    <t>last4DigitsOfAccNum</t>
   </si>
 </sst>
 </file>
@@ -3248,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC09DCA-5CB4-4866-8FBA-9095C34DB2E7}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,6 +3294,70 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33675B9-729F-4100-8198-C9B5CD9CC64B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2">
+        <v>220</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" s="21">
+        <v>3203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Vehicle Security loan -Two Wheeler loan (23027) transfer flow completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FF130C-5C97-4B30-9684-72A384ABF7BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99528E31-FB31-40AB-A35D-7C6CEECD2245}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -854,7 +854,7 @@
     <t>AWZUXX8P7EA123456</t>
   </si>
   <si>
-    <t>J</t>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -1615,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2093,6 +2093,7 @@
     <col min="32" max="32" width="17.453125" customWidth="1"/>
     <col min="33" max="33" width="19.7265625" customWidth="1"/>
     <col min="34" max="34" width="17.36328125" customWidth="1"/>
+    <col min="35" max="35" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
GL transaction transfer updated code
GL transaction transfer updated code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D11018-EA59-43AB-BA97-BB5A0DA69DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC952D-5297-4F13-905B-1577292E7C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="13" activeTab="13" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="16" activeTab="19" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -30,8 +30,9 @@
     <sheet name="Jewel_Gold_Loan_Renewal_Cash" sheetId="16" r:id="rId15"/>
     <sheet name="Jewel_Loan_Transcharge_Transfer" sheetId="20" r:id="rId16"/>
     <sheet name="Jewel_Loan_Transcharge_Cash" sheetId="19" r:id="rId17"/>
-    <sheet name="GL_Acc_Trans_Transfer" sheetId="22" r:id="rId18"/>
-    <sheet name="GL_Acc_Trans_Cash" sheetId="21" r:id="rId19"/>
+    <sheet name="GL_Acc_Trans_Cash" sheetId="21" r:id="rId18"/>
+    <sheet name="GL_Acc_Trans_Transfer" sheetId="22" r:id="rId19"/>
+    <sheet name="Share_Transfer" sheetId="23" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="322">
   <si>
     <t>Run</t>
   </si>
@@ -1000,6 +1001,15 @@
   </si>
   <si>
     <t>GL_Acc_Transaction_Transfer</t>
+  </si>
+  <si>
+    <t>Share_Transfer</t>
+  </si>
+  <si>
+    <t>Account_No</t>
+  </si>
+  <si>
+    <t>Account_No1</t>
   </si>
 </sst>
 </file>
@@ -2715,7 +2725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B90D486-903F-4F95-9CDA-9638AB00129B}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -3107,6 +3117,90 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AECF4C-F4E6-4F57-8D51-CCB135FF85E6}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="44">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="R2" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C47C40-1604-468B-979E-291CAC04260A}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -3164,90 +3258,6 @@
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>318</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="44">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="R2" s="41"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AECF4C-F4E6-4F57-8D51-CCB135FF85E6}">
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>316</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>317</v>
-      </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>315</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>2</v>
@@ -3350,6 +3360,83 @@
       <c r="I2" s="11" t="s">
         <v>67</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBDBD46-ED90-4296-8FC0-9A3B68B64832}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="16">
+        <v>86</v>
+      </c>
+      <c r="F2" s="16">
+        <v>87</v>
+      </c>
+      <c r="Q2" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Module - LoanCollectionTransfer Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C06C18-2609-4402-A524-F680A6082E94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81D54BB-134C-4E04-9CFB-3E3591DF0991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="18" activeTab="21" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="19" activeTab="22" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="MembMang_Deposit" sheetId="23" r:id="rId20"/>
     <sheet name="NomineeMang" sheetId="24" r:id="rId21"/>
     <sheet name="CollectionImporting" sheetId="25" r:id="rId22"/>
+    <sheet name="LoanCollectionTransfer" sheetId="26" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="323">
   <si>
     <t>Run</t>
   </si>
@@ -1012,6 +1013,9 @@
   </si>
   <si>
     <t>last4DigitsOfAccNum</t>
+  </si>
+  <si>
+    <t>Loan_Collection_Transfer</t>
   </si>
 </sst>
 </file>
@@ -2927,7 +2931,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,8 +3305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33675B9-729F-4100-8198-C9B5CD9CC64B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3353,6 +3357,66 @@
       </c>
       <c r="G2" s="21">
         <v>3203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A503D7F2-EA7A-492B-A3E2-1E7F00085F78}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="45">
+        <v>146414</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Admin Module - Debenture_Type_setting first push
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99528E31-FB31-40AB-A35D-7C6CEECD2245}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F5D70C-F8FE-4DE2-ABB0-948F4E4C1657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,7 @@
     <sheet name="AccountOpening_FixedDeposit" sheetId="13" r:id="rId10"/>
     <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId11"/>
     <sheet name="AccountOpening_Loan_ACOPL_TwoWh" sheetId="14" r:id="rId12"/>
+    <sheet name="Debenture_Type_setting" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="279">
   <si>
     <t>Run</t>
   </si>
@@ -734,9 +735,6 @@
     <t>ResolutionNo</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>ResoultionDate</t>
   </si>
   <si>
@@ -821,9 +819,6 @@
     <t>DL</t>
   </si>
   <si>
-    <t>25/10/2300</t>
-  </si>
-  <si>
     <t>InsuredFutureDate</t>
   </si>
   <si>
@@ -854,7 +849,31 @@
     <t>AWZUXX8P7EA123456</t>
   </si>
   <si>
-    <t>K</t>
+    <t>Debenture_Type_setting</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>validAmount</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>NewDebe</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>25/12/2300</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -2058,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2119,85 +2138,85 @@
         <v>231</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I1" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="27" t="s">
         <v>235</v>
       </c>
-      <c r="J1" s="27" t="s">
-        <v>236</v>
-      </c>
       <c r="K1" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="L1" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="M1" s="27" t="s">
-        <v>240</v>
-      </c>
       <c r="N1" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="O1" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="P1" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="Q1" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="R1" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="S1" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W1" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="X1" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z1" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA1" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB1" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="AC1" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="AD1" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="AE1" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="AF1" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="AG1" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="X1" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="Y1" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="Z1" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="AA1" s="27" t="s">
-        <v>255</v>
-      </c>
-      <c r="AB1" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="AC1" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="AD1" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="AE1" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="AF1" s="52" t="s">
+      <c r="AH1" s="27" t="s">
         <v>264</v>
-      </c>
-      <c r="AG1" s="27" t="s">
-        <v>265</v>
-      </c>
-      <c r="AH1" s="27" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
@@ -2214,22 +2233,22 @@
         <v>87</v>
       </c>
       <c r="E2" s="53">
-        <v>103000012417</v>
+        <v>102000000001</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>232</v>
+        <v>276</v>
       </c>
       <c r="G2" s="41">
         <v>1342</v>
       </c>
       <c r="H2" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J2" s="45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K2" s="41">
         <v>7</v>
@@ -2238,7 +2257,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N2" s="41">
         <v>9500</v>
@@ -2259,7 +2278,7 @@
         <v>500</v>
       </c>
       <c r="T2" s="55" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="U2" s="55">
         <v>2025</v>
@@ -2271,31 +2290,31 @@
         <v>47556</v>
       </c>
       <c r="X2" s="55" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Y2" s="45">
         <v>45740</v>
       </c>
       <c r="Z2" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA2" s="55" t="s">
+        <v>268</v>
+      </c>
+      <c r="AB2" s="55" t="s">
         <v>269</v>
       </c>
-      <c r="AA2" s="55" t="s">
-        <v>270</v>
-      </c>
-      <c r="AB2" s="55" t="s">
-        <v>271</v>
-      </c>
       <c r="AC2" s="55" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AD2" s="55" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AE2" s="45" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="AF2" s="53" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="AG2">
         <v>8519</v>
@@ -2303,6 +2322,160 @@
       <c r="AH2">
         <v>36</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8504464F-0319-4257-80D2-AF88871DE21D}">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" customWidth="1"/>
+    <col min="14" max="14" width="18.08984375" customWidth="1"/>
+    <col min="15" max="15" width="13.36328125" customWidth="1"/>
+    <col min="16" max="16" width="10.08984375" customWidth="1"/>
+    <col min="17" max="17" width="17.1796875" customWidth="1"/>
+    <col min="18" max="18" width="14.90625" customWidth="1"/>
+    <col min="19" max="19" width="13.1796875" customWidth="1"/>
+    <col min="20" max="20" width="15.6328125" customWidth="1"/>
+    <col min="21" max="21" width="17.1796875" customWidth="1"/>
+    <col min="23" max="23" width="16.54296875" customWidth="1"/>
+    <col min="24" max="24" width="14.81640625" customWidth="1"/>
+    <col min="25" max="25" width="11.453125" customWidth="1"/>
+    <col min="26" max="26" width="18.1796875" customWidth="1"/>
+    <col min="27" max="27" width="16" customWidth="1"/>
+    <col min="28" max="28" width="19.6328125" customWidth="1"/>
+    <col min="29" max="29" width="14" customWidth="1"/>
+    <col min="30" max="30" width="11.7265625" customWidth="1"/>
+    <col min="31" max="31" width="18.7265625" customWidth="1"/>
+    <col min="32" max="32" width="17.453125" customWidth="1"/>
+    <col min="33" max="33" width="19.7265625" customWidth="1"/>
+    <col min="34" max="34" width="17.36328125" customWidth="1"/>
+    <col min="35" max="35" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+    </row>
+    <row r="2" spans="1:34" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" s="41">
+        <v>1500</v>
+      </c>
+      <c r="G2" s="41">
+        <v>12</v>
+      </c>
+      <c r="H2" s="41">
+        <v>10</v>
+      </c>
+      <c r="I2" s="41">
+        <v>100</v>
+      </c>
+      <c r="J2" s="45"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TestData refreshed and pushed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81D54BB-134C-4E04-9CFB-3E3591DF0991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EA5449-485C-41B2-88F5-E6D968C43499}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="19" activeTab="22" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="20" activeTab="22" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="NomineeMang" sheetId="24" r:id="rId21"/>
     <sheet name="CollectionImporting" sheetId="25" r:id="rId22"/>
     <sheet name="LoanCollectionTransfer" sheetId="26" r:id="rId23"/>
+    <sheet name="BondConfiguration" sheetId="27" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="324">
   <si>
     <t>Run</t>
   </si>
@@ -1016,6 +1017,9 @@
   </si>
   <si>
     <t>Loan_Collection_Transfer</t>
+  </si>
+  <si>
+    <t>Bond_Configuration</t>
   </si>
 </sst>
 </file>
@@ -3370,7 +3374,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3422,6 +3426,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3469311B-4334-4F2F-ACF4-C3EB95B03B41}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="45"/>
+      <c r="F2" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Admin - Debenture_Issue_setting sub moudle first push.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F5D70C-F8FE-4DE2-ABB0-948F4E4C1657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036043D5-0DC9-46DA-B5D6-D3C1E8D5C3DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Customer_QuickCustomer" sheetId="12" r:id="rId11"/>
     <sheet name="AccountOpening_Loan_ACOPL_TwoWh" sheetId="14" r:id="rId12"/>
     <sheet name="Debenture_Type_setting" sheetId="15" r:id="rId13"/>
+    <sheet name="Debenture_Issue_setting" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="288">
   <si>
     <t>Run</t>
   </si>
@@ -874,6 +875,33 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>IssueFromDate</t>
+  </si>
+  <si>
+    <t>UnitValue</t>
+  </si>
+  <si>
+    <t>ReturnROI</t>
+  </si>
+  <si>
+    <t>CallDate</t>
+  </si>
+  <si>
+    <t>PutDate</t>
+  </si>
+  <si>
+    <t>15/03/2301</t>
+  </si>
+  <si>
+    <t>20/04/2301</t>
+  </si>
+  <si>
+    <t>CallDatePrematureROI</t>
+  </si>
+  <si>
+    <t>PutDatePrematureROI</t>
   </si>
 </sst>
 </file>
@@ -976,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1113,6 +1141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2077,8 +2106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2334,7 +2363,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2480,6 +2509,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DDB8B09-0FF3-461C-ACD2-A2FE66DBC353}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" customWidth="1"/>
+    <col min="10" max="10" width="20.90625" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>280</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>286</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2">
+        <v>250</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>284</v>
+      </c>
+      <c r="I2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Module - Bond Configuration Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EA5449-485C-41B2-88F5-E6D968C43499}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFCE253-C78C-414E-A708-7A238067581C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="20" activeTab="22" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="20" activeTab="23" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="328">
   <si>
     <t>Run</t>
   </si>
@@ -1020,6 +1020,18 @@
   </si>
   <si>
     <t>Bond_Configuration</t>
+  </si>
+  <si>
+    <t>faceValue</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>minAmt</t>
+  </si>
+  <si>
+    <t>maxAmt</t>
   </si>
 </sst>
 </file>
@@ -3373,7 +3385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A503D7F2-EA7A-492B-A3E2-1E7F00085F78}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3431,15 +3443,18 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3469311B-4334-4F2F-ACF4-C3EB95B03B41}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="47"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -3452,10 +3467,23 @@
       <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E1" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>323</v>
       </c>
@@ -3468,8 +3496,21 @@
       <c r="D2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="21"/>
+      <c r="E2" s="47">
+        <v>100</v>
+      </c>
+      <c r="F2" s="47">
+        <v>12</v>
+      </c>
+      <c r="G2" s="47">
+        <v>30</v>
+      </c>
+      <c r="H2" s="47">
+        <v>500</v>
+      </c>
+      <c r="I2" s="47">
+        <v>10000000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Updated the xpath issue for Loan collection transfer Module.
2. Module - Centre Group Registration, Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFCE253-C78C-414E-A708-7A238067581C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBACE01-E7BE-4D84-8BF0-E5FB35698F74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="20" activeTab="23" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="21" activeTab="24" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="CollectionImporting" sheetId="25" r:id="rId22"/>
     <sheet name="LoanCollectionTransfer" sheetId="26" r:id="rId23"/>
     <sheet name="BondConfiguration" sheetId="27" r:id="rId24"/>
+    <sheet name="CentreGroupRegistration" sheetId="28" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="332">
   <si>
     <t>Run</t>
   </si>
@@ -1032,6 +1033,18 @@
   </si>
   <si>
     <t>maxAmt</t>
+  </si>
+  <si>
+    <t>Centre Group Registration</t>
+  </si>
+  <si>
+    <t>groupName</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>custName2</t>
   </si>
 </sst>
 </file>
@@ -3445,8 +3458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3469311B-4334-4F2F-ACF4-C3EB95B03B41}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3514,6 +3527,68 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BAAA4A-EC12-405A-B8D9-B8C13E9F311D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
VehicleLoan opening (Cash/transfer) Branch updated, Customer changed and Relative xpath updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036043D5-0DC9-46DA-B5D6-D3C1E8D5C3DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820A165E-0911-4478-9C73-8C928425F7AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="AccountOpening_Loan_ACOPL_TwoWh" sheetId="14" r:id="rId12"/>
     <sheet name="Debenture_Type_setting" sheetId="15" r:id="rId13"/>
     <sheet name="Debenture_Issue_setting" sheetId="16" r:id="rId14"/>
+    <sheet name="Debenture_Application" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="291">
   <si>
     <t>Run</t>
   </si>
@@ -902,6 +903,15 @@
   </si>
   <si>
     <t>PutDatePrematureROI</t>
+  </si>
+  <si>
+    <t>CustID</t>
+  </si>
+  <si>
+    <t>NoofUnit</t>
+  </si>
+  <si>
+    <t>DematAccNo</t>
   </si>
 </sst>
 </file>
@@ -2363,7 +2373,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2516,8 +2526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DDB8B09-0FF3-461C-ACD2-A2FE66DBC353}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2603,6 +2613,79 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF40BF29-AC38-4DC2-B6B8-93DE885164A8}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="19.08984375" customWidth="1"/>
+    <col min="6" max="7" width="13.90625" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>288</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>289</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="53">
+        <v>102000000001</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="G2" s="41">
+        <v>20</v>
+      </c>
+      <c r="H2" s="41">
+        <v>1342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Module - Group Loan Application. Status - Completed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBACE01-E7BE-4D84-8BF0-E5FB35698F74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E77050-AE24-4489-AA39-7E4B275119DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="21" activeTab="24" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="23" activeTab="25" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="LoanCollectionTransfer" sheetId="26" r:id="rId23"/>
     <sheet name="BondConfiguration" sheetId="27" r:id="rId24"/>
     <sheet name="CentreGroupRegistration" sheetId="28" r:id="rId25"/>
+    <sheet name="GroupLoanApplication" sheetId="29" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="334">
   <si>
     <t>Run</t>
   </si>
@@ -1045,6 +1046,12 @@
   </si>
   <si>
     <t>custName2</t>
+  </si>
+  <si>
+    <t>Group Loan Application</t>
+  </si>
+  <si>
+    <t>loan</t>
   </si>
 </sst>
 </file>
@@ -3534,8 +3541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BAAA4A-EC12-405A-B8D9-B8C13E9F311D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3589,6 +3596,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8417BA-CA60-4B56-9698-8581C819DF0A}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2">
+        <v>25000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Module - Group Loan Agreement & Group Loan Sanction. Status - Completed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E77050-AE24-4489-AA39-7E4B275119DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB643EC5-A45A-4EDE-9BD9-04C57FCAB06F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="23" activeTab="25" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="24" activeTab="27" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -39,6 +39,8 @@
     <sheet name="BondConfiguration" sheetId="27" r:id="rId24"/>
     <sheet name="CentreGroupRegistration" sheetId="28" r:id="rId25"/>
     <sheet name="GroupLoanApplication" sheetId="29" r:id="rId26"/>
+    <sheet name="GroupLoanAgreement" sheetId="30" r:id="rId27"/>
+    <sheet name="GroupLoanSanction" sheetId="31" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="336">
   <si>
     <t>Run</t>
   </si>
@@ -1052,6 +1054,12 @@
   </si>
   <si>
     <t>loan</t>
+  </si>
+  <si>
+    <t>Group Loan Agreement</t>
+  </si>
+  <si>
+    <t>Group Loan Sanction</t>
   </si>
 </sst>
 </file>
@@ -3603,8 +3611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8417BA-CA60-4B56-9698-8581C819DF0A}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3641,6 +3649,92 @@
       </c>
       <c r="E2">
         <v>25000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A02D50-C7D3-4375-AB7B-D5A1D6C62374}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8FD6BD-ACB3-4CAF-B414-DD19B6B63789}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module - Investment_Opening Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Transactions_Jewel" sheetId="19" r:id="rId16"/>
     <sheet name="InvestmentOpn" sheetId="20" r:id="rId17"/>
     <sheet name="Centre_Registration" sheetId="21" r:id="rId18"/>
+    <sheet name="Debenture_series_setting" sheetId="22" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="327">
   <si>
     <t>Run</t>
   </si>
@@ -976,34 +977,64 @@
     <t>Transactions_Jewel</t>
   </si>
   <si>
-    <t>19digitNum</t>
-  </si>
-  <si>
-    <t>20digitNum</t>
-  </si>
-  <si>
-    <t>21digitNum</t>
-  </si>
-  <si>
     <t>Investment_Opening</t>
   </si>
   <si>
     <t>Centre_Registration</t>
+  </si>
+  <si>
+    <t>Debenture_series_setting</t>
+  </si>
+  <si>
+    <t>accAtBranch</t>
+  </si>
+  <si>
+    <t>openAmt</t>
+  </si>
+  <si>
+    <t>IntGLhead</t>
+  </si>
+  <si>
+    <t>RceiptNo</t>
+  </si>
+  <si>
+    <t>depstName</t>
+  </si>
+  <si>
+    <t>shradda</t>
+  </si>
+  <si>
+    <t>reMarks</t>
+  </si>
+  <si>
+    <t>No remarks</t>
+  </si>
+  <si>
+    <t>EnterrelatioN</t>
+  </si>
+  <si>
+    <t>Daughter</t>
+  </si>
+  <si>
+    <t>RemarksTOenter</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>SPiinfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="8">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000000"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="00000000000000"/>
-    <numFmt numFmtId="169" formatCode="0000000000000000000"/>
-    <numFmt numFmtId="170" formatCode="00000000000000000000"/>
-    <numFmt numFmtId="171" formatCode="000000000000000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1095,7 +1126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1227,9 +1258,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2905,20 +2934,21 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -2932,18 +2962,39 @@
         <v>86</v>
       </c>
       <c r="E1" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>311</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>314</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -2954,14 +3005,29 @@
       <c r="D2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="51">
-        <v>1.93456789012345E+19</v>
-      </c>
-      <c r="F2" s="52">
-        <v>2.0345678901231399E+19</v>
-      </c>
-      <c r="G2" s="53">
-        <v>2.13456789012314E+20</v>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="51">
+        <v>200</v>
+      </c>
+      <c r="G2">
+        <v>160</v>
+      </c>
+      <c r="H2">
+        <v>3232</v>
+      </c>
+      <c r="I2" t="s">
+        <v>319</v>
+      </c>
+      <c r="J2" t="s">
+        <v>321</v>
+      </c>
+      <c r="K2" t="s">
+        <v>323</v>
+      </c>
+      <c r="L2" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2974,8 +3040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,7 +3062,7 @@
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -3011,6 +3077,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Module- Group registration Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="338">
   <si>
     <t>Run</t>
   </si>
@@ -1023,6 +1023,39 @@
   </si>
   <si>
     <t>SPiinfo</t>
+  </si>
+  <si>
+    <t>StreetName</t>
+  </si>
+  <si>
+    <t>2nd cross ashok nagar</t>
+  </si>
+  <si>
+    <t>CentrName</t>
+  </si>
+  <si>
+    <t>KHUSHI</t>
+  </si>
+  <si>
+    <t>DisfromBranch</t>
+  </si>
+  <si>
+    <t>BlockFld</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>LandMark</t>
+  </si>
+  <si>
+    <t>Meeting_Time</t>
+  </si>
+  <si>
+    <t>next to goeri appartments</t>
+  </si>
+  <si>
+    <t>Meeting_Min</t>
   </si>
 </sst>
 </file>
@@ -3038,15 +3071,18 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -3059,8 +3095,31 @@
       <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
+      <c r="E1" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>312</v>
       </c>
@@ -3072,6 +3131,27 @@
       </c>
       <c r="D2" s="29" t="s">
         <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debenture Type/Issue and Vehicle loan opening error fixed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820A165E-0911-4478-9C73-8C928425F7AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E4A720-20FD-45E8-902C-220A69A34030}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="295">
   <si>
     <t>Run</t>
   </si>
@@ -912,6 +912,18 @@
   </si>
   <si>
     <t>DematAccNo</t>
+  </si>
+  <si>
+    <t>NomineeName</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Debenture_Issue_setting</t>
+  </si>
+  <si>
+    <t>Debenture_Application</t>
   </si>
 </sst>
 </file>
@@ -2116,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2373,7 +2385,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2527,7 +2539,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2578,7 +2590,7 @@
     </row>
     <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -2618,10 +2630,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF40BF29-AC38-4DC2-B6B8-93DE885164A8}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2629,9 +2641,10 @@
     <col min="5" max="5" width="19.08984375" customWidth="1"/>
     <col min="6" max="7" width="13.90625" customWidth="1"/>
     <col min="8" max="8" width="22.453125" customWidth="1"/>
+    <col min="9" max="9" width="18.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -2656,10 +2669,13 @@
       <c r="H1" s="52" t="s">
         <v>290</v>
       </c>
+      <c r="I1" s="52" t="s">
+        <v>291</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -2681,6 +2697,9 @@
       </c>
       <c r="H2" s="41">
         <v>1342</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module - Debenture series setting Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,8 @@
     <sheet name="Transactions_Jewel" sheetId="19" r:id="rId16"/>
     <sheet name="InvestmentOpn" sheetId="20" r:id="rId17"/>
     <sheet name="Centre_Registration" sheetId="21" r:id="rId18"/>
-    <sheet name="Debenture_series_setting" sheetId="22" r:id="rId19"/>
+    <sheet name="Debenture_Series_Setting" sheetId="22" r:id="rId19"/>
+    <sheet name="DebentureSeriesSetting" sheetId="23" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="347">
   <si>
     <t>Run</t>
   </si>
@@ -1056,18 +1057,48 @@
   </si>
   <si>
     <t>Meeting_Min</t>
+  </si>
+  <si>
+    <t>RoI</t>
+  </si>
+  <si>
+    <t>Acc_Code</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>Int_Acc_Code</t>
+  </si>
+  <si>
+    <t>TempROI</t>
+  </si>
+  <si>
+    <t>Print_GL_Acc_Code</t>
+  </si>
+  <si>
+    <t>ROI_Effect_From_Date_Selection</t>
+  </si>
+  <si>
+    <t>ROI_Effect_To_Date_Selection</t>
+  </si>
+  <si>
+    <t>Debenture Series Setting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000000"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="00000000000000"/>
+    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="dd\/mm\/yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1159,7 +1190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1292,6 +1323,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2506,7 +2540,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,7 +3107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -3162,15 +3196,22 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -3183,8 +3224,32 @@
       <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
+      <c r="E1" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>345</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>313</v>
       </c>
@@ -3197,9 +3262,37 @@
       <c r="D2" s="29" t="s">
         <v>87</v>
       </c>
+      <c r="E2">
+        <v>1234567890</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2" s="52">
+        <v>45756</v>
+      </c>
+      <c r="L2" s="52">
+        <v>46487</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U7" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3282,6 +3375,101 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="51">
+        <v>888888889</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2" s="54">
+        <v>45756</v>
+      </c>
+      <c r="L2" s="54">
+        <v>46487</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Multiple fd intrest payment (Rework)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinusha.shetty\Documents\GitHub\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8AD8A3-64A2-4B9A-A9BE-CB4427DF10DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E0AB2E-2C98-40B1-B6FE-8591F8A80F3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="14" activeTab="19" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="20" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="SuspenseAsset" sheetId="21" r:id="rId18"/>
     <sheet name="MultipleFD" sheetId="22" r:id="rId19"/>
     <sheet name="BondApp" sheetId="23" r:id="rId20"/>
+    <sheet name="Bondissue" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="323">
   <si>
     <t>Run</t>
   </si>
@@ -1001,6 +1002,18 @@
   </si>
   <si>
     <t>Vinusha</t>
+  </si>
+  <si>
+    <t>Bond_Issue</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Rejected</t>
   </si>
 </sst>
 </file>
@@ -3268,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9951296-08D0-4B89-AAA5-5A377C35A323}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3371,6 +3384,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87505F6A-FF99-46A2-A2AC-51D9ADDDE079}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="F2">
+        <v>500000</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="H2">
+        <v>500000</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" s="21">
+        <v>300</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="21">
+        <v>200</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>318</v>
+      </c>
+      <c r="P2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Module - Group Loan Payment_CASH Status - Completed
Module - Group Loan Payment_TRANSFER
Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB643EC5-A45A-4EDE-9BD9-04C57FCAB06F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06DE082-E48D-480A-A629-F6864882B11F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="24" activeTab="27" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="25" activeTab="28" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <sheet name="GroupLoanApplication" sheetId="29" r:id="rId26"/>
     <sheet name="GroupLoanAgreement" sheetId="30" r:id="rId27"/>
     <sheet name="GroupLoanSanction" sheetId="31" r:id="rId28"/>
+    <sheet name="GroupLoanCollection" sheetId="32" r:id="rId29"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="337">
   <si>
     <t>Run</t>
   </si>
@@ -1060,6 +1061,9 @@
   </si>
   <si>
     <t>Group Loan Sanction</t>
+  </si>
+  <si>
+    <t>Group Loan Collection</t>
   </si>
 </sst>
 </file>
@@ -3703,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8FD6BD-ACB3-4CAF-B414-DD19B6B63789}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3726,6 +3730,49 @@
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>335</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB8E3D9-FD65-43CE-ACEE-9C9681E76DFB}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>336</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Module - Investment Opening
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="17" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="Centre_Registration" sheetId="21" r:id="rId18"/>
     <sheet name="Debenture_Series_Setting" sheetId="22" r:id="rId19"/>
     <sheet name="DebentureSeriesSetting" sheetId="23" r:id="rId20"/>
+    <sheet name="Debenture_Transfer" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="348">
   <si>
     <t>Run</t>
   </si>
@@ -1084,6 +1085,9 @@
   </si>
   <si>
     <t>Debenture Series Setting</t>
+  </si>
+  <si>
+    <t>Debenture_Transfer</t>
   </si>
 </sst>
 </file>
@@ -3004,7 +3008,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3382,8 +3386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3470,6 +3474,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Multiple FD intrest payment Bond issue
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinusha.shetty\Documents\GitHub\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAB18AF-EEE0-42AC-921F-95532C3F4582}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD4B98F-E4DA-4FE6-B400-A56EF4BF88CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="15" activeTab="20" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="325">
   <si>
     <t>Run</t>
   </si>
@@ -1014,6 +1014,12 @@
   </si>
   <si>
     <t>Rejected</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>GLcode</t>
   </si>
 </sst>
 </file>
@@ -3389,15 +3395,15 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87505F6A-FF99-46A2-A2AC-51D9ADDDE079}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -3446,8 +3452,11 @@
       <c r="P1" s="26" t="s">
         <v>321</v>
       </c>
+      <c r="Q1" s="26" t="s">
+        <v>324</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>319</v>
       </c>
@@ -3470,13 +3479,13 @@
         <v>304</v>
       </c>
       <c r="H2">
-        <v>500000</v>
+        <v>500</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>304</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K2" s="21">
         <v>300</v>
@@ -3495,10 +3504,14 @@
       </c>
       <c r="P2" t="s">
         <v>322</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Debenture Application Cashflow Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D10DEF2-32EA-4528-B9EA-B00F4A87909F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B935F6-FA56-48E2-B020-B85F80AEB0A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2633,7 +2633,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2696,7 +2696,7 @@
         <v>20</v>
       </c>
       <c r="H2" s="41">
-        <v>32985342</v>
+        <v>923914143</v>
       </c>
       <c r="I2" s="41" t="s">
         <v>294</v>

</xml_diff>

<commit_message>
Module - Investment Opening Cash
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="17" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="16" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="DepoOpn_FxdDepo_BondCumulative" sheetId="17" r:id="rId14"/>
     <sheet name="GeneralOpening_SuspenseAsset" sheetId="18" r:id="rId15"/>
     <sheet name="Transactions_Jewel" sheetId="19" r:id="rId16"/>
-    <sheet name="InvestmentOpn" sheetId="20" r:id="rId17"/>
+    <sheet name="Investment_Opening_Cash" sheetId="20" r:id="rId17"/>
     <sheet name="Centre_Registration" sheetId="21" r:id="rId18"/>
     <sheet name="Debenture_Series_Setting" sheetId="22" r:id="rId19"/>
     <sheet name="DebentureSeriesSetting" sheetId="23" r:id="rId20"/>
@@ -979,9 +979,6 @@
     <t>Transactions_Jewel</t>
   </si>
   <si>
-    <t>Investment_Opening</t>
-  </si>
-  <si>
     <t>Centre_Registration</t>
   </si>
   <si>
@@ -1088,6 +1085,9 @@
   </si>
   <si>
     <t>Debenture_Transfer</t>
+  </si>
+  <si>
+    <t>Investment_Opening_Cash</t>
   </si>
 </sst>
 </file>
@@ -3007,8 +3007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3033,39 +3033,39 @@
         <v>86</v>
       </c>
       <c r="E1" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>318</v>
-      </c>
       <c r="J1" s="26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>311</v>
+        <v>347</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -3089,16 +3089,16 @@
         <v>3232</v>
       </c>
       <c r="I2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3134,32 +3134,32 @@
         <v>86</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G1" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>331</v>
       </c>
-      <c r="H1" s="26" t="s">
-        <v>332</v>
-      </c>
       <c r="I1" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>334</v>
       </c>
-      <c r="J1" s="26" t="s">
-        <v>335</v>
-      </c>
       <c r="K1" s="26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -3171,19 +3171,19 @@
         <v>87</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J2">
         <v>10</v>
@@ -3229,33 +3229,33 @@
         <v>86</v>
       </c>
       <c r="E1" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>338</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>339</v>
-      </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="J1" s="26" t="s">
-        <v>342</v>
-      </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>344</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -3409,33 +3409,33 @@
         <v>86</v>
       </c>
       <c r="E1" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>338</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>339</v>
-      </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="J1" s="26" t="s">
-        <v>342</v>
-      </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>344</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -3481,7 +3481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -3509,7 +3509,7 @@
     </row>
     <row r="2" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Module - Group Loan Collection_Cash | Status - Completed Module - Group Loan Collection_Transfer | Status - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06DE082-E48D-480A-A629-F6864882B11F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA51D88-EF83-4F8F-8874-4A03AC0AE349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="25" activeTab="28" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="340">
   <si>
     <t>Run</t>
   </si>
@@ -1064,6 +1064,15 @@
   </si>
   <si>
     <t>Group Loan Collection</t>
+  </si>
+  <si>
+    <t>numOfInt</t>
+  </si>
+  <si>
+    <t>particulars</t>
+  </si>
+  <si>
+    <t>amountToBePaid</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1301,6 +1310,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3748,15 +3760,19 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB8E3D9-FD65-43CE-ACEE-9C9681E76DFB}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -3769,8 +3785,17 @@
       <c r="D1" s="26" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>336</v>
       </c>
@@ -3783,9 +3808,19 @@
       <c r="D2" s="29" t="s">
         <v>87</v>
       </c>
+      <c r="E2" s="47">
+        <v>1</v>
+      </c>
+      <c r="F2" s="52">
+        <v>100</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>301</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
First Commit - Bond Transfer
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nbfc_automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E77050-AE24-4489-AA39-7E4B275119DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95ADDAF-B824-46FC-BE88-27BBD13A0167}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="23" activeTab="25" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -37,8 +37,9 @@
     <sheet name="CollectionImporting" sheetId="25" r:id="rId22"/>
     <sheet name="LoanCollectionTransfer" sheetId="26" r:id="rId23"/>
     <sheet name="BondConfiguration" sheetId="27" r:id="rId24"/>
-    <sheet name="CentreGroupRegistration" sheetId="28" r:id="rId25"/>
-    <sheet name="GroupLoanApplication" sheetId="29" r:id="rId26"/>
+    <sheet name="GroupLoanApplication" sheetId="29" r:id="rId25"/>
+    <sheet name="BondTransfer" sheetId="31" r:id="rId26"/>
+    <sheet name="CentreGroupRegistration" sheetId="28" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="340">
   <si>
     <t>Run</t>
   </si>
@@ -1052,19 +1053,38 @@
   </si>
   <si>
     <t>loan</t>
+  </si>
+  <si>
+    <t>Custname</t>
+  </si>
+  <si>
+    <t>Custid</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Test Remarks</t>
+  </si>
+  <si>
+    <t>Bond_Transfer</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000000"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="00000000000000"/>
     <numFmt numFmtId="169" formatCode="0000.00"/>
+    <numFmt numFmtId="170" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1156,7 +1176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1289,6 +1309,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1607,7 +1628,7 @@
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection sqref="A1:U2"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3538,11 +3559,137 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8417BA-CA60-4B56-9698-8581C819DF0A}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2">
+        <v>25000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34836A54-4025-4B7B-9EB2-6E1B80BBF54B}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="52">
+        <v>102140040000113</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="G2" s="52">
+        <v>102000001875</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BAAA4A-EC12-405A-B8D9-B8C13E9F311D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3596,55 +3743,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8417BA-CA60-4B56-9698-8581C819DF0A}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>332</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2">
-        <v>25000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4280,8 +4378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43876BD-E772-4993-8A82-594262F04F89}">
   <dimension ref="A1:AR3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
commited task -Debenture interest payment cash
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\O360-AI-master\O360-AI\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT HUB AUTOMATION\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E77050-AE24-4489-AA39-7E4B275119DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734D1641-136A-47D6-90DA-F0AC25C20F76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="23" activeTab="25" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="667" firstSheet="24" activeTab="27" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -39,6 +39,8 @@
     <sheet name="BondConfiguration" sheetId="27" r:id="rId24"/>
     <sheet name="CentreGroupRegistration" sheetId="28" r:id="rId25"/>
     <sheet name="GroupLoanApplication" sheetId="29" r:id="rId26"/>
+    <sheet name="DebentureAllotment" sheetId="31" r:id="rId27"/>
+    <sheet name="DebtIntpaymentcash" sheetId="32" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="337">
   <si>
     <t>Run</t>
   </si>
@@ -1052,19 +1054,29 @@
   </si>
   <si>
     <t>loan</t>
+  </si>
+  <si>
+    <t>accnumber</t>
+  </si>
+  <si>
+    <t>Debenture Interest payment -cash</t>
+  </si>
+  <si>
+    <t>Duration1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000000"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="00000000000000"/>
     <numFmt numFmtId="169" formatCode="0000.00"/>
+    <numFmt numFmtId="170" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1156,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1289,6 +1301,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1607,7 +1631,7 @@
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection sqref="A1:U2"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3603,8 +3627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8417BA-CA60-4B56-9698-8581C819DF0A}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3645,6 +3669,121 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6595211-A0FC-4BBF-AF76-45C787789E2A}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C5E120-9F01-4BB7-8F6A-FDE277225D42}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22" style="53" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="54">
+        <v>1029006800000010</v>
+      </c>
+      <c r="F2" s="55">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Vehicle Loan opening (cash/transfer) - Transaction date updated in application, so script modified and pushed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72CC825-1C80-44D1-BBD9-4C57C3A0E114}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2BA75C-D5EA-40FD-AA1B-1B6F919FFC2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="296">
   <si>
     <t>Run</t>
   </si>
@@ -2132,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2365,8 +2365,8 @@
       <c r="AD2" s="55" t="s">
         <v>259</v>
       </c>
-      <c r="AE2" s="45" t="s">
-        <v>277</v>
+      <c r="AE2" s="45">
+        <v>146748</v>
       </c>
       <c r="AF2" s="53" t="s">
         <v>278</v>
@@ -2716,7 +2716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D27FF5-15B0-41C1-82FD-AD28ABCCC965}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Debenture and Day End
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NBFC_CLS_2.0-master (1)\NBFC_CLS_2.0-master\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silpa.sivanandan\Desktop\NBFC_CLS_2.0-master\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B4B984-F452-48FE-9FB3-8D1DAEEB8827}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1439A0-F994-4E23-832D-46A5AA398098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" firstSheet="26" activeTab="27" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" firstSheet="27" activeTab="29" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -41,6 +41,8 @@
     <sheet name="GroupLoanApplication" sheetId="29" r:id="rId26"/>
     <sheet name="GLaccBulkTransImport" sheetId="30" r:id="rId27"/>
     <sheet name="GLaccBulkTransImportTransfer" sheetId="31" r:id="rId28"/>
+    <sheet name="Debenture_Interest_Adjustment" sheetId="32" r:id="rId29"/>
+    <sheet name="DayEnd" sheetId="33" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="337">
   <si>
     <t>Run</t>
   </si>
@@ -1057,6 +1059,12 @@
   </si>
   <si>
     <t>GLAccBulk Transaction Import Cash</t>
+  </si>
+  <si>
+    <t>Debenture Interest Adjustment</t>
+  </si>
+  <si>
+    <t>Day End</t>
   </si>
 </sst>
 </file>
@@ -3729,8 +3737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A669D8-3A0D-4786-9D35-2A545BAA5A50}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3784,6 +3792,75 @@
         <v>301</v>
       </c>
       <c r="G2" s="8">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567C2407-C250-4139-A7CA-9965F34C705D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" s="7">
         <v>10000</v>
       </c>
     </row>
@@ -3859,6 +3936,74 @@
       <c r="H2" s="18"/>
       <c r="I2" s="19" t="s">
         <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0853BF-34D8-43FF-895B-FED49E6FA9C6}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" s="7">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Account Opening - Fixed Deposit (Cash/transfer) Relative xpath and Customer, nominee and operators modified.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2BA75C-D5EA-40FD-AA1B-1B6F919FFC2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FFDBF3-5911-407E-BE3A-929BBDDD830E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -1689,14 +1689,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="5" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.26953125" customWidth="1"/>
@@ -1716,7 +1717,7 @@
       <c r="D1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="52" t="s">
         <v>208</v>
       </c>
       <c r="F1" s="48" t="s">
@@ -1781,8 +1782,8 @@
       <c r="D2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="49">
-        <v>102000015729</v>
+      <c r="E2" s="53">
+        <v>102000000001</v>
       </c>
       <c r="F2" s="50">
         <v>200000</v>
@@ -1809,10 +1810,10 @@
         <v>219</v>
       </c>
       <c r="N2" s="49">
-        <v>103000012745</v>
+        <v>102000000084</v>
       </c>
       <c r="O2" s="53">
-        <v>103000012519</v>
+        <v>102000000099</v>
       </c>
       <c r="P2" t="s">
         <v>177</v>
@@ -2132,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AccountOpening - Loan Opening - InsuredFutureDate updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Beacon Automation\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FFDBF3-5911-407E-BE3A-929BBDDD830E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDA2E9B-7C95-40E9-B455-AE26B723F186}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12040" windowHeight="5650" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeSheetModule" sheetId="3" r:id="rId1"/>
@@ -1689,7 +1689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2133,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FAD840-61C0-4B20-8B32-4FBE2554B309}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2367,7 +2367,7 @@
         <v>259</v>
       </c>
       <c r="AE2" s="45">
-        <v>146748</v>
+        <v>165010</v>
       </c>
       <c r="AF2" s="53" t="s">
         <v>278</v>

</xml_diff>

<commit_message>
Day end test data committed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sanoop\Sanoop_Automation\KSIDC\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB30A729-F78A-4EBF-899A-97F9B6B2C990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4895D939-5C77-45BE-9D1C-428F0172C988}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="70" activeTab="72" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="70" activeTab="73" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_CustSearch" sheetId="11" r:id="rId1"/>
@@ -86,7 +86,8 @@
     <sheet name="BondTransfer" sheetId="84" r:id="rId71"/>
     <sheet name="AccountOpening_FixedDeposit" sheetId="66" r:id="rId72"/>
     <sheet name="DebtIntpaymentcash" sheetId="85" r:id="rId73"/>
-    <sheet name="GroupLoanCollection" sheetId="32" r:id="rId74"/>
+    <sheet name="DayEnd" sheetId="86" r:id="rId74"/>
+    <sheet name="GroupLoanCollection" sheetId="32" r:id="rId75"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="639">
   <si>
     <t>Run</t>
   </si>
@@ -2012,6 +2013,9 @@
   </si>
   <si>
     <t>Debenture Interest payment -cash</t>
+  </si>
+  <si>
+    <t>Day End</t>
   </si>
 </sst>
 </file>
@@ -2146,7 +2150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2325,6 +2329,12 @@
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9828,7 +9838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CE793E-C149-4585-8B74-259348F84D86}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -9880,6 +9890,67 @@
 </file>
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D808A0-23B7-4F4F-A13E-318766F76185}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="71" t="s">
+        <v>638</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="72">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB8E3D9-FD65-43CE-ACEE-9C9681E76DFB}">
   <dimension ref="A1:G2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Vinusha's code correction committed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sanoop\Sanoop_Automation\KSIDC\NBFC_CLS_2.0\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99BC7E4-1997-4270-9F92-5E843CCE5C6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93ABEEAA-B4C3-4583-8F5A-727A9298C430}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="45" activeTab="46" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="45" activeTab="47" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_CustSearch" sheetId="11" r:id="rId1"/>
@@ -60,35 +60,36 @@
     <sheet name="GL_Acc_Trans_Transfer" sheetId="57" r:id="rId45"/>
     <sheet name="Customer_CustRating" sheetId="58" r:id="rId46"/>
     <sheet name="User_creation" sheetId="59" r:id="rId47"/>
-    <sheet name="InstitutionalCustomer" sheetId="60" r:id="rId48"/>
-    <sheet name="documensecurity-Cash" sheetId="61" r:id="rId49"/>
-    <sheet name="documensecurity-Transfer" sheetId="62" r:id="rId50"/>
-    <sheet name="Otherloanopeningjewelsecurity-C" sheetId="63" r:id="rId51"/>
-    <sheet name="Otherloanopeningjewelsecurity-T" sheetId="64" r:id="rId52"/>
-    <sheet name="AccountOpening_Loan_ACOPL_TwoWh" sheetId="65" r:id="rId53"/>
-    <sheet name="Debenture_Type_setting" sheetId="67" r:id="rId54"/>
-    <sheet name="Debenture_Issue_setting" sheetId="68" r:id="rId55"/>
-    <sheet name="Debenture_Application" sheetId="69" r:id="rId56"/>
-    <sheet name="Transaction" sheetId="70" r:id="rId57"/>
-    <sheet name="TransactionClosure" sheetId="71" r:id="rId58"/>
-    <sheet name="JewelClosure" sheetId="72" r:id="rId59"/>
-    <sheet name="BondApp" sheetId="73" r:id="rId60"/>
-    <sheet name="Bondissue" sheetId="74" r:id="rId61"/>
-    <sheet name="GeneralOpening" sheetId="75" r:id="rId62"/>
-    <sheet name="SuspenseAsset" sheetId="76" r:id="rId63"/>
-    <sheet name="MultipleFD" sheetId="77" r:id="rId64"/>
-    <sheet name="Investment_Opening_Cash" sheetId="78" r:id="rId65"/>
-    <sheet name="Investment_Opening_Transfer" sheetId="79" r:id="rId66"/>
-    <sheet name="Centre_Registration" sheetId="80" r:id="rId67"/>
-    <sheet name="GLaccBulkTransImport" sheetId="81" r:id="rId68"/>
-    <sheet name="GLaccBulkTransImportTransfer" sheetId="82" r:id="rId69"/>
-    <sheet name="DebentureRedemption" sheetId="83" r:id="rId70"/>
-    <sheet name="BondTransfer" sheetId="84" r:id="rId71"/>
-    <sheet name="AccountOpening_FixedDeposit" sheetId="66" r:id="rId72"/>
-    <sheet name="DebtIntpaymentcash" sheetId="85" r:id="rId73"/>
-    <sheet name="DayEnd" sheetId="86" r:id="rId74"/>
-    <sheet name="Account_Search" sheetId="87" r:id="rId75"/>
-    <sheet name="GroupLoanCollection" sheetId="32" r:id="rId76"/>
+    <sheet name="Debenture" sheetId="88" r:id="rId48"/>
+    <sheet name="InstitutionalCustomer" sheetId="60" r:id="rId49"/>
+    <sheet name="documensecurity-Cash" sheetId="61" r:id="rId50"/>
+    <sheet name="documensecurity-Transfer" sheetId="62" r:id="rId51"/>
+    <sheet name="Otherloanopeningjewelsecurity-C" sheetId="63" r:id="rId52"/>
+    <sheet name="Otherloanopeningjewelsecurity-T" sheetId="64" r:id="rId53"/>
+    <sheet name="AccountOpening_Loan_ACOPL_TwoWh" sheetId="65" r:id="rId54"/>
+    <sheet name="Debenture_Type_setting" sheetId="67" r:id="rId55"/>
+    <sheet name="Debenture_Issue_setting" sheetId="68" r:id="rId56"/>
+    <sheet name="Debenture_Application" sheetId="69" r:id="rId57"/>
+    <sheet name="Transaction" sheetId="70" r:id="rId58"/>
+    <sheet name="TransactionClosure" sheetId="71" r:id="rId59"/>
+    <sheet name="JewelClosure" sheetId="72" r:id="rId60"/>
+    <sheet name="BondApp" sheetId="73" r:id="rId61"/>
+    <sheet name="Bondissue" sheetId="74" r:id="rId62"/>
+    <sheet name="GeneralOpening" sheetId="75" r:id="rId63"/>
+    <sheet name="SuspenseAsset" sheetId="76" r:id="rId64"/>
+    <sheet name="MultipleFD" sheetId="77" r:id="rId65"/>
+    <sheet name="Investment_Opening_Cash" sheetId="78" r:id="rId66"/>
+    <sheet name="Investment_Opening_Transfer" sheetId="79" r:id="rId67"/>
+    <sheet name="Centre_Registration" sheetId="80" r:id="rId68"/>
+    <sheet name="GLaccBulkTransImport" sheetId="81" r:id="rId69"/>
+    <sheet name="GLaccBulkTransImportTransfer" sheetId="82" r:id="rId70"/>
+    <sheet name="DebentureRedemption" sheetId="83" r:id="rId71"/>
+    <sheet name="BondTransfer" sheetId="84" r:id="rId72"/>
+    <sheet name="AccountOpening_FixedDeposit" sheetId="66" r:id="rId73"/>
+    <sheet name="DebtIntpaymentcash" sheetId="85" r:id="rId74"/>
+    <sheet name="DayEnd" sheetId="86" r:id="rId75"/>
+    <sheet name="Account_Search" sheetId="87" r:id="rId76"/>
+    <sheet name="GroupLoanCollection" sheetId="32" r:id="rId77"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -100,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="646">
   <si>
     <t>Run</t>
   </si>
@@ -2035,6 +2036,9 @@
   </si>
   <si>
     <t>Naveenmo</t>
+  </si>
+  <si>
+    <t>Debenture_Interest_Payment_Transfer</t>
   </si>
 </sst>
 </file>
@@ -6377,8 +6381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB937661-368A-4872-8F37-D8864DFF8FC0}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6508,6 +6512,82 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DBFAA1-5B05-4CE7-9B11-1646F89A1E94}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>266</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>267</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>268</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="49">
+        <v>102000000001</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="G2" s="24">
+        <v>20</v>
+      </c>
+      <c r="H2" s="24">
+        <v>923914143</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D05FF53-BDCE-401B-B7DF-247AD98A117B}">
   <dimension ref="A1:CH2"/>
   <sheetViews>
@@ -7039,245 +7119,6 @@
     <hyperlink ref="I2" r:id="rId1" xr:uid="{DD7A611B-81B8-40B8-95BA-59493E1868E1}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{3D93502D-4D5B-41C5-A2C5-FD1023322A02}"/>
     <hyperlink ref="X2" r:id="rId3" xr:uid="{6F5927CB-5B16-42B0-A357-18490AC7A302}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8447F3E7-1537-4679-AB27-5D8C1807B167}">
-  <dimension ref="A1:AJ2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:36" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>319</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>320</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>476</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>322</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>477</v>
-      </c>
-      <c r="J1" s="51" t="s">
-        <v>478</v>
-      </c>
-      <c r="K1" s="51" t="s">
-        <v>199</v>
-      </c>
-      <c r="L1" s="51" t="s">
-        <v>479</v>
-      </c>
-      <c r="M1" s="51" t="s">
-        <v>480</v>
-      </c>
-      <c r="N1" s="51" t="s">
-        <v>481</v>
-      </c>
-      <c r="O1" s="51" t="s">
-        <v>482</v>
-      </c>
-      <c r="P1" s="51" t="s">
-        <v>483</v>
-      </c>
-      <c r="Q1" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="R1" s="51" t="s">
-        <v>202</v>
-      </c>
-      <c r="S1" s="51" t="s">
-        <v>203</v>
-      </c>
-      <c r="T1" s="51" t="s">
-        <v>204</v>
-      </c>
-      <c r="U1" s="51" t="s">
-        <v>484</v>
-      </c>
-      <c r="V1" s="51" t="s">
-        <v>422</v>
-      </c>
-      <c r="W1" s="51" t="s">
-        <v>423</v>
-      </c>
-      <c r="X1" s="51" t="s">
-        <v>485</v>
-      </c>
-      <c r="Y1" s="51" t="s">
-        <v>486</v>
-      </c>
-      <c r="Z1" s="51" t="s">
-        <v>405</v>
-      </c>
-      <c r="AA1" s="51" t="s">
-        <v>487</v>
-      </c>
-      <c r="AB1" s="51" t="s">
-        <v>488</v>
-      </c>
-      <c r="AC1" s="51" t="s">
-        <v>489</v>
-      </c>
-      <c r="AD1" s="51" t="s">
-        <v>490</v>
-      </c>
-      <c r="AE1" s="51" t="s">
-        <v>491</v>
-      </c>
-      <c r="AF1" s="51" t="s">
-        <v>492</v>
-      </c>
-      <c r="AG1" s="51" t="s">
-        <v>207</v>
-      </c>
-      <c r="AH1" s="51" t="s">
-        <v>493</v>
-      </c>
-      <c r="AI1" s="51" t="s">
-        <v>494</v>
-      </c>
-      <c r="AJ1" s="51" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="F2" s="48" t="s">
-        <v>329</v>
-      </c>
-      <c r="G2" s="49">
-        <v>123456789012</v>
-      </c>
-      <c r="H2" s="49">
-        <v>102000000084</v>
-      </c>
-      <c r="I2" s="49">
-        <v>103000012486</v>
-      </c>
-      <c r="J2">
-        <v>12</v>
-      </c>
-      <c r="K2" s="59">
-        <v>45575</v>
-      </c>
-      <c r="L2">
-        <v>12</v>
-      </c>
-      <c r="M2" s="59">
-        <v>45575</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>497</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>498</v>
-      </c>
-      <c r="R2">
-        <v>3</v>
-      </c>
-      <c r="S2">
-        <v>12</v>
-      </c>
-      <c r="T2">
-        <v>22</v>
-      </c>
-      <c r="U2">
-        <v>12000</v>
-      </c>
-      <c r="V2" t="s">
-        <v>472</v>
-      </c>
-      <c r="W2" s="42" t="s">
-        <v>473</v>
-      </c>
-      <c r="X2">
-        <v>2024</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>499</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>500</v>
-      </c>
-      <c r="AA2" s="59">
-        <v>45575</v>
-      </c>
-      <c r="AB2">
-        <v>2200000</v>
-      </c>
-      <c r="AC2">
-        <v>2300000</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>501</v>
-      </c>
-      <c r="AE2" s="59">
-        <v>35713</v>
-      </c>
-      <c r="AF2">
-        <v>690</v>
-      </c>
-      <c r="AG2">
-        <v>11100</v>
-      </c>
-      <c r="AH2">
-        <v>50</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>328</v>
-      </c>
-      <c r="AJ2">
-        <v>11046</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{48E96FF8-C647-4A3B-9CDF-D5A4C1C8BC57}"/>
-    <hyperlink ref="W2" r:id="rId2" xr:uid="{64BC90D3-0F6A-4830-BB31-ABA562D60534}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7296,6 +7137,245 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8447F3E7-1537-4679-AB27-5D8C1807B167}">
+  <dimension ref="A1:AJ2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>320</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>476</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>322</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>477</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>478</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="L1" s="51" t="s">
+        <v>479</v>
+      </c>
+      <c r="M1" s="51" t="s">
+        <v>480</v>
+      </c>
+      <c r="N1" s="51" t="s">
+        <v>481</v>
+      </c>
+      <c r="O1" s="51" t="s">
+        <v>482</v>
+      </c>
+      <c r="P1" s="51" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q1" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="R1" s="51" t="s">
+        <v>202</v>
+      </c>
+      <c r="S1" s="51" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1" s="51" t="s">
+        <v>204</v>
+      </c>
+      <c r="U1" s="51" t="s">
+        <v>484</v>
+      </c>
+      <c r="V1" s="51" t="s">
+        <v>422</v>
+      </c>
+      <c r="W1" s="51" t="s">
+        <v>423</v>
+      </c>
+      <c r="X1" s="51" t="s">
+        <v>485</v>
+      </c>
+      <c r="Y1" s="51" t="s">
+        <v>486</v>
+      </c>
+      <c r="Z1" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="AA1" s="51" t="s">
+        <v>487</v>
+      </c>
+      <c r="AB1" s="51" t="s">
+        <v>488</v>
+      </c>
+      <c r="AC1" s="51" t="s">
+        <v>489</v>
+      </c>
+      <c r="AD1" s="51" t="s">
+        <v>490</v>
+      </c>
+      <c r="AE1" s="51" t="s">
+        <v>491</v>
+      </c>
+      <c r="AF1" s="51" t="s">
+        <v>492</v>
+      </c>
+      <c r="AG1" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="AH1" s="51" t="s">
+        <v>493</v>
+      </c>
+      <c r="AI1" s="51" t="s">
+        <v>494</v>
+      </c>
+      <c r="AJ1" s="51" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>329</v>
+      </c>
+      <c r="G2" s="49">
+        <v>123456789012</v>
+      </c>
+      <c r="H2" s="49">
+        <v>102000000084</v>
+      </c>
+      <c r="I2" s="49">
+        <v>103000012486</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2" s="59">
+        <v>45575</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2" s="59">
+        <v>45575</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>498</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>12</v>
+      </c>
+      <c r="T2">
+        <v>22</v>
+      </c>
+      <c r="U2">
+        <v>12000</v>
+      </c>
+      <c r="V2" t="s">
+        <v>472</v>
+      </c>
+      <c r="W2" s="42" t="s">
+        <v>473</v>
+      </c>
+      <c r="X2">
+        <v>2024</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>499</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>500</v>
+      </c>
+      <c r="AA2" s="59">
+        <v>45575</v>
+      </c>
+      <c r="AB2">
+        <v>2200000</v>
+      </c>
+      <c r="AC2">
+        <v>2300000</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>501</v>
+      </c>
+      <c r="AE2" s="59">
+        <v>35713</v>
+      </c>
+      <c r="AF2">
+        <v>690</v>
+      </c>
+      <c r="AG2">
+        <v>11100</v>
+      </c>
+      <c r="AH2">
+        <v>50</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>328</v>
+      </c>
+      <c r="AJ2">
+        <v>11046</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{48E96FF8-C647-4A3B-9CDF-D5A4C1C8BC57}"/>
+    <hyperlink ref="W2" r:id="rId2" xr:uid="{64BC90D3-0F6A-4830-BB31-ABA562D60534}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECE5D8D-FA94-4188-823E-662EDE50B36B}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
@@ -7534,7 +7614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36858E2-F0EA-4635-9BC2-1183A127E49E}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -7736,7 +7816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB3638D-C83E-4A6F-819F-771D3A2A4656}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -7938,7 +8018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D52E09F-8B96-4265-9506-82F252F44BBE}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
@@ -8161,7 +8241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9159E0D-9089-4878-B664-707C0105256B}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
@@ -8282,7 +8362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC2912E-97A5-4172-92A7-D95EC75D7467}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -8367,7 +8447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BBCF75-0907-4665-B05B-5F646DCC77B0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -8440,7 +8520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FBF668-E128-4040-B6ED-93F1F8C58976}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -8525,7 +8605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA3F161-58BC-448B-B5E3-6D635EBE27B5}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -8603,85 +8683,6 @@
       </c>
       <c r="K2" s="5">
         <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC3ED26-FC7E-4813-9284-FC44192916A8}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>581</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>588</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>585</v>
-      </c>
-      <c r="F2">
-        <v>500000</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="H2">
-        <v>500000</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8702,6 +8703,85 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC3ED26-FC7E-4813-9284-FC44192916A8}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>588</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="F2">
+        <v>500000</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="H2">
+        <v>500000</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD220DAE-DC66-47B2-9E7D-7C8BFE585BF7}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -8810,7 +8890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6699088-8B78-41CE-92A9-486BBF01C239}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -8931,7 +9011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A5C99B-D48F-4A68-B0E1-540E17409C14}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -8998,7 +9078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B08CE7-F106-4EA6-A0D8-9AB88F831D8E}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -9083,7 +9163,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105D85E1-2AC3-4124-9833-125B772A9F19}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -9174,7 +9254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA71F65B-A788-4DCC-B907-03EB11DB4AAD}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -9271,7 +9351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8414E631-EEE6-4701-9BE8-E616D7A5F2F3}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -9386,7 +9466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D296740-0570-4ECD-A3B8-91504FAD9B16}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -9473,73 +9553,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C8D0AF-EA18-422A-B740-5AA64B6DDA49}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
-        <v>629</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="G2" s="3">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2E8482-DDC0-4CC9-984C-7A8877C98CC3}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9608,6 +9627,67 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2E8482-DDC0-4CC9-984C-7A8877C98CC3}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6239EED-1B9B-4584-B1A3-A9B07AF11AD0}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -9664,7 +9744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD432F5-62C4-45EF-AC68-5C1252194A64}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -9725,7 +9805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6169293-DEC5-42AE-A79F-E12C5B9D7CC2}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -9870,7 +9950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CE793E-C149-4585-8B74-259348F84D86}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -9925,7 +10005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D808A0-23B7-4F4F-A13E-318766F76185}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -9986,7 +10066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3E3B17-56ED-4E7C-954A-B0243A3C61FD}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -10044,7 +10124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB8E3D9-FD65-43CE-ACEE-9C9681E76DFB}">
   <dimension ref="A1:G2"/>
   <sheetViews>

</xml_diff>